<commit_message>
RJH2-Issue381 - Update of Issue #381 Implementation - Based on new combined CBECC Main code - Ignore Existing elements - Add IfValidAnd() checks
</commit_message>
<xml_diff>
--- a/Documentation/T24Res/T24RCustomStdDesign.xlsx
+++ b/Documentation/T24Res/T24RCustomStdDesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\git-vscode\CBECC-Dev\Documentation\T24Res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\SVN\branches\CBECC-Com_MFamRestructure\Documentation\T24Res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDE9C57-C7E1-4939-B768-B6C30AC952B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71481180-D713-48D8-97D8-A5E088BA1223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="2580" windowWidth="26790" windowHeight="14340" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
+    <workbookView xWindow="24549" yWindow="2571" windowWidth="22868" windowHeight="14615" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="67">
   <si>
     <t>;</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>default  -or-  Electricity  -or-  Gas</t>
-  </si>
-  <si>
-    <t>09/18/25 - SAC - modified '2025 Final' LowRiseRes records for DHW, CompactDHW &amp; DrnWtrHtRec data</t>
   </si>
 </sst>
 </file>
@@ -289,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,12 +296,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -438,19 +429,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -767,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C373ABC9-0F2E-48ED-B208-F0F9FC7924F4}">
-  <dimension ref="A1:V94"/>
+  <dimension ref="A1:V92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,8 +767,7 @@
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="9" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.5703125" customWidth="1"/>
@@ -829,7 +814,7 @@
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -837,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -845,7 +830,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -853,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -861,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -869,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -877,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,28 +886,31 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" t="s">
-        <v>15</v>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -930,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -941,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -952,10 +940,10 @@
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -963,10 +951,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -974,37 +962,37 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>19</v>
+      <c r="E22" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>27</v>
+      <c r="E23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E24" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1012,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1023,10 +1011,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,10 +1022,10 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1045,10 +1033,10 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" t="s">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1056,10 +1044,10 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1067,128 +1055,177 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="5" t="s">
+    <row r="34" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F34" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H34" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J34" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K34" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L35" s="8" t="s">
+      <c r="L34" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="M34" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N35" s="8" t="s">
+      <c r="N34" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O35" s="8" t="s">
+      <c r="O34" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P35" s="8" t="s">
+      <c r="P34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Q35" s="8" t="s">
+      <c r="Q34" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="R35" s="8" t="s">
+      <c r="R34" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="S35" s="8" t="s">
+      <c r="S34" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="T35" s="5"/>
-      <c r="U35" s="5"/>
-      <c r="V35" s="5"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>57</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D35" t="s">
         <v>36</v>
       </c>
+      <c r="E35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="15">
+        <v>1</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L35" s="26">
+        <v>0.7</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0</v>
+      </c>
+      <c r="N35" s="9">
+        <v>0</v>
+      </c>
+      <c r="O35" s="9">
+        <v>0</v>
+      </c>
+      <c r="P35" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="T35" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C36" s="20" t="str">
+        <f>C35</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="E36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F36" s="15">
+        <v>16</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="M36" s="7">
         <v>1</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L36" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M36" s="9">
-        <v>0</v>
-      </c>
       <c r="N36" s="9">
         <v>0</v>
       </c>
@@ -1207,14 +1244,10 @@
       <c r="S36" s="9">
         <v>-1</v>
       </c>
-      <c r="T36" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T36" s="10"/>
+      <c r="U36" s="1"/>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C37" s="20" t="str">
         <f>C36</f>
         <v>2025 Final</v>
@@ -1225,8 +1258,8 @@
       <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="15">
-        <v>16</v>
+      <c r="F37" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>30</v>
@@ -1243,11 +1276,11 @@
       <c r="K37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L37" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="M37" s="7">
-        <v>1</v>
+      <c r="L37" s="9">
+        <v>0</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0</v>
       </c>
       <c r="N37" s="9">
         <v>0</v>
@@ -1270,359 +1303,364 @@
       <c r="T37" s="10"/>
       <c r="U37" s="1"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C38" s="20" t="str">
-        <f>C37</f>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C38" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="24">
+        <v>16</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L38" s="27">
+        <v>0</v>
+      </c>
+      <c r="M38" s="27">
+        <v>0</v>
+      </c>
+      <c r="N38" s="27">
+        <v>0</v>
+      </c>
+      <c r="O38" s="27">
+        <v>0</v>
+      </c>
+      <c r="P38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T38" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U38" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="V38" s="22"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C39" s="20" t="str">
+        <f>C38</f>
         <v>2025 Final</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D39" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L39" s="9">
+        <v>0</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0</v>
+      </c>
+      <c r="N39" s="9">
+        <v>0</v>
+      </c>
+      <c r="O39" s="9">
+        <v>0</v>
+      </c>
+      <c r="P39" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S39" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C40" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="24">
+        <v>1</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" s="27">
+        <v>0</v>
+      </c>
+      <c r="M40" s="27">
+        <v>0</v>
+      </c>
+      <c r="N40" s="27">
+        <v>0</v>
+      </c>
+      <c r="O40" s="27">
+        <v>0</v>
+      </c>
+      <c r="P40" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T40" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U40" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="V40" s="22"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C41" s="20" t="str">
+        <f t="shared" ref="C41" si="0">C40</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="15">
+        <v>16</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="L41" s="29">
+        <v>0</v>
+      </c>
+      <c r="M41" s="29">
+        <v>0</v>
+      </c>
+      <c r="N41" s="29">
+        <v>0</v>
+      </c>
+      <c r="O41" s="29">
+        <v>0</v>
+      </c>
+      <c r="P41" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="R41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="S41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C42" s="20" t="str">
+        <f t="shared" ref="C42" si="1">C41</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L42" s="9">
+        <v>0</v>
+      </c>
+      <c r="M42" s="9">
+        <v>0</v>
+      </c>
+      <c r="N42" s="9">
+        <v>0</v>
+      </c>
+      <c r="O42" s="9">
+        <v>0</v>
+      </c>
+      <c r="P42" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S42" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C43" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L38" s="9">
-        <v>0</v>
-      </c>
-      <c r="M38" s="9">
-        <v>0</v>
-      </c>
-      <c r="N38" s="9">
-        <v>0</v>
-      </c>
-      <c r="O38" s="9">
-        <v>0</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="T38" s="10"/>
-      <c r="U38" s="1"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C39" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="24">
+      <c r="E43" s="23">
+        <v>0</v>
+      </c>
+      <c r="F43" s="24">
         <v>1</v>
       </c>
-      <c r="G39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I39" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="L39" s="32">
+      <c r="G43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L43" s="26">
         <v>0.7</v>
       </c>
-      <c r="M39" s="27">
-        <v>0</v>
-      </c>
-      <c r="N39" s="27">
-        <v>0</v>
-      </c>
-      <c r="O39" s="27">
-        <v>0</v>
-      </c>
-      <c r="P39" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T39" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U39" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="V39" s="22"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C40" s="20" t="str">
-        <f>C39</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D40" s="20" t="str">
-        <f>D39</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="15">
-        <v>16</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="K40" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L40" s="33">
-        <v>0.7</v>
-      </c>
-      <c r="M40" s="33">
-        <v>1</v>
-      </c>
-      <c r="N40" s="9">
-        <v>0</v>
-      </c>
-      <c r="O40" s="9">
-        <v>0</v>
-      </c>
-      <c r="P40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S40" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C41" s="20" t="str">
-        <f>C40</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D41" s="20" t="str">
-        <f>D40</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K41" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L41" s="9">
-        <v>0</v>
-      </c>
-      <c r="M41" s="9">
-        <v>0</v>
-      </c>
-      <c r="N41" s="9">
-        <v>0</v>
-      </c>
-      <c r="O41" s="9">
-        <v>0</v>
-      </c>
-      <c r="P41" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S41" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C42" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="24">
-        <v>1</v>
-      </c>
-      <c r="G42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I42" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J42" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="L42" s="27">
-        <v>0</v>
-      </c>
-      <c r="M42" s="27">
-        <v>0</v>
-      </c>
-      <c r="N42" s="27">
-        <v>0</v>
-      </c>
-      <c r="O42" s="27">
-        <v>0</v>
-      </c>
-      <c r="P42" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T42" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U42" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="V42" s="22"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C43" s="20" t="str">
-        <f t="shared" ref="C43" si="0">C42</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="15">
-        <v>16</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L43" s="9">
-        <v>0</v>
-      </c>
-      <c r="M43" s="9">
-        <v>0</v>
-      </c>
-      <c r="N43" s="9">
-        <v>0</v>
-      </c>
-      <c r="O43" s="9">
-        <v>0</v>
-      </c>
-      <c r="P43" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S43" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C44" s="20" t="str">
-        <f t="shared" ref="C44" si="1">C43</f>
-        <v>2025 Final</v>
+      <c r="M43" s="27">
+        <v>0</v>
+      </c>
+      <c r="N43" s="27">
+        <v>0</v>
+      </c>
+      <c r="O43" s="27">
+        <v>0</v>
+      </c>
+      <c r="P43" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T43" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U43" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="V43" s="22"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C44" s="20" t="s">
+        <v>56</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="E44" s="9">
+        <v>0</v>
+      </c>
+      <c r="F44" s="15">
+        <f>F43+1</f>
+        <v>2</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>30</v>
@@ -1631,13 +1669,13 @@
         <v>30</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="L44" s="9">
         <v>0</v>
@@ -1664,67 +1702,61 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C45" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="22" t="s">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C45" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="23">
-        <v>0</v>
-      </c>
-      <c r="F45" s="24">
-        <v>1</v>
-      </c>
-      <c r="G45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="J45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="K45" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="L45" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M45" s="27">
-        <v>0</v>
-      </c>
-      <c r="N45" s="27">
-        <v>0</v>
-      </c>
-      <c r="O45" s="27">
-        <v>0</v>
-      </c>
-      <c r="P45" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T45" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U45" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="V45" s="22"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E45" s="9">
+        <v>0</v>
+      </c>
+      <c r="F45" s="15">
+        <f t="shared" ref="F45:F58" si="2">F44+1</f>
+        <v>3</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L45" s="9">
+        <v>0</v>
+      </c>
+      <c r="M45" s="9">
+        <v>0</v>
+      </c>
+      <c r="N45" s="9">
+        <v>0</v>
+      </c>
+      <c r="O45" s="9">
+        <v>0</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S45" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C46" s="20" t="s">
         <v>56</v>
       </c>
@@ -1735,8 +1767,8 @@
         <v>0</v>
       </c>
       <c r="F46" s="15">
-        <f>F45+1</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>30</v>
@@ -1745,13 +1777,13 @@
         <v>30</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L46" s="9">
         <v>0</v>
@@ -1778,7 +1810,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C47" s="20" t="s">
         <v>56</v>
       </c>
@@ -1789,8 +1821,8 @@
         <v>0</v>
       </c>
       <c r="F47" s="15">
-        <f t="shared" ref="F47:F60" si="2">F46+1</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>30</v>
@@ -1799,13 +1831,13 @@
         <v>30</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L47" s="9">
         <v>0</v>
@@ -1832,7 +1864,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C48" s="20" t="s">
         <v>56</v>
       </c>
@@ -1844,7 +1876,7 @@
       </c>
       <c r="F48" s="15">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>30</v>
@@ -1853,13 +1885,13 @@
         <v>30</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L48" s="9">
         <v>0</v>
@@ -1898,7 +1930,7 @@
       </c>
       <c r="F49" s="15">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>30</v>
@@ -1952,7 +1984,7 @@
       </c>
       <c r="F50" s="15">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G50" s="10" t="s">
         <v>30</v>
@@ -2006,7 +2038,7 @@
       </c>
       <c r="F51" s="15">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G51" s="10" t="s">
         <v>30</v>
@@ -2060,7 +2092,7 @@
       </c>
       <c r="F52" s="15">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G52" s="10" t="s">
         <v>30</v>
@@ -2114,7 +2146,7 @@
       </c>
       <c r="F53" s="15">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G53" s="10" t="s">
         <v>30</v>
@@ -2168,7 +2200,7 @@
       </c>
       <c r="F54" s="15">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>30</v>
@@ -2222,7 +2254,7 @@
       </c>
       <c r="F55" s="15">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G55" s="10" t="s">
         <v>30</v>
@@ -2231,13 +2263,13 @@
         <v>30</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L55" s="9">
         <v>0</v>
@@ -2276,7 +2308,7 @@
       </c>
       <c r="F56" s="15">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>30</v>
@@ -2285,13 +2317,13 @@
         <v>30</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L56" s="9">
         <v>0</v>
@@ -2330,7 +2362,7 @@
       </c>
       <c r="F57" s="15">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>30</v>
@@ -2339,13 +2371,13 @@
         <v>30</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L57" s="9">
         <v>0</v>
@@ -2373,72 +2405,74 @@
       </c>
     </row>
     <row r="58" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C58" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D58" s="20" t="s">
+      <c r="C58" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="9">
-        <v>0</v>
-      </c>
-      <c r="F58" s="15">
+      <c r="E58" s="12">
+        <v>0</v>
+      </c>
+      <c r="F58" s="16">
         <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L58" s="9">
-        <v>0</v>
-      </c>
-      <c r="M58" s="9">
-        <v>0</v>
-      </c>
-      <c r="N58" s="9">
-        <v>0</v>
-      </c>
-      <c r="O58" s="9">
-        <v>0</v>
-      </c>
-      <c r="P58" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S58" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L58" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M58" s="8">
+        <v>1</v>
+      </c>
+      <c r="N58" s="12">
+        <v>0</v>
+      </c>
+      <c r="O58" s="12">
+        <v>0</v>
+      </c>
+      <c r="P58" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
     </row>
     <row r="59" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C59" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D59" s="20" t="s">
+      <c r="C59" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" t="s">
         <v>36</v>
       </c>
-      <c r="E59" s="9">
-        <v>0</v>
+      <c r="E59" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F59" s="15">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G59" s="10" t="s">
         <v>30</v>
@@ -2455,8 +2489,8 @@
       <c r="K59" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L59" s="9">
-        <v>0</v>
+      <c r="L59" s="7">
+        <v>0.7</v>
       </c>
       <c r="M59" s="9">
         <v>0</v>
@@ -2479,76 +2513,80 @@
       <c r="S59" s="9">
         <v>-1</v>
       </c>
+      <c r="T59" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U59" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="60" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C60" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D60" s="21" t="s">
+      <c r="C60" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="12">
-        <v>0</v>
-      </c>
-      <c r="F60" s="16">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L60" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M60" s="8">
-        <v>1</v>
-      </c>
-      <c r="N60" s="12">
-        <v>0</v>
-      </c>
-      <c r="O60" s="12">
-        <v>0</v>
-      </c>
-      <c r="P60" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
+      <c r="E60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="15">
+        <f>F59+1</f>
+        <v>2</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L60" s="9">
+        <v>0</v>
+      </c>
+      <c r="M60" s="9">
+        <v>0</v>
+      </c>
+      <c r="N60" s="9">
+        <v>0</v>
+      </c>
+      <c r="O60" s="9">
+        <v>0</v>
+      </c>
+      <c r="P60" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S60" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="61" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>56</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="C61" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F61" s="15">
-        <v>1</v>
+        <f t="shared" ref="F61:F74" si="3">F60+1</f>
+        <v>3</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>30</v>
@@ -2565,8 +2603,8 @@
       <c r="K61" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L61" s="7">
-        <v>0.7</v>
+      <c r="L61" s="9">
+        <v>0</v>
       </c>
       <c r="M61" s="9">
         <v>0</v>
@@ -2588,12 +2626,6 @@
       </c>
       <c r="S61" s="9">
         <v>-1</v>
-      </c>
-      <c r="T61" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U61" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="62" spans="3:22" x14ac:dyDescent="0.25">
@@ -2607,8 +2639,8 @@
         <v>9</v>
       </c>
       <c r="F62" s="15">
-        <f>F61+1</f>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>30</v>
@@ -2661,8 +2693,8 @@
         <v>9</v>
       </c>
       <c r="F63" s="15">
-        <f t="shared" ref="F63:F76" si="3">F62+1</f>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>30</v>
@@ -2716,7 +2748,7 @@
       </c>
       <c r="F64" s="15">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G64" s="10" t="s">
         <v>30</v>
@@ -2770,7 +2802,7 @@
       </c>
       <c r="F65" s="15">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>30</v>
@@ -2824,7 +2856,7 @@
       </c>
       <c r="F66" s="15">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G66" s="10" t="s">
         <v>30</v>
@@ -2878,7 +2910,7 @@
       </c>
       <c r="F67" s="15">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G67" s="10" t="s">
         <v>30</v>
@@ -2932,7 +2964,7 @@
       </c>
       <c r="F68" s="15">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G68" s="10" t="s">
         <v>30</v>
@@ -2986,7 +3018,7 @@
       </c>
       <c r="F69" s="15">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G69" s="10" t="s">
         <v>30</v>
@@ -3040,7 +3072,7 @@
       </c>
       <c r="F70" s="15">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G70" s="10" t="s">
         <v>30</v>
@@ -3094,7 +3126,7 @@
       </c>
       <c r="F71" s="15">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G71" s="10" t="s">
         <v>30</v>
@@ -3148,7 +3180,7 @@
       </c>
       <c r="F72" s="15">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G72" s="10" t="s">
         <v>30</v>
@@ -3202,7 +3234,7 @@
       </c>
       <c r="F73" s="15">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G73" s="10" t="s">
         <v>30</v>
@@ -3245,72 +3277,74 @@
       </c>
     </row>
     <row r="74" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C74" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D74" s="20" t="s">
+      <c r="C74" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E74" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="15">
+      <c r="E74" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="16">
         <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="G74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L74" s="9">
-        <v>0</v>
-      </c>
-      <c r="M74" s="9">
-        <v>0</v>
-      </c>
-      <c r="N74" s="9">
-        <v>0</v>
-      </c>
-      <c r="O74" s="9">
-        <v>0</v>
-      </c>
-      <c r="P74" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S74" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L74" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M74" s="8">
+        <v>1</v>
+      </c>
+      <c r="N74" s="12">
+        <v>0</v>
+      </c>
+      <c r="O74" s="12">
+        <v>0</v>
+      </c>
+      <c r="P74" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+      <c r="V74" s="3"/>
     </row>
     <row r="75" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C75" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E75" s="9" t="s">
+      <c r="C75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="15">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G75" s="10" t="s">
         <v>30</v>
@@ -3319,13 +3353,13 @@
         <v>30</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="K75" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="L75" s="9">
         <v>0</v>
@@ -3351,76 +3385,80 @@
       <c r="S75" s="9">
         <v>-1</v>
       </c>
+      <c r="T75" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U75" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="76" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C76" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D76" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="16">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K76" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L76" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M76" s="8">
-        <v>1</v>
-      </c>
-      <c r="N76" s="12">
-        <v>0</v>
-      </c>
-      <c r="O76" s="12">
-        <v>0</v>
-      </c>
-      <c r="P76" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T76" s="3"/>
-      <c r="U76" s="3"/>
-      <c r="V76" s="3"/>
+      <c r="C76" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="15">
+        <f>F75+1</f>
+        <v>2</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L76" s="9">
+        <v>0</v>
+      </c>
+      <c r="M76" s="9">
+        <v>0</v>
+      </c>
+      <c r="N76" s="9">
+        <v>0</v>
+      </c>
+      <c r="O76" s="9">
+        <v>0</v>
+      </c>
+      <c r="P76" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S76" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="77" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>56</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="2" t="s">
+      <c r="C77" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="15">
-        <v>1</v>
+        <f t="shared" ref="F77:F90" si="4">F76+1</f>
+        <v>3</v>
       </c>
       <c r="G77" s="10" t="s">
         <v>30</v>
@@ -3460,12 +3498,6 @@
       </c>
       <c r="S77" s="9">
         <v>-1</v>
-      </c>
-      <c r="T77" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U77" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="78" spans="3:22" x14ac:dyDescent="0.25">
@@ -3479,8 +3511,8 @@
         <v>9</v>
       </c>
       <c r="F78" s="15">
-        <f>F77+1</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="G78" s="10" t="s">
         <v>30</v>
@@ -3509,11 +3541,11 @@
       <c r="O78" s="9">
         <v>0</v>
       </c>
-      <c r="P78" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q78" s="9">
-        <v>-1</v>
+      <c r="P78" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q78" s="19">
+        <v>0.4</v>
       </c>
       <c r="R78" s="9">
         <v>-1</v>
@@ -3533,8 +3565,8 @@
         <v>9</v>
       </c>
       <c r="F79" s="15">
-        <f t="shared" ref="F79:F92" si="4">F78+1</f>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="G79" s="10" t="s">
         <v>30</v>
@@ -3563,11 +3595,11 @@
       <c r="O79" s="9">
         <v>0</v>
       </c>
-      <c r="P79" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q79" s="9">
-        <v>-1</v>
+      <c r="P79" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q79" s="19">
+        <v>0.4</v>
       </c>
       <c r="R79" s="9">
         <v>-1</v>
@@ -3588,7 +3620,7 @@
       </c>
       <c r="F80" s="15">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G80" s="10" t="s">
         <v>30</v>
@@ -3642,7 +3674,7 @@
       </c>
       <c r="F81" s="15">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G81" s="10" t="s">
         <v>30</v>
@@ -3696,7 +3728,7 @@
       </c>
       <c r="F82" s="15">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G82" s="10" t="s">
         <v>30</v>
@@ -3750,7 +3782,7 @@
       </c>
       <c r="F83" s="15">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G83" s="10" t="s">
         <v>30</v>
@@ -3804,7 +3836,7 @@
       </c>
       <c r="F84" s="15">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G84" s="10" t="s">
         <v>30</v>
@@ -3858,7 +3890,7 @@
       </c>
       <c r="F85" s="15">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G85" s="10" t="s">
         <v>30</v>
@@ -3887,11 +3919,11 @@
       <c r="O85" s="9">
         <v>0</v>
       </c>
-      <c r="P85" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q85" s="19">
-        <v>0.4</v>
+      <c r="P85" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q85" s="9">
+        <v>-1</v>
       </c>
       <c r="R85" s="9">
         <v>-1</v>
@@ -3912,7 +3944,7 @@
       </c>
       <c r="F86" s="15">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G86" s="10" t="s">
         <v>30</v>
@@ -3941,11 +3973,11 @@
       <c r="O86" s="9">
         <v>0</v>
       </c>
-      <c r="P86" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q86" s="19">
-        <v>0.4</v>
+      <c r="P86" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q86" s="9">
+        <v>-1</v>
       </c>
       <c r="R86" s="9">
         <v>-1</v>
@@ -3966,7 +3998,7 @@
       </c>
       <c r="F87" s="15">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G87" s="10" t="s">
         <v>30</v>
@@ -4020,7 +4052,7 @@
       </c>
       <c r="F88" s="15">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G88" s="10" t="s">
         <v>30</v>
@@ -4049,17 +4081,17 @@
       <c r="O88" s="9">
         <v>0</v>
       </c>
-      <c r="P88" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S88" s="9">
-        <v>-1</v>
+      <c r="P88" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q88" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R88" s="19">
+        <v>67</v>
+      </c>
+      <c r="S88" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="2:22" x14ac:dyDescent="0.25">
@@ -4074,7 +4106,7 @@
       </c>
       <c r="F89" s="15">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G89" s="10" t="s">
         <v>30</v>
@@ -4103,245 +4135,137 @@
       <c r="O89" s="9">
         <v>0</v>
       </c>
-      <c r="P89" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S89" s="9">
-        <v>-1</v>
+      <c r="P89" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q89" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R89" s="19">
+        <v>67</v>
+      </c>
+      <c r="S89" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="21" t="s">
         <v>56</v>
       </c>
       <c r="D90" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E90" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F90" s="15">
+      <c r="E90" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="16">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="G90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L90" s="9">
-        <v>0</v>
-      </c>
-      <c r="M90" s="9">
-        <v>0</v>
-      </c>
-      <c r="N90" s="9">
-        <v>0</v>
-      </c>
-      <c r="O90" s="9">
-        <v>0</v>
-      </c>
-      <c r="P90" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q90" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R90" s="19">
-        <v>67</v>
-      </c>
-      <c r="S90" s="19">
-        <v>72</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L90" s="12">
+        <v>0</v>
+      </c>
+      <c r="M90" s="12">
+        <v>0</v>
+      </c>
+      <c r="N90" s="12">
+        <v>0</v>
+      </c>
+      <c r="O90" s="12">
+        <v>0</v>
+      </c>
+      <c r="P90" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
     </row>
     <row r="91" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C91" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D91" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F91" s="15">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="G91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L91" s="9">
-        <v>0</v>
-      </c>
-      <c r="M91" s="9">
-        <v>0</v>
-      </c>
-      <c r="N91" s="9">
-        <v>0</v>
-      </c>
-      <c r="O91" s="9">
-        <v>0</v>
-      </c>
-      <c r="P91" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q91" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R91" s="19">
-        <v>67</v>
-      </c>
-      <c r="S91" s="19">
-        <v>72</v>
+      <c r="C91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L91" s="13">
+        <v>0</v>
+      </c>
+      <c r="M91" s="13">
+        <v>0</v>
+      </c>
+      <c r="N91" s="13">
+        <v>0</v>
+      </c>
+      <c r="O91" s="13">
+        <v>0</v>
+      </c>
+      <c r="P91" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="R91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="S91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="T91" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U91" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C92" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D92" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F92" s="16">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="G92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L92" s="12">
-        <v>0</v>
-      </c>
-      <c r="M92" s="12">
-        <v>0</v>
-      </c>
-      <c r="N92" s="12">
-        <v>0</v>
-      </c>
-      <c r="O92" s="12">
-        <v>0</v>
-      </c>
-      <c r="P92" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T92" s="3"/>
-      <c r="U92" s="3"/>
-      <c r="V92" s="3"/>
-    </row>
-    <row r="93" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F93" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="L93" s="13">
-        <v>0</v>
-      </c>
-      <c r="M93" s="13">
-        <v>0</v>
-      </c>
-      <c r="N93" s="13">
-        <v>0</v>
-      </c>
-      <c r="O93" s="13">
-        <v>0</v>
-      </c>
-      <c r="P93" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="R93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="S93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="T93" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U93" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="94" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+      <c r="B92" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CUAC rate updates 2025.09
</commit_message>
<xml_diff>
--- a/Documentation/T24Res/T24RCustomStdDesign.xlsx
+++ b/Documentation/T24Res/T24RCustomStdDesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\git-vscode\CBECC-Dev\Documentation\T24Res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\SVN\branches\CBECC-Com_MFamRestructure\Documentation\T24Res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDE9C57-C7E1-4939-B768-B6C30AC952B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71481180-D713-48D8-97D8-A5E088BA1223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="2580" windowWidth="26790" windowHeight="14340" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
+    <workbookView xWindow="24549" yWindow="2571" windowWidth="22868" windowHeight="14615" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="67">
   <si>
     <t>;</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>default  -or-  Electricity  -or-  Gas</t>
-  </si>
-  <si>
-    <t>09/18/25 - SAC - modified '2025 Final' LowRiseRes records for DHW, CompactDHW &amp; DrnWtrHtRec data</t>
   </si>
 </sst>
 </file>
@@ -289,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,12 +296,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -438,19 +429,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -767,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C373ABC9-0F2E-48ED-B208-F0F9FC7924F4}">
-  <dimension ref="A1:V94"/>
+  <dimension ref="A1:V92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,8 +767,7 @@
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="9" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.5703125" customWidth="1"/>
@@ -829,7 +814,7 @@
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -837,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -845,7 +830,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -853,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -861,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -869,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -877,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,28 +886,31 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" t="s">
-        <v>15</v>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -930,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -941,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -952,10 +940,10 @@
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -963,10 +951,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -974,37 +962,37 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>19</v>
+      <c r="E22" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>27</v>
+      <c r="E23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E24" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1012,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1023,10 +1011,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,10 +1022,10 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1045,10 +1033,10 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" t="s">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1056,10 +1044,10 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1067,128 +1055,177 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="5" t="s">
+    <row r="34" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F34" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H34" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J34" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K34" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L35" s="8" t="s">
+      <c r="L34" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="M34" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N35" s="8" t="s">
+      <c r="N34" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O35" s="8" t="s">
+      <c r="O34" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P35" s="8" t="s">
+      <c r="P34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Q35" s="8" t="s">
+      <c r="Q34" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="R35" s="8" t="s">
+      <c r="R34" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="S35" s="8" t="s">
+      <c r="S34" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="T35" s="5"/>
-      <c r="U35" s="5"/>
-      <c r="V35" s="5"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>57</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D35" t="s">
         <v>36</v>
       </c>
+      <c r="E35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="15">
+        <v>1</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L35" s="26">
+        <v>0.7</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0</v>
+      </c>
+      <c r="N35" s="9">
+        <v>0</v>
+      </c>
+      <c r="O35" s="9">
+        <v>0</v>
+      </c>
+      <c r="P35" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="T35" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C36" s="20" t="str">
+        <f>C35</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="E36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F36" s="15">
+        <v>16</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="M36" s="7">
         <v>1</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L36" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M36" s="9">
-        <v>0</v>
-      </c>
       <c r="N36" s="9">
         <v>0</v>
       </c>
@@ -1207,14 +1244,10 @@
       <c r="S36" s="9">
         <v>-1</v>
       </c>
-      <c r="T36" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T36" s="10"/>
+      <c r="U36" s="1"/>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C37" s="20" t="str">
         <f>C36</f>
         <v>2025 Final</v>
@@ -1225,8 +1258,8 @@
       <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="15">
-        <v>16</v>
+      <c r="F37" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>30</v>
@@ -1243,11 +1276,11 @@
       <c r="K37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L37" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="M37" s="7">
-        <v>1</v>
+      <c r="L37" s="9">
+        <v>0</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0</v>
       </c>
       <c r="N37" s="9">
         <v>0</v>
@@ -1270,359 +1303,364 @@
       <c r="T37" s="10"/>
       <c r="U37" s="1"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C38" s="20" t="str">
-        <f>C37</f>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C38" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="24">
+        <v>16</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L38" s="27">
+        <v>0</v>
+      </c>
+      <c r="M38" s="27">
+        <v>0</v>
+      </c>
+      <c r="N38" s="27">
+        <v>0</v>
+      </c>
+      <c r="O38" s="27">
+        <v>0</v>
+      </c>
+      <c r="P38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T38" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U38" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="V38" s="22"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C39" s="20" t="str">
+        <f>C38</f>
         <v>2025 Final</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D39" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L39" s="9">
+        <v>0</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0</v>
+      </c>
+      <c r="N39" s="9">
+        <v>0</v>
+      </c>
+      <c r="O39" s="9">
+        <v>0</v>
+      </c>
+      <c r="P39" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S39" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C40" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="24">
+        <v>1</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" s="27">
+        <v>0</v>
+      </c>
+      <c r="M40" s="27">
+        <v>0</v>
+      </c>
+      <c r="N40" s="27">
+        <v>0</v>
+      </c>
+      <c r="O40" s="27">
+        <v>0</v>
+      </c>
+      <c r="P40" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T40" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U40" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="V40" s="22"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C41" s="20" t="str">
+        <f t="shared" ref="C41" si="0">C40</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="15">
+        <v>16</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="L41" s="29">
+        <v>0</v>
+      </c>
+      <c r="M41" s="29">
+        <v>0</v>
+      </c>
+      <c r="N41" s="29">
+        <v>0</v>
+      </c>
+      <c r="O41" s="29">
+        <v>0</v>
+      </c>
+      <c r="P41" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="R41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="S41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C42" s="20" t="str">
+        <f t="shared" ref="C42" si="1">C41</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L42" s="9">
+        <v>0</v>
+      </c>
+      <c r="M42" s="9">
+        <v>0</v>
+      </c>
+      <c r="N42" s="9">
+        <v>0</v>
+      </c>
+      <c r="O42" s="9">
+        <v>0</v>
+      </c>
+      <c r="P42" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S42" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C43" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L38" s="9">
-        <v>0</v>
-      </c>
-      <c r="M38" s="9">
-        <v>0</v>
-      </c>
-      <c r="N38" s="9">
-        <v>0</v>
-      </c>
-      <c r="O38" s="9">
-        <v>0</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="T38" s="10"/>
-      <c r="U38" s="1"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C39" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="24">
+      <c r="E43" s="23">
+        <v>0</v>
+      </c>
+      <c r="F43" s="24">
         <v>1</v>
       </c>
-      <c r="G39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I39" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="L39" s="32">
+      <c r="G43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L43" s="26">
         <v>0.7</v>
       </c>
-      <c r="M39" s="27">
-        <v>0</v>
-      </c>
-      <c r="N39" s="27">
-        <v>0</v>
-      </c>
-      <c r="O39" s="27">
-        <v>0</v>
-      </c>
-      <c r="P39" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T39" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U39" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="V39" s="22"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C40" s="20" t="str">
-        <f>C39</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D40" s="20" t="str">
-        <f>D39</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="15">
-        <v>16</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="K40" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L40" s="33">
-        <v>0.7</v>
-      </c>
-      <c r="M40" s="33">
-        <v>1</v>
-      </c>
-      <c r="N40" s="9">
-        <v>0</v>
-      </c>
-      <c r="O40" s="9">
-        <v>0</v>
-      </c>
-      <c r="P40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S40" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C41" s="20" t="str">
-        <f>C40</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D41" s="20" t="str">
-        <f>D40</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K41" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L41" s="9">
-        <v>0</v>
-      </c>
-      <c r="M41" s="9">
-        <v>0</v>
-      </c>
-      <c r="N41" s="9">
-        <v>0</v>
-      </c>
-      <c r="O41" s="9">
-        <v>0</v>
-      </c>
-      <c r="P41" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S41" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C42" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="24">
-        <v>1</v>
-      </c>
-      <c r="G42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I42" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J42" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="L42" s="27">
-        <v>0</v>
-      </c>
-      <c r="M42" s="27">
-        <v>0</v>
-      </c>
-      <c r="N42" s="27">
-        <v>0</v>
-      </c>
-      <c r="O42" s="27">
-        <v>0</v>
-      </c>
-      <c r="P42" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T42" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U42" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="V42" s="22"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C43" s="20" t="str">
-        <f t="shared" ref="C43" si="0">C42</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="15">
-        <v>16</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L43" s="9">
-        <v>0</v>
-      </c>
-      <c r="M43" s="9">
-        <v>0</v>
-      </c>
-      <c r="N43" s="9">
-        <v>0</v>
-      </c>
-      <c r="O43" s="9">
-        <v>0</v>
-      </c>
-      <c r="P43" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S43" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C44" s="20" t="str">
-        <f t="shared" ref="C44" si="1">C43</f>
-        <v>2025 Final</v>
+      <c r="M43" s="27">
+        <v>0</v>
+      </c>
+      <c r="N43" s="27">
+        <v>0</v>
+      </c>
+      <c r="O43" s="27">
+        <v>0</v>
+      </c>
+      <c r="P43" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T43" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U43" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="V43" s="22"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C44" s="20" t="s">
+        <v>56</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="E44" s="9">
+        <v>0</v>
+      </c>
+      <c r="F44" s="15">
+        <f>F43+1</f>
+        <v>2</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>30</v>
@@ -1631,13 +1669,13 @@
         <v>30</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="L44" s="9">
         <v>0</v>
@@ -1664,67 +1702,61 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C45" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="22" t="s">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C45" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="23">
-        <v>0</v>
-      </c>
-      <c r="F45" s="24">
-        <v>1</v>
-      </c>
-      <c r="G45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="J45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="K45" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="L45" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M45" s="27">
-        <v>0</v>
-      </c>
-      <c r="N45" s="27">
-        <v>0</v>
-      </c>
-      <c r="O45" s="27">
-        <v>0</v>
-      </c>
-      <c r="P45" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T45" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U45" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="V45" s="22"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E45" s="9">
+        <v>0</v>
+      </c>
+      <c r="F45" s="15">
+        <f t="shared" ref="F45:F58" si="2">F44+1</f>
+        <v>3</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L45" s="9">
+        <v>0</v>
+      </c>
+      <c r="M45" s="9">
+        <v>0</v>
+      </c>
+      <c r="N45" s="9">
+        <v>0</v>
+      </c>
+      <c r="O45" s="9">
+        <v>0</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S45" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C46" s="20" t="s">
         <v>56</v>
       </c>
@@ -1735,8 +1767,8 @@
         <v>0</v>
       </c>
       <c r="F46" s="15">
-        <f>F45+1</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>30</v>
@@ -1745,13 +1777,13 @@
         <v>30</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L46" s="9">
         <v>0</v>
@@ -1778,7 +1810,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C47" s="20" t="s">
         <v>56</v>
       </c>
@@ -1789,8 +1821,8 @@
         <v>0</v>
       </c>
       <c r="F47" s="15">
-        <f t="shared" ref="F47:F60" si="2">F46+1</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>30</v>
@@ -1799,13 +1831,13 @@
         <v>30</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L47" s="9">
         <v>0</v>
@@ -1832,7 +1864,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C48" s="20" t="s">
         <v>56</v>
       </c>
@@ -1844,7 +1876,7 @@
       </c>
       <c r="F48" s="15">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>30</v>
@@ -1853,13 +1885,13 @@
         <v>30</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L48" s="9">
         <v>0</v>
@@ -1898,7 +1930,7 @@
       </c>
       <c r="F49" s="15">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>30</v>
@@ -1952,7 +1984,7 @@
       </c>
       <c r="F50" s="15">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G50" s="10" t="s">
         <v>30</v>
@@ -2006,7 +2038,7 @@
       </c>
       <c r="F51" s="15">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G51" s="10" t="s">
         <v>30</v>
@@ -2060,7 +2092,7 @@
       </c>
       <c r="F52" s="15">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G52" s="10" t="s">
         <v>30</v>
@@ -2114,7 +2146,7 @@
       </c>
       <c r="F53" s="15">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G53" s="10" t="s">
         <v>30</v>
@@ -2168,7 +2200,7 @@
       </c>
       <c r="F54" s="15">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>30</v>
@@ -2222,7 +2254,7 @@
       </c>
       <c r="F55" s="15">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G55" s="10" t="s">
         <v>30</v>
@@ -2231,13 +2263,13 @@
         <v>30</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L55" s="9">
         <v>0</v>
@@ -2276,7 +2308,7 @@
       </c>
       <c r="F56" s="15">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>30</v>
@@ -2285,13 +2317,13 @@
         <v>30</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L56" s="9">
         <v>0</v>
@@ -2330,7 +2362,7 @@
       </c>
       <c r="F57" s="15">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>30</v>
@@ -2339,13 +2371,13 @@
         <v>30</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L57" s="9">
         <v>0</v>
@@ -2373,72 +2405,74 @@
       </c>
     </row>
     <row r="58" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C58" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D58" s="20" t="s">
+      <c r="C58" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="9">
-        <v>0</v>
-      </c>
-      <c r="F58" s="15">
+      <c r="E58" s="12">
+        <v>0</v>
+      </c>
+      <c r="F58" s="16">
         <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L58" s="9">
-        <v>0</v>
-      </c>
-      <c r="M58" s="9">
-        <v>0</v>
-      </c>
-      <c r="N58" s="9">
-        <v>0</v>
-      </c>
-      <c r="O58" s="9">
-        <v>0</v>
-      </c>
-      <c r="P58" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S58" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L58" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M58" s="8">
+        <v>1</v>
+      </c>
+      <c r="N58" s="12">
+        <v>0</v>
+      </c>
+      <c r="O58" s="12">
+        <v>0</v>
+      </c>
+      <c r="P58" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
     </row>
     <row r="59" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C59" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D59" s="20" t="s">
+      <c r="C59" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" t="s">
         <v>36</v>
       </c>
-      <c r="E59" s="9">
-        <v>0</v>
+      <c r="E59" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F59" s="15">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G59" s="10" t="s">
         <v>30</v>
@@ -2455,8 +2489,8 @@
       <c r="K59" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L59" s="9">
-        <v>0</v>
+      <c r="L59" s="7">
+        <v>0.7</v>
       </c>
       <c r="M59" s="9">
         <v>0</v>
@@ -2479,76 +2513,80 @@
       <c r="S59" s="9">
         <v>-1</v>
       </c>
+      <c r="T59" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U59" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="60" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C60" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D60" s="21" t="s">
+      <c r="C60" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="12">
-        <v>0</v>
-      </c>
-      <c r="F60" s="16">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L60" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M60" s="8">
-        <v>1</v>
-      </c>
-      <c r="N60" s="12">
-        <v>0</v>
-      </c>
-      <c r="O60" s="12">
-        <v>0</v>
-      </c>
-      <c r="P60" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
+      <c r="E60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="15">
+        <f>F59+1</f>
+        <v>2</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L60" s="9">
+        <v>0</v>
+      </c>
+      <c r="M60" s="9">
+        <v>0</v>
+      </c>
+      <c r="N60" s="9">
+        <v>0</v>
+      </c>
+      <c r="O60" s="9">
+        <v>0</v>
+      </c>
+      <c r="P60" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S60" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="61" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>56</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="C61" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F61" s="15">
-        <v>1</v>
+        <f t="shared" ref="F61:F74" si="3">F60+1</f>
+        <v>3</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>30</v>
@@ -2565,8 +2603,8 @@
       <c r="K61" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L61" s="7">
-        <v>0.7</v>
+      <c r="L61" s="9">
+        <v>0</v>
       </c>
       <c r="M61" s="9">
         <v>0</v>
@@ -2588,12 +2626,6 @@
       </c>
       <c r="S61" s="9">
         <v>-1</v>
-      </c>
-      <c r="T61" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U61" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="62" spans="3:22" x14ac:dyDescent="0.25">
@@ -2607,8 +2639,8 @@
         <v>9</v>
       </c>
       <c r="F62" s="15">
-        <f>F61+1</f>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>30</v>
@@ -2661,8 +2693,8 @@
         <v>9</v>
       </c>
       <c r="F63" s="15">
-        <f t="shared" ref="F63:F76" si="3">F62+1</f>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>30</v>
@@ -2716,7 +2748,7 @@
       </c>
       <c r="F64" s="15">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G64" s="10" t="s">
         <v>30</v>
@@ -2770,7 +2802,7 @@
       </c>
       <c r="F65" s="15">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>30</v>
@@ -2824,7 +2856,7 @@
       </c>
       <c r="F66" s="15">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G66" s="10" t="s">
         <v>30</v>
@@ -2878,7 +2910,7 @@
       </c>
       <c r="F67" s="15">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G67" s="10" t="s">
         <v>30</v>
@@ -2932,7 +2964,7 @@
       </c>
       <c r="F68" s="15">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G68" s="10" t="s">
         <v>30</v>
@@ -2986,7 +3018,7 @@
       </c>
       <c r="F69" s="15">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G69" s="10" t="s">
         <v>30</v>
@@ -3040,7 +3072,7 @@
       </c>
       <c r="F70" s="15">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G70" s="10" t="s">
         <v>30</v>
@@ -3094,7 +3126,7 @@
       </c>
       <c r="F71" s="15">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G71" s="10" t="s">
         <v>30</v>
@@ -3148,7 +3180,7 @@
       </c>
       <c r="F72" s="15">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G72" s="10" t="s">
         <v>30</v>
@@ -3202,7 +3234,7 @@
       </c>
       <c r="F73" s="15">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G73" s="10" t="s">
         <v>30</v>
@@ -3245,72 +3277,74 @@
       </c>
     </row>
     <row r="74" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C74" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D74" s="20" t="s">
+      <c r="C74" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E74" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="15">
+      <c r="E74" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="16">
         <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="G74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L74" s="9">
-        <v>0</v>
-      </c>
-      <c r="M74" s="9">
-        <v>0</v>
-      </c>
-      <c r="N74" s="9">
-        <v>0</v>
-      </c>
-      <c r="O74" s="9">
-        <v>0</v>
-      </c>
-      <c r="P74" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S74" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L74" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M74" s="8">
+        <v>1</v>
+      </c>
+      <c r="N74" s="12">
+        <v>0</v>
+      </c>
+      <c r="O74" s="12">
+        <v>0</v>
+      </c>
+      <c r="P74" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+      <c r="V74" s="3"/>
     </row>
     <row r="75" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C75" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E75" s="9" t="s">
+      <c r="C75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="15">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G75" s="10" t="s">
         <v>30</v>
@@ -3319,13 +3353,13 @@
         <v>30</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="K75" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="L75" s="9">
         <v>0</v>
@@ -3351,76 +3385,80 @@
       <c r="S75" s="9">
         <v>-1</v>
       </c>
+      <c r="T75" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U75" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="76" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C76" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D76" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="16">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K76" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L76" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M76" s="8">
-        <v>1</v>
-      </c>
-      <c r="N76" s="12">
-        <v>0</v>
-      </c>
-      <c r="O76" s="12">
-        <v>0</v>
-      </c>
-      <c r="P76" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T76" s="3"/>
-      <c r="U76" s="3"/>
-      <c r="V76" s="3"/>
+      <c r="C76" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="15">
+        <f>F75+1</f>
+        <v>2</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L76" s="9">
+        <v>0</v>
+      </c>
+      <c r="M76" s="9">
+        <v>0</v>
+      </c>
+      <c r="N76" s="9">
+        <v>0</v>
+      </c>
+      <c r="O76" s="9">
+        <v>0</v>
+      </c>
+      <c r="P76" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S76" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="77" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>56</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="2" t="s">
+      <c r="C77" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="15">
-        <v>1</v>
+        <f t="shared" ref="F77:F90" si="4">F76+1</f>
+        <v>3</v>
       </c>
       <c r="G77" s="10" t="s">
         <v>30</v>
@@ -3460,12 +3498,6 @@
       </c>
       <c r="S77" s="9">
         <v>-1</v>
-      </c>
-      <c r="T77" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U77" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="78" spans="3:22" x14ac:dyDescent="0.25">
@@ -3479,8 +3511,8 @@
         <v>9</v>
       </c>
       <c r="F78" s="15">
-        <f>F77+1</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="G78" s="10" t="s">
         <v>30</v>
@@ -3509,11 +3541,11 @@
       <c r="O78" s="9">
         <v>0</v>
       </c>
-      <c r="P78" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q78" s="9">
-        <v>-1</v>
+      <c r="P78" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q78" s="19">
+        <v>0.4</v>
       </c>
       <c r="R78" s="9">
         <v>-1</v>
@@ -3533,8 +3565,8 @@
         <v>9</v>
       </c>
       <c r="F79" s="15">
-        <f t="shared" ref="F79:F92" si="4">F78+1</f>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="G79" s="10" t="s">
         <v>30</v>
@@ -3563,11 +3595,11 @@
       <c r="O79" s="9">
         <v>0</v>
       </c>
-      <c r="P79" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q79" s="9">
-        <v>-1</v>
+      <c r="P79" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q79" s="19">
+        <v>0.4</v>
       </c>
       <c r="R79" s="9">
         <v>-1</v>
@@ -3588,7 +3620,7 @@
       </c>
       <c r="F80" s="15">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G80" s="10" t="s">
         <v>30</v>
@@ -3642,7 +3674,7 @@
       </c>
       <c r="F81" s="15">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G81" s="10" t="s">
         <v>30</v>
@@ -3696,7 +3728,7 @@
       </c>
       <c r="F82" s="15">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G82" s="10" t="s">
         <v>30</v>
@@ -3750,7 +3782,7 @@
       </c>
       <c r="F83" s="15">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G83" s="10" t="s">
         <v>30</v>
@@ -3804,7 +3836,7 @@
       </c>
       <c r="F84" s="15">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G84" s="10" t="s">
         <v>30</v>
@@ -3858,7 +3890,7 @@
       </c>
       <c r="F85" s="15">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G85" s="10" t="s">
         <v>30</v>
@@ -3887,11 +3919,11 @@
       <c r="O85" s="9">
         <v>0</v>
       </c>
-      <c r="P85" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q85" s="19">
-        <v>0.4</v>
+      <c r="P85" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q85" s="9">
+        <v>-1</v>
       </c>
       <c r="R85" s="9">
         <v>-1</v>
@@ -3912,7 +3944,7 @@
       </c>
       <c r="F86" s="15">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G86" s="10" t="s">
         <v>30</v>
@@ -3941,11 +3973,11 @@
       <c r="O86" s="9">
         <v>0</v>
       </c>
-      <c r="P86" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q86" s="19">
-        <v>0.4</v>
+      <c r="P86" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q86" s="9">
+        <v>-1</v>
       </c>
       <c r="R86" s="9">
         <v>-1</v>
@@ -3966,7 +3998,7 @@
       </c>
       <c r="F87" s="15">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G87" s="10" t="s">
         <v>30</v>
@@ -4020,7 +4052,7 @@
       </c>
       <c r="F88" s="15">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G88" s="10" t="s">
         <v>30</v>
@@ -4049,17 +4081,17 @@
       <c r="O88" s="9">
         <v>0</v>
       </c>
-      <c r="P88" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S88" s="9">
-        <v>-1</v>
+      <c r="P88" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q88" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R88" s="19">
+        <v>67</v>
+      </c>
+      <c r="S88" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="2:22" x14ac:dyDescent="0.25">
@@ -4074,7 +4106,7 @@
       </c>
       <c r="F89" s="15">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G89" s="10" t="s">
         <v>30</v>
@@ -4103,245 +4135,137 @@
       <c r="O89" s="9">
         <v>0</v>
       </c>
-      <c r="P89" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S89" s="9">
-        <v>-1</v>
+      <c r="P89" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q89" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R89" s="19">
+        <v>67</v>
+      </c>
+      <c r="S89" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="21" t="s">
         <v>56</v>
       </c>
       <c r="D90" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E90" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F90" s="15">
+      <c r="E90" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="16">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="G90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L90" s="9">
-        <v>0</v>
-      </c>
-      <c r="M90" s="9">
-        <v>0</v>
-      </c>
-      <c r="N90" s="9">
-        <v>0</v>
-      </c>
-      <c r="O90" s="9">
-        <v>0</v>
-      </c>
-      <c r="P90" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q90" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R90" s="19">
-        <v>67</v>
-      </c>
-      <c r="S90" s="19">
-        <v>72</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L90" s="12">
+        <v>0</v>
+      </c>
+      <c r="M90" s="12">
+        <v>0</v>
+      </c>
+      <c r="N90" s="12">
+        <v>0</v>
+      </c>
+      <c r="O90" s="12">
+        <v>0</v>
+      </c>
+      <c r="P90" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
     </row>
     <row r="91" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C91" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D91" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F91" s="15">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="G91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L91" s="9">
-        <v>0</v>
-      </c>
-      <c r="M91" s="9">
-        <v>0</v>
-      </c>
-      <c r="N91" s="9">
-        <v>0</v>
-      </c>
-      <c r="O91" s="9">
-        <v>0</v>
-      </c>
-      <c r="P91" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q91" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R91" s="19">
-        <v>67</v>
-      </c>
-      <c r="S91" s="19">
-        <v>72</v>
+      <c r="C91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L91" s="13">
+        <v>0</v>
+      </c>
+      <c r="M91" s="13">
+        <v>0</v>
+      </c>
+      <c r="N91" s="13">
+        <v>0</v>
+      </c>
+      <c r="O91" s="13">
+        <v>0</v>
+      </c>
+      <c r="P91" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="R91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="S91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="T91" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U91" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C92" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D92" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F92" s="16">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="G92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L92" s="12">
-        <v>0</v>
-      </c>
-      <c r="M92" s="12">
-        <v>0</v>
-      </c>
-      <c r="N92" s="12">
-        <v>0</v>
-      </c>
-      <c r="O92" s="12">
-        <v>0</v>
-      </c>
-      <c r="P92" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T92" s="3"/>
-      <c r="U92" s="3"/>
-      <c r="V92" s="3"/>
-    </row>
-    <row r="93" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F93" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="L93" s="13">
-        <v>0</v>
-      </c>
-      <c r="M93" s="13">
-        <v>0</v>
-      </c>
-      <c r="N93" s="13">
-        <v>0</v>
-      </c>
-      <c r="O93" s="13">
-        <v>0</v>
-      </c>
-      <c r="P93" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="R93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="S93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="T93" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U93" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="94" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+      <c r="B92" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding single family ductlessHP sample files
</commit_message>
<xml_diff>
--- a/Documentation/T24Res/T24RCustomStdDesign.xlsx
+++ b/Documentation/T24Res/T24RCustomStdDesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\git-vscode\CBECC-Dev\Documentation\T24Res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\SVN\branches\CBECC-Com_MFamRestructure\Documentation\T24Res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDE9C57-C7E1-4939-B768-B6C30AC952B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71481180-D713-48D8-97D8-A5E088BA1223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="2580" windowWidth="26790" windowHeight="14340" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
+    <workbookView xWindow="24549" yWindow="2571" windowWidth="22868" windowHeight="14615" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="67">
   <si>
     <t>;</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>default  -or-  Electricity  -or-  Gas</t>
-  </si>
-  <si>
-    <t>09/18/25 - SAC - modified '2025 Final' LowRiseRes records for DHW, CompactDHW &amp; DrnWtrHtRec data</t>
   </si>
 </sst>
 </file>
@@ -289,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,12 +296,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -438,19 +429,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -767,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C373ABC9-0F2E-48ED-B208-F0F9FC7924F4}">
-  <dimension ref="A1:V94"/>
+  <dimension ref="A1:V92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,8 +767,7 @@
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="9" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.5703125" customWidth="1"/>
@@ -829,7 +814,7 @@
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -837,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -845,7 +830,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -853,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -861,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -869,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -877,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,28 +886,31 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" t="s">
-        <v>15</v>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -930,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -941,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -952,10 +940,10 @@
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -963,10 +951,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -974,37 +962,37 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>19</v>
+      <c r="E22" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>27</v>
+      <c r="E23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E24" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1012,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1023,10 +1011,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,10 +1022,10 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1045,10 +1033,10 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" t="s">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1056,10 +1044,10 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1067,128 +1055,177 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="5" t="s">
+    <row r="34" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F34" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H34" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J34" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K34" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L35" s="8" t="s">
+      <c r="L34" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="M34" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N35" s="8" t="s">
+      <c r="N34" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O35" s="8" t="s">
+      <c r="O34" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P35" s="8" t="s">
+      <c r="P34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Q35" s="8" t="s">
+      <c r="Q34" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="R35" s="8" t="s">
+      <c r="R34" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="S35" s="8" t="s">
+      <c r="S34" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="T35" s="5"/>
-      <c r="U35" s="5"/>
-      <c r="V35" s="5"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>57</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D35" t="s">
         <v>36</v>
       </c>
+      <c r="E35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="15">
+        <v>1</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L35" s="26">
+        <v>0.7</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0</v>
+      </c>
+      <c r="N35" s="9">
+        <v>0</v>
+      </c>
+      <c r="O35" s="9">
+        <v>0</v>
+      </c>
+      <c r="P35" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="T35" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C36" s="20" t="str">
+        <f>C35</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="E36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F36" s="15">
+        <v>16</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="M36" s="7">
         <v>1</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L36" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M36" s="9">
-        <v>0</v>
-      </c>
       <c r="N36" s="9">
         <v>0</v>
       </c>
@@ -1207,14 +1244,10 @@
       <c r="S36" s="9">
         <v>-1</v>
       </c>
-      <c r="T36" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T36" s="10"/>
+      <c r="U36" s="1"/>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C37" s="20" t="str">
         <f>C36</f>
         <v>2025 Final</v>
@@ -1225,8 +1258,8 @@
       <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="15">
-        <v>16</v>
+      <c r="F37" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>30</v>
@@ -1243,11 +1276,11 @@
       <c r="K37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L37" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="M37" s="7">
-        <v>1</v>
+      <c r="L37" s="9">
+        <v>0</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0</v>
       </c>
       <c r="N37" s="9">
         <v>0</v>
@@ -1270,359 +1303,364 @@
       <c r="T37" s="10"/>
       <c r="U37" s="1"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C38" s="20" t="str">
-        <f>C37</f>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C38" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="24">
+        <v>16</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L38" s="27">
+        <v>0</v>
+      </c>
+      <c r="M38" s="27">
+        <v>0</v>
+      </c>
+      <c r="N38" s="27">
+        <v>0</v>
+      </c>
+      <c r="O38" s="27">
+        <v>0</v>
+      </c>
+      <c r="P38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T38" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U38" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="V38" s="22"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C39" s="20" t="str">
+        <f>C38</f>
         <v>2025 Final</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D39" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L39" s="9">
+        <v>0</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0</v>
+      </c>
+      <c r="N39" s="9">
+        <v>0</v>
+      </c>
+      <c r="O39" s="9">
+        <v>0</v>
+      </c>
+      <c r="P39" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S39" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C40" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="24">
+        <v>1</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" s="27">
+        <v>0</v>
+      </c>
+      <c r="M40" s="27">
+        <v>0</v>
+      </c>
+      <c r="N40" s="27">
+        <v>0</v>
+      </c>
+      <c r="O40" s="27">
+        <v>0</v>
+      </c>
+      <c r="P40" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T40" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U40" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="V40" s="22"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C41" s="20" t="str">
+        <f t="shared" ref="C41" si="0">C40</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="15">
+        <v>16</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="L41" s="29">
+        <v>0</v>
+      </c>
+      <c r="M41" s="29">
+        <v>0</v>
+      </c>
+      <c r="N41" s="29">
+        <v>0</v>
+      </c>
+      <c r="O41" s="29">
+        <v>0</v>
+      </c>
+      <c r="P41" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="R41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="S41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C42" s="20" t="str">
+        <f t="shared" ref="C42" si="1">C41</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L42" s="9">
+        <v>0</v>
+      </c>
+      <c r="M42" s="9">
+        <v>0</v>
+      </c>
+      <c r="N42" s="9">
+        <v>0</v>
+      </c>
+      <c r="O42" s="9">
+        <v>0</v>
+      </c>
+      <c r="P42" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S42" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C43" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L38" s="9">
-        <v>0</v>
-      </c>
-      <c r="M38" s="9">
-        <v>0</v>
-      </c>
-      <c r="N38" s="9">
-        <v>0</v>
-      </c>
-      <c r="O38" s="9">
-        <v>0</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="T38" s="10"/>
-      <c r="U38" s="1"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C39" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="24">
+      <c r="E43" s="23">
+        <v>0</v>
+      </c>
+      <c r="F43" s="24">
         <v>1</v>
       </c>
-      <c r="G39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I39" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="L39" s="32">
+      <c r="G43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L43" s="26">
         <v>0.7</v>
       </c>
-      <c r="M39" s="27">
-        <v>0</v>
-      </c>
-      <c r="N39" s="27">
-        <v>0</v>
-      </c>
-      <c r="O39" s="27">
-        <v>0</v>
-      </c>
-      <c r="P39" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T39" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U39" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="V39" s="22"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C40" s="20" t="str">
-        <f>C39</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D40" s="20" t="str">
-        <f>D39</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="15">
-        <v>16</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="K40" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L40" s="33">
-        <v>0.7</v>
-      </c>
-      <c r="M40" s="33">
-        <v>1</v>
-      </c>
-      <c r="N40" s="9">
-        <v>0</v>
-      </c>
-      <c r="O40" s="9">
-        <v>0</v>
-      </c>
-      <c r="P40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S40" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C41" s="20" t="str">
-        <f>C40</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D41" s="20" t="str">
-        <f>D40</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K41" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L41" s="9">
-        <v>0</v>
-      </c>
-      <c r="M41" s="9">
-        <v>0</v>
-      </c>
-      <c r="N41" s="9">
-        <v>0</v>
-      </c>
-      <c r="O41" s="9">
-        <v>0</v>
-      </c>
-      <c r="P41" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S41" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C42" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="24">
-        <v>1</v>
-      </c>
-      <c r="G42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I42" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J42" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="L42" s="27">
-        <v>0</v>
-      </c>
-      <c r="M42" s="27">
-        <v>0</v>
-      </c>
-      <c r="N42" s="27">
-        <v>0</v>
-      </c>
-      <c r="O42" s="27">
-        <v>0</v>
-      </c>
-      <c r="P42" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T42" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U42" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="V42" s="22"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C43" s="20" t="str">
-        <f t="shared" ref="C43" si="0">C42</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="15">
-        <v>16</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L43" s="9">
-        <v>0</v>
-      </c>
-      <c r="M43" s="9">
-        <v>0</v>
-      </c>
-      <c r="N43" s="9">
-        <v>0</v>
-      </c>
-      <c r="O43" s="9">
-        <v>0</v>
-      </c>
-      <c r="P43" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S43" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C44" s="20" t="str">
-        <f t="shared" ref="C44" si="1">C43</f>
-        <v>2025 Final</v>
+      <c r="M43" s="27">
+        <v>0</v>
+      </c>
+      <c r="N43" s="27">
+        <v>0</v>
+      </c>
+      <c r="O43" s="27">
+        <v>0</v>
+      </c>
+      <c r="P43" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T43" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U43" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="V43" s="22"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C44" s="20" t="s">
+        <v>56</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="E44" s="9">
+        <v>0</v>
+      </c>
+      <c r="F44" s="15">
+        <f>F43+1</f>
+        <v>2</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>30</v>
@@ -1631,13 +1669,13 @@
         <v>30</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="L44" s="9">
         <v>0</v>
@@ -1664,67 +1702,61 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C45" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="22" t="s">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C45" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="23">
-        <v>0</v>
-      </c>
-      <c r="F45" s="24">
-        <v>1</v>
-      </c>
-      <c r="G45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="J45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="K45" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="L45" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M45" s="27">
-        <v>0</v>
-      </c>
-      <c r="N45" s="27">
-        <v>0</v>
-      </c>
-      <c r="O45" s="27">
-        <v>0</v>
-      </c>
-      <c r="P45" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T45" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U45" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="V45" s="22"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E45" s="9">
+        <v>0</v>
+      </c>
+      <c r="F45" s="15">
+        <f t="shared" ref="F45:F58" si="2">F44+1</f>
+        <v>3</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L45" s="9">
+        <v>0</v>
+      </c>
+      <c r="M45" s="9">
+        <v>0</v>
+      </c>
+      <c r="N45" s="9">
+        <v>0</v>
+      </c>
+      <c r="O45" s="9">
+        <v>0</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S45" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C46" s="20" t="s">
         <v>56</v>
       </c>
@@ -1735,8 +1767,8 @@
         <v>0</v>
       </c>
       <c r="F46" s="15">
-        <f>F45+1</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>30</v>
@@ -1745,13 +1777,13 @@
         <v>30</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L46" s="9">
         <v>0</v>
@@ -1778,7 +1810,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C47" s="20" t="s">
         <v>56</v>
       </c>
@@ -1789,8 +1821,8 @@
         <v>0</v>
       </c>
       <c r="F47" s="15">
-        <f t="shared" ref="F47:F60" si="2">F46+1</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>30</v>
@@ -1799,13 +1831,13 @@
         <v>30</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L47" s="9">
         <v>0</v>
@@ -1832,7 +1864,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C48" s="20" t="s">
         <v>56</v>
       </c>
@@ -1844,7 +1876,7 @@
       </c>
       <c r="F48" s="15">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>30</v>
@@ -1853,13 +1885,13 @@
         <v>30</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L48" s="9">
         <v>0</v>
@@ -1898,7 +1930,7 @@
       </c>
       <c r="F49" s="15">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>30</v>
@@ -1952,7 +1984,7 @@
       </c>
       <c r="F50" s="15">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G50" s="10" t="s">
         <v>30</v>
@@ -2006,7 +2038,7 @@
       </c>
       <c r="F51" s="15">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G51" s="10" t="s">
         <v>30</v>
@@ -2060,7 +2092,7 @@
       </c>
       <c r="F52" s="15">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G52" s="10" t="s">
         <v>30</v>
@@ -2114,7 +2146,7 @@
       </c>
       <c r="F53" s="15">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G53" s="10" t="s">
         <v>30</v>
@@ -2168,7 +2200,7 @@
       </c>
       <c r="F54" s="15">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>30</v>
@@ -2222,7 +2254,7 @@
       </c>
       <c r="F55" s="15">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G55" s="10" t="s">
         <v>30</v>
@@ -2231,13 +2263,13 @@
         <v>30</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L55" s="9">
         <v>0</v>
@@ -2276,7 +2308,7 @@
       </c>
       <c r="F56" s="15">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>30</v>
@@ -2285,13 +2317,13 @@
         <v>30</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L56" s="9">
         <v>0</v>
@@ -2330,7 +2362,7 @@
       </c>
       <c r="F57" s="15">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>30</v>
@@ -2339,13 +2371,13 @@
         <v>30</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L57" s="9">
         <v>0</v>
@@ -2373,72 +2405,74 @@
       </c>
     </row>
     <row r="58" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C58" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D58" s="20" t="s">
+      <c r="C58" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="9">
-        <v>0</v>
-      </c>
-      <c r="F58" s="15">
+      <c r="E58" s="12">
+        <v>0</v>
+      </c>
+      <c r="F58" s="16">
         <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L58" s="9">
-        <v>0</v>
-      </c>
-      <c r="M58" s="9">
-        <v>0</v>
-      </c>
-      <c r="N58" s="9">
-        <v>0</v>
-      </c>
-      <c r="O58" s="9">
-        <v>0</v>
-      </c>
-      <c r="P58" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S58" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L58" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M58" s="8">
+        <v>1</v>
+      </c>
+      <c r="N58" s="12">
+        <v>0</v>
+      </c>
+      <c r="O58" s="12">
+        <v>0</v>
+      </c>
+      <c r="P58" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
     </row>
     <row r="59" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C59" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D59" s="20" t="s">
+      <c r="C59" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" t="s">
         <v>36</v>
       </c>
-      <c r="E59" s="9">
-        <v>0</v>
+      <c r="E59" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F59" s="15">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G59" s="10" t="s">
         <v>30</v>
@@ -2455,8 +2489,8 @@
       <c r="K59" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L59" s="9">
-        <v>0</v>
+      <c r="L59" s="7">
+        <v>0.7</v>
       </c>
       <c r="M59" s="9">
         <v>0</v>
@@ -2479,76 +2513,80 @@
       <c r="S59" s="9">
         <v>-1</v>
       </c>
+      <c r="T59" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U59" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="60" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C60" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D60" s="21" t="s">
+      <c r="C60" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="12">
-        <v>0</v>
-      </c>
-      <c r="F60" s="16">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L60" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M60" s="8">
-        <v>1</v>
-      </c>
-      <c r="N60" s="12">
-        <v>0</v>
-      </c>
-      <c r="O60" s="12">
-        <v>0</v>
-      </c>
-      <c r="P60" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
+      <c r="E60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="15">
+        <f>F59+1</f>
+        <v>2</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L60" s="9">
+        <v>0</v>
+      </c>
+      <c r="M60" s="9">
+        <v>0</v>
+      </c>
+      <c r="N60" s="9">
+        <v>0</v>
+      </c>
+      <c r="O60" s="9">
+        <v>0</v>
+      </c>
+      <c r="P60" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S60" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="61" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>56</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="C61" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F61" s="15">
-        <v>1</v>
+        <f t="shared" ref="F61:F74" si="3">F60+1</f>
+        <v>3</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>30</v>
@@ -2565,8 +2603,8 @@
       <c r="K61" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L61" s="7">
-        <v>0.7</v>
+      <c r="L61" s="9">
+        <v>0</v>
       </c>
       <c r="M61" s="9">
         <v>0</v>
@@ -2588,12 +2626,6 @@
       </c>
       <c r="S61" s="9">
         <v>-1</v>
-      </c>
-      <c r="T61" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U61" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="62" spans="3:22" x14ac:dyDescent="0.25">
@@ -2607,8 +2639,8 @@
         <v>9</v>
       </c>
       <c r="F62" s="15">
-        <f>F61+1</f>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>30</v>
@@ -2661,8 +2693,8 @@
         <v>9</v>
       </c>
       <c r="F63" s="15">
-        <f t="shared" ref="F63:F76" si="3">F62+1</f>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>30</v>
@@ -2716,7 +2748,7 @@
       </c>
       <c r="F64" s="15">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G64" s="10" t="s">
         <v>30</v>
@@ -2770,7 +2802,7 @@
       </c>
       <c r="F65" s="15">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>30</v>
@@ -2824,7 +2856,7 @@
       </c>
       <c r="F66" s="15">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G66" s="10" t="s">
         <v>30</v>
@@ -2878,7 +2910,7 @@
       </c>
       <c r="F67" s="15">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G67" s="10" t="s">
         <v>30</v>
@@ -2932,7 +2964,7 @@
       </c>
       <c r="F68" s="15">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G68" s="10" t="s">
         <v>30</v>
@@ -2986,7 +3018,7 @@
       </c>
       <c r="F69" s="15">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G69" s="10" t="s">
         <v>30</v>
@@ -3040,7 +3072,7 @@
       </c>
       <c r="F70" s="15">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G70" s="10" t="s">
         <v>30</v>
@@ -3094,7 +3126,7 @@
       </c>
       <c r="F71" s="15">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G71" s="10" t="s">
         <v>30</v>
@@ -3148,7 +3180,7 @@
       </c>
       <c r="F72" s="15">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G72" s="10" t="s">
         <v>30</v>
@@ -3202,7 +3234,7 @@
       </c>
       <c r="F73" s="15">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G73" s="10" t="s">
         <v>30</v>
@@ -3245,72 +3277,74 @@
       </c>
     </row>
     <row r="74" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C74" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D74" s="20" t="s">
+      <c r="C74" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E74" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="15">
+      <c r="E74" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="16">
         <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="G74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L74" s="9">
-        <v>0</v>
-      </c>
-      <c r="M74" s="9">
-        <v>0</v>
-      </c>
-      <c r="N74" s="9">
-        <v>0</v>
-      </c>
-      <c r="O74" s="9">
-        <v>0</v>
-      </c>
-      <c r="P74" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S74" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L74" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M74" s="8">
+        <v>1</v>
+      </c>
+      <c r="N74" s="12">
+        <v>0</v>
+      </c>
+      <c r="O74" s="12">
+        <v>0</v>
+      </c>
+      <c r="P74" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+      <c r="V74" s="3"/>
     </row>
     <row r="75" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C75" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E75" s="9" t="s">
+      <c r="C75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="15">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G75" s="10" t="s">
         <v>30</v>
@@ -3319,13 +3353,13 @@
         <v>30</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="K75" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="L75" s="9">
         <v>0</v>
@@ -3351,76 +3385,80 @@
       <c r="S75" s="9">
         <v>-1</v>
       </c>
+      <c r="T75" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U75" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="76" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C76" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D76" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="16">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K76" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L76" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M76" s="8">
-        <v>1</v>
-      </c>
-      <c r="N76" s="12">
-        <v>0</v>
-      </c>
-      <c r="O76" s="12">
-        <v>0</v>
-      </c>
-      <c r="P76" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T76" s="3"/>
-      <c r="U76" s="3"/>
-      <c r="V76" s="3"/>
+      <c r="C76" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="15">
+        <f>F75+1</f>
+        <v>2</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L76" s="9">
+        <v>0</v>
+      </c>
+      <c r="M76" s="9">
+        <v>0</v>
+      </c>
+      <c r="N76" s="9">
+        <v>0</v>
+      </c>
+      <c r="O76" s="9">
+        <v>0</v>
+      </c>
+      <c r="P76" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S76" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="77" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>56</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="2" t="s">
+      <c r="C77" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="15">
-        <v>1</v>
+        <f t="shared" ref="F77:F90" si="4">F76+1</f>
+        <v>3</v>
       </c>
       <c r="G77" s="10" t="s">
         <v>30</v>
@@ -3460,12 +3498,6 @@
       </c>
       <c r="S77" s="9">
         <v>-1</v>
-      </c>
-      <c r="T77" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U77" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="78" spans="3:22" x14ac:dyDescent="0.25">
@@ -3479,8 +3511,8 @@
         <v>9</v>
       </c>
       <c r="F78" s="15">
-        <f>F77+1</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="G78" s="10" t="s">
         <v>30</v>
@@ -3509,11 +3541,11 @@
       <c r="O78" s="9">
         <v>0</v>
       </c>
-      <c r="P78" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q78" s="9">
-        <v>-1</v>
+      <c r="P78" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q78" s="19">
+        <v>0.4</v>
       </c>
       <c r="R78" s="9">
         <v>-1</v>
@@ -3533,8 +3565,8 @@
         <v>9</v>
       </c>
       <c r="F79" s="15">
-        <f t="shared" ref="F79:F92" si="4">F78+1</f>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="G79" s="10" t="s">
         <v>30</v>
@@ -3563,11 +3595,11 @@
       <c r="O79" s="9">
         <v>0</v>
       </c>
-      <c r="P79" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q79" s="9">
-        <v>-1</v>
+      <c r="P79" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q79" s="19">
+        <v>0.4</v>
       </c>
       <c r="R79" s="9">
         <v>-1</v>
@@ -3588,7 +3620,7 @@
       </c>
       <c r="F80" s="15">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G80" s="10" t="s">
         <v>30</v>
@@ -3642,7 +3674,7 @@
       </c>
       <c r="F81" s="15">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G81" s="10" t="s">
         <v>30</v>
@@ -3696,7 +3728,7 @@
       </c>
       <c r="F82" s="15">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G82" s="10" t="s">
         <v>30</v>
@@ -3750,7 +3782,7 @@
       </c>
       <c r="F83" s="15">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G83" s="10" t="s">
         <v>30</v>
@@ -3804,7 +3836,7 @@
       </c>
       <c r="F84" s="15">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G84" s="10" t="s">
         <v>30</v>
@@ -3858,7 +3890,7 @@
       </c>
       <c r="F85" s="15">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G85" s="10" t="s">
         <v>30</v>
@@ -3887,11 +3919,11 @@
       <c r="O85" s="9">
         <v>0</v>
       </c>
-      <c r="P85" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q85" s="19">
-        <v>0.4</v>
+      <c r="P85" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q85" s="9">
+        <v>-1</v>
       </c>
       <c r="R85" s="9">
         <v>-1</v>
@@ -3912,7 +3944,7 @@
       </c>
       <c r="F86" s="15">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G86" s="10" t="s">
         <v>30</v>
@@ -3941,11 +3973,11 @@
       <c r="O86" s="9">
         <v>0</v>
       </c>
-      <c r="P86" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q86" s="19">
-        <v>0.4</v>
+      <c r="P86" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q86" s="9">
+        <v>-1</v>
       </c>
       <c r="R86" s="9">
         <v>-1</v>
@@ -3966,7 +3998,7 @@
       </c>
       <c r="F87" s="15">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G87" s="10" t="s">
         <v>30</v>
@@ -4020,7 +4052,7 @@
       </c>
       <c r="F88" s="15">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G88" s="10" t="s">
         <v>30</v>
@@ -4049,17 +4081,17 @@
       <c r="O88" s="9">
         <v>0</v>
       </c>
-      <c r="P88" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S88" s="9">
-        <v>-1</v>
+      <c r="P88" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q88" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R88" s="19">
+        <v>67</v>
+      </c>
+      <c r="S88" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="2:22" x14ac:dyDescent="0.25">
@@ -4074,7 +4106,7 @@
       </c>
       <c r="F89" s="15">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G89" s="10" t="s">
         <v>30</v>
@@ -4103,245 +4135,137 @@
       <c r="O89" s="9">
         <v>0</v>
       </c>
-      <c r="P89" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S89" s="9">
-        <v>-1</v>
+      <c r="P89" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q89" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R89" s="19">
+        <v>67</v>
+      </c>
+      <c r="S89" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="21" t="s">
         <v>56</v>
       </c>
       <c r="D90" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E90" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F90" s="15">
+      <c r="E90" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="16">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="G90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L90" s="9">
-        <v>0</v>
-      </c>
-      <c r="M90" s="9">
-        <v>0</v>
-      </c>
-      <c r="N90" s="9">
-        <v>0</v>
-      </c>
-      <c r="O90" s="9">
-        <v>0</v>
-      </c>
-      <c r="P90" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q90" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R90" s="19">
-        <v>67</v>
-      </c>
-      <c r="S90" s="19">
-        <v>72</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L90" s="12">
+        <v>0</v>
+      </c>
+      <c r="M90" s="12">
+        <v>0</v>
+      </c>
+      <c r="N90" s="12">
+        <v>0</v>
+      </c>
+      <c r="O90" s="12">
+        <v>0</v>
+      </c>
+      <c r="P90" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
     </row>
     <row r="91" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C91" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D91" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F91" s="15">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="G91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L91" s="9">
-        <v>0</v>
-      </c>
-      <c r="M91" s="9">
-        <v>0</v>
-      </c>
-      <c r="N91" s="9">
-        <v>0</v>
-      </c>
-      <c r="O91" s="9">
-        <v>0</v>
-      </c>
-      <c r="P91" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q91" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R91" s="19">
-        <v>67</v>
-      </c>
-      <c r="S91" s="19">
-        <v>72</v>
+      <c r="C91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L91" s="13">
+        <v>0</v>
+      </c>
+      <c r="M91" s="13">
+        <v>0</v>
+      </c>
+      <c r="N91" s="13">
+        <v>0</v>
+      </c>
+      <c r="O91" s="13">
+        <v>0</v>
+      </c>
+      <c r="P91" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="R91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="S91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="T91" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U91" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C92" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D92" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F92" s="16">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="G92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L92" s="12">
-        <v>0</v>
-      </c>
-      <c r="M92" s="12">
-        <v>0</v>
-      </c>
-      <c r="N92" s="12">
-        <v>0</v>
-      </c>
-      <c r="O92" s="12">
-        <v>0</v>
-      </c>
-      <c r="P92" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T92" s="3"/>
-      <c r="U92" s="3"/>
-      <c r="V92" s="3"/>
-    </row>
-    <row r="93" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F93" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="L93" s="13">
-        <v>0</v>
-      </c>
-      <c r="M93" s="13">
-        <v>0</v>
-      </c>
-      <c r="N93" s="13">
-        <v>0</v>
-      </c>
-      <c r="O93" s="13">
-        <v>0</v>
-      </c>
-      <c r="P93" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="R93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="S93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="T93" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U93" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="94" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+      <c r="B92" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Branch intermediate commit for form reporting updates
</commit_message>
<xml_diff>
--- a/Documentation/T24Res/T24RCustomStdDesign.xlsx
+++ b/Documentation/T24Res/T24RCustomStdDesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\git-vscode\CBECC-Dev\Documentation\T24Res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\SVN\branches\CBECC-Com_MFamRestructure\Documentation\T24Res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDE9C57-C7E1-4939-B768-B6C30AC952B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71481180-D713-48D8-97D8-A5E088BA1223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="2580" windowWidth="26790" windowHeight="14340" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
+    <workbookView xWindow="24549" yWindow="2571" windowWidth="22868" windowHeight="14615" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="67">
   <si>
     <t>;</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>default  -or-  Electricity  -or-  Gas</t>
-  </si>
-  <si>
-    <t>09/18/25 - SAC - modified '2025 Final' LowRiseRes records for DHW, CompactDHW &amp; DrnWtrHtRec data</t>
   </si>
 </sst>
 </file>
@@ -289,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,12 +296,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -438,19 +429,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -767,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C373ABC9-0F2E-48ED-B208-F0F9FC7924F4}">
-  <dimension ref="A1:V94"/>
+  <dimension ref="A1:V92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,8 +767,7 @@
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="9" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.5703125" customWidth="1"/>
@@ -829,7 +814,7 @@
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -837,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -845,7 +830,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -853,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -861,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -869,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -877,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,28 +886,31 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" t="s">
-        <v>15</v>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -930,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -941,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -952,10 +940,10 @@
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -963,10 +951,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -974,37 +962,37 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>19</v>
+      <c r="E22" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>27</v>
+      <c r="E23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E24" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1012,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1023,10 +1011,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,10 +1022,10 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1045,10 +1033,10 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" t="s">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1056,10 +1044,10 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1067,128 +1055,177 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="5" t="s">
+    <row r="34" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F34" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H34" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J34" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K34" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L35" s="8" t="s">
+      <c r="L34" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="M34" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N35" s="8" t="s">
+      <c r="N34" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O35" s="8" t="s">
+      <c r="O34" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P35" s="8" t="s">
+      <c r="P34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Q35" s="8" t="s">
+      <c r="Q34" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="R35" s="8" t="s">
+      <c r="R34" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="S35" s="8" t="s">
+      <c r="S34" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="T35" s="5"/>
-      <c r="U35" s="5"/>
-      <c r="V35" s="5"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>57</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D35" t="s">
         <v>36</v>
       </c>
+      <c r="E35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="15">
+        <v>1</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L35" s="26">
+        <v>0.7</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0</v>
+      </c>
+      <c r="N35" s="9">
+        <v>0</v>
+      </c>
+      <c r="O35" s="9">
+        <v>0</v>
+      </c>
+      <c r="P35" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="T35" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C36" s="20" t="str">
+        <f>C35</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="E36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F36" s="15">
+        <v>16</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="M36" s="7">
         <v>1</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L36" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M36" s="9">
-        <v>0</v>
-      </c>
       <c r="N36" s="9">
         <v>0</v>
       </c>
@@ -1207,14 +1244,10 @@
       <c r="S36" s="9">
         <v>-1</v>
       </c>
-      <c r="T36" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T36" s="10"/>
+      <c r="U36" s="1"/>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C37" s="20" t="str">
         <f>C36</f>
         <v>2025 Final</v>
@@ -1225,8 +1258,8 @@
       <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="15">
-        <v>16</v>
+      <c r="F37" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>30</v>
@@ -1243,11 +1276,11 @@
       <c r="K37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L37" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="M37" s="7">
-        <v>1</v>
+      <c r="L37" s="9">
+        <v>0</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0</v>
       </c>
       <c r="N37" s="9">
         <v>0</v>
@@ -1270,359 +1303,364 @@
       <c r="T37" s="10"/>
       <c r="U37" s="1"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C38" s="20" t="str">
-        <f>C37</f>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C38" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="24">
+        <v>16</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L38" s="27">
+        <v>0</v>
+      </c>
+      <c r="M38" s="27">
+        <v>0</v>
+      </c>
+      <c r="N38" s="27">
+        <v>0</v>
+      </c>
+      <c r="O38" s="27">
+        <v>0</v>
+      </c>
+      <c r="P38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T38" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U38" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="V38" s="22"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C39" s="20" t="str">
+        <f>C38</f>
         <v>2025 Final</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D39" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L39" s="9">
+        <v>0</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0</v>
+      </c>
+      <c r="N39" s="9">
+        <v>0</v>
+      </c>
+      <c r="O39" s="9">
+        <v>0</v>
+      </c>
+      <c r="P39" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S39" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C40" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="24">
+        <v>1</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" s="27">
+        <v>0</v>
+      </c>
+      <c r="M40" s="27">
+        <v>0</v>
+      </c>
+      <c r="N40" s="27">
+        <v>0</v>
+      </c>
+      <c r="O40" s="27">
+        <v>0</v>
+      </c>
+      <c r="P40" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T40" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U40" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="V40" s="22"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C41" s="20" t="str">
+        <f t="shared" ref="C41" si="0">C40</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="15">
+        <v>16</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="L41" s="29">
+        <v>0</v>
+      </c>
+      <c r="M41" s="29">
+        <v>0</v>
+      </c>
+      <c r="N41" s="29">
+        <v>0</v>
+      </c>
+      <c r="O41" s="29">
+        <v>0</v>
+      </c>
+      <c r="P41" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="R41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="S41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C42" s="20" t="str">
+        <f t="shared" ref="C42" si="1">C41</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L42" s="9">
+        <v>0</v>
+      </c>
+      <c r="M42" s="9">
+        <v>0</v>
+      </c>
+      <c r="N42" s="9">
+        <v>0</v>
+      </c>
+      <c r="O42" s="9">
+        <v>0</v>
+      </c>
+      <c r="P42" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S42" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C43" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L38" s="9">
-        <v>0</v>
-      </c>
-      <c r="M38" s="9">
-        <v>0</v>
-      </c>
-      <c r="N38" s="9">
-        <v>0</v>
-      </c>
-      <c r="O38" s="9">
-        <v>0</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="T38" s="10"/>
-      <c r="U38" s="1"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C39" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="24">
+      <c r="E43" s="23">
+        <v>0</v>
+      </c>
+      <c r="F43" s="24">
         <v>1</v>
       </c>
-      <c r="G39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I39" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="L39" s="32">
+      <c r="G43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L43" s="26">
         <v>0.7</v>
       </c>
-      <c r="M39" s="27">
-        <v>0</v>
-      </c>
-      <c r="N39" s="27">
-        <v>0</v>
-      </c>
-      <c r="O39" s="27">
-        <v>0</v>
-      </c>
-      <c r="P39" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T39" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U39" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="V39" s="22"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C40" s="20" t="str">
-        <f>C39</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D40" s="20" t="str">
-        <f>D39</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="15">
-        <v>16</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="K40" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L40" s="33">
-        <v>0.7</v>
-      </c>
-      <c r="M40" s="33">
-        <v>1</v>
-      </c>
-      <c r="N40" s="9">
-        <v>0</v>
-      </c>
-      <c r="O40" s="9">
-        <v>0</v>
-      </c>
-      <c r="P40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S40" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C41" s="20" t="str">
-        <f>C40</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D41" s="20" t="str">
-        <f>D40</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K41" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L41" s="9">
-        <v>0</v>
-      </c>
-      <c r="M41" s="9">
-        <v>0</v>
-      </c>
-      <c r="N41" s="9">
-        <v>0</v>
-      </c>
-      <c r="O41" s="9">
-        <v>0</v>
-      </c>
-      <c r="P41" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S41" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C42" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="24">
-        <v>1</v>
-      </c>
-      <c r="G42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I42" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J42" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="L42" s="27">
-        <v>0</v>
-      </c>
-      <c r="M42" s="27">
-        <v>0</v>
-      </c>
-      <c r="N42" s="27">
-        <v>0</v>
-      </c>
-      <c r="O42" s="27">
-        <v>0</v>
-      </c>
-      <c r="P42" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T42" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U42" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="V42" s="22"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C43" s="20" t="str">
-        <f t="shared" ref="C43" si="0">C42</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="15">
-        <v>16</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L43" s="9">
-        <v>0</v>
-      </c>
-      <c r="M43" s="9">
-        <v>0</v>
-      </c>
-      <c r="N43" s="9">
-        <v>0</v>
-      </c>
-      <c r="O43" s="9">
-        <v>0</v>
-      </c>
-      <c r="P43" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S43" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C44" s="20" t="str">
-        <f t="shared" ref="C44" si="1">C43</f>
-        <v>2025 Final</v>
+      <c r="M43" s="27">
+        <v>0</v>
+      </c>
+      <c r="N43" s="27">
+        <v>0</v>
+      </c>
+      <c r="O43" s="27">
+        <v>0</v>
+      </c>
+      <c r="P43" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T43" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U43" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="V43" s="22"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C44" s="20" t="s">
+        <v>56</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="E44" s="9">
+        <v>0</v>
+      </c>
+      <c r="F44" s="15">
+        <f>F43+1</f>
+        <v>2</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>30</v>
@@ -1631,13 +1669,13 @@
         <v>30</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="L44" s="9">
         <v>0</v>
@@ -1664,67 +1702,61 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C45" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="22" t="s">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C45" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="23">
-        <v>0</v>
-      </c>
-      <c r="F45" s="24">
-        <v>1</v>
-      </c>
-      <c r="G45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="J45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="K45" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="L45" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M45" s="27">
-        <v>0</v>
-      </c>
-      <c r="N45" s="27">
-        <v>0</v>
-      </c>
-      <c r="O45" s="27">
-        <v>0</v>
-      </c>
-      <c r="P45" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T45" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U45" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="V45" s="22"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E45" s="9">
+        <v>0</v>
+      </c>
+      <c r="F45" s="15">
+        <f t="shared" ref="F45:F58" si="2">F44+1</f>
+        <v>3</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L45" s="9">
+        <v>0</v>
+      </c>
+      <c r="M45" s="9">
+        <v>0</v>
+      </c>
+      <c r="N45" s="9">
+        <v>0</v>
+      </c>
+      <c r="O45" s="9">
+        <v>0</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S45" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C46" s="20" t="s">
         <v>56</v>
       </c>
@@ -1735,8 +1767,8 @@
         <v>0</v>
       </c>
       <c r="F46" s="15">
-        <f>F45+1</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>30</v>
@@ -1745,13 +1777,13 @@
         <v>30</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L46" s="9">
         <v>0</v>
@@ -1778,7 +1810,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C47" s="20" t="s">
         <v>56</v>
       </c>
@@ -1789,8 +1821,8 @@
         <v>0</v>
       </c>
       <c r="F47" s="15">
-        <f t="shared" ref="F47:F60" si="2">F46+1</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>30</v>
@@ -1799,13 +1831,13 @@
         <v>30</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L47" s="9">
         <v>0</v>
@@ -1832,7 +1864,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C48" s="20" t="s">
         <v>56</v>
       </c>
@@ -1844,7 +1876,7 @@
       </c>
       <c r="F48" s="15">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>30</v>
@@ -1853,13 +1885,13 @@
         <v>30</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L48" s="9">
         <v>0</v>
@@ -1898,7 +1930,7 @@
       </c>
       <c r="F49" s="15">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>30</v>
@@ -1952,7 +1984,7 @@
       </c>
       <c r="F50" s="15">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G50" s="10" t="s">
         <v>30</v>
@@ -2006,7 +2038,7 @@
       </c>
       <c r="F51" s="15">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G51" s="10" t="s">
         <v>30</v>
@@ -2060,7 +2092,7 @@
       </c>
       <c r="F52" s="15">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G52" s="10" t="s">
         <v>30</v>
@@ -2114,7 +2146,7 @@
       </c>
       <c r="F53" s="15">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G53" s="10" t="s">
         <v>30</v>
@@ -2168,7 +2200,7 @@
       </c>
       <c r="F54" s="15">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>30</v>
@@ -2222,7 +2254,7 @@
       </c>
       <c r="F55" s="15">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G55" s="10" t="s">
         <v>30</v>
@@ -2231,13 +2263,13 @@
         <v>30</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L55" s="9">
         <v>0</v>
@@ -2276,7 +2308,7 @@
       </c>
       <c r="F56" s="15">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>30</v>
@@ -2285,13 +2317,13 @@
         <v>30</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L56" s="9">
         <v>0</v>
@@ -2330,7 +2362,7 @@
       </c>
       <c r="F57" s="15">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>30</v>
@@ -2339,13 +2371,13 @@
         <v>30</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L57" s="9">
         <v>0</v>
@@ -2373,72 +2405,74 @@
       </c>
     </row>
     <row r="58" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C58" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D58" s="20" t="s">
+      <c r="C58" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="9">
-        <v>0</v>
-      </c>
-      <c r="F58" s="15">
+      <c r="E58" s="12">
+        <v>0</v>
+      </c>
+      <c r="F58" s="16">
         <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L58" s="9">
-        <v>0</v>
-      </c>
-      <c r="M58" s="9">
-        <v>0</v>
-      </c>
-      <c r="N58" s="9">
-        <v>0</v>
-      </c>
-      <c r="O58" s="9">
-        <v>0</v>
-      </c>
-      <c r="P58" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S58" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L58" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M58" s="8">
+        <v>1</v>
+      </c>
+      <c r="N58" s="12">
+        <v>0</v>
+      </c>
+      <c r="O58" s="12">
+        <v>0</v>
+      </c>
+      <c r="P58" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
     </row>
     <row r="59" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C59" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D59" s="20" t="s">
+      <c r="C59" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" t="s">
         <v>36</v>
       </c>
-      <c r="E59" s="9">
-        <v>0</v>
+      <c r="E59" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F59" s="15">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G59" s="10" t="s">
         <v>30</v>
@@ -2455,8 +2489,8 @@
       <c r="K59" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L59" s="9">
-        <v>0</v>
+      <c r="L59" s="7">
+        <v>0.7</v>
       </c>
       <c r="M59" s="9">
         <v>0</v>
@@ -2479,76 +2513,80 @@
       <c r="S59" s="9">
         <v>-1</v>
       </c>
+      <c r="T59" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U59" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="60" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C60" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D60" s="21" t="s">
+      <c r="C60" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="12">
-        <v>0</v>
-      </c>
-      <c r="F60" s="16">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L60" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M60" s="8">
-        <v>1</v>
-      </c>
-      <c r="N60" s="12">
-        <v>0</v>
-      </c>
-      <c r="O60" s="12">
-        <v>0</v>
-      </c>
-      <c r="P60" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
+      <c r="E60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="15">
+        <f>F59+1</f>
+        <v>2</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L60" s="9">
+        <v>0</v>
+      </c>
+      <c r="M60" s="9">
+        <v>0</v>
+      </c>
+      <c r="N60" s="9">
+        <v>0</v>
+      </c>
+      <c r="O60" s="9">
+        <v>0</v>
+      </c>
+      <c r="P60" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S60" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="61" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>56</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="C61" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F61" s="15">
-        <v>1</v>
+        <f t="shared" ref="F61:F74" si="3">F60+1</f>
+        <v>3</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>30</v>
@@ -2565,8 +2603,8 @@
       <c r="K61" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L61" s="7">
-        <v>0.7</v>
+      <c r="L61" s="9">
+        <v>0</v>
       </c>
       <c r="M61" s="9">
         <v>0</v>
@@ -2588,12 +2626,6 @@
       </c>
       <c r="S61" s="9">
         <v>-1</v>
-      </c>
-      <c r="T61" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U61" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="62" spans="3:22" x14ac:dyDescent="0.25">
@@ -2607,8 +2639,8 @@
         <v>9</v>
       </c>
       <c r="F62" s="15">
-        <f>F61+1</f>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>30</v>
@@ -2661,8 +2693,8 @@
         <v>9</v>
       </c>
       <c r="F63" s="15">
-        <f t="shared" ref="F63:F76" si="3">F62+1</f>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>30</v>
@@ -2716,7 +2748,7 @@
       </c>
       <c r="F64" s="15">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G64" s="10" t="s">
         <v>30</v>
@@ -2770,7 +2802,7 @@
       </c>
       <c r="F65" s="15">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>30</v>
@@ -2824,7 +2856,7 @@
       </c>
       <c r="F66" s="15">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G66" s="10" t="s">
         <v>30</v>
@@ -2878,7 +2910,7 @@
       </c>
       <c r="F67" s="15">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G67" s="10" t="s">
         <v>30</v>
@@ -2932,7 +2964,7 @@
       </c>
       <c r="F68" s="15">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G68" s="10" t="s">
         <v>30</v>
@@ -2986,7 +3018,7 @@
       </c>
       <c r="F69" s="15">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G69" s="10" t="s">
         <v>30</v>
@@ -3040,7 +3072,7 @@
       </c>
       <c r="F70" s="15">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G70" s="10" t="s">
         <v>30</v>
@@ -3094,7 +3126,7 @@
       </c>
       <c r="F71" s="15">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G71" s="10" t="s">
         <v>30</v>
@@ -3148,7 +3180,7 @@
       </c>
       <c r="F72" s="15">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G72" s="10" t="s">
         <v>30</v>
@@ -3202,7 +3234,7 @@
       </c>
       <c r="F73" s="15">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G73" s="10" t="s">
         <v>30</v>
@@ -3245,72 +3277,74 @@
       </c>
     </row>
     <row r="74" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C74" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D74" s="20" t="s">
+      <c r="C74" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E74" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="15">
+      <c r="E74" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="16">
         <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="G74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L74" s="9">
-        <v>0</v>
-      </c>
-      <c r="M74" s="9">
-        <v>0</v>
-      </c>
-      <c r="N74" s="9">
-        <v>0</v>
-      </c>
-      <c r="O74" s="9">
-        <v>0</v>
-      </c>
-      <c r="P74" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S74" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L74" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M74" s="8">
+        <v>1</v>
+      </c>
+      <c r="N74" s="12">
+        <v>0</v>
+      </c>
+      <c r="O74" s="12">
+        <v>0</v>
+      </c>
+      <c r="P74" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+      <c r="V74" s="3"/>
     </row>
     <row r="75" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C75" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E75" s="9" t="s">
+      <c r="C75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="15">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G75" s="10" t="s">
         <v>30</v>
@@ -3319,13 +3353,13 @@
         <v>30</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="K75" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="L75" s="9">
         <v>0</v>
@@ -3351,76 +3385,80 @@
       <c r="S75" s="9">
         <v>-1</v>
       </c>
+      <c r="T75" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U75" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="76" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C76" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D76" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="16">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K76" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L76" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M76" s="8">
-        <v>1</v>
-      </c>
-      <c r="N76" s="12">
-        <v>0</v>
-      </c>
-      <c r="O76" s="12">
-        <v>0</v>
-      </c>
-      <c r="P76" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T76" s="3"/>
-      <c r="U76" s="3"/>
-      <c r="V76" s="3"/>
+      <c r="C76" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="15">
+        <f>F75+1</f>
+        <v>2</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L76" s="9">
+        <v>0</v>
+      </c>
+      <c r="M76" s="9">
+        <v>0</v>
+      </c>
+      <c r="N76" s="9">
+        <v>0</v>
+      </c>
+      <c r="O76" s="9">
+        <v>0</v>
+      </c>
+      <c r="P76" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S76" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="77" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>56</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="2" t="s">
+      <c r="C77" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="15">
-        <v>1</v>
+        <f t="shared" ref="F77:F90" si="4">F76+1</f>
+        <v>3</v>
       </c>
       <c r="G77" s="10" t="s">
         <v>30</v>
@@ -3460,12 +3498,6 @@
       </c>
       <c r="S77" s="9">
         <v>-1</v>
-      </c>
-      <c r="T77" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U77" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="78" spans="3:22" x14ac:dyDescent="0.25">
@@ -3479,8 +3511,8 @@
         <v>9</v>
       </c>
       <c r="F78" s="15">
-        <f>F77+1</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="G78" s="10" t="s">
         <v>30</v>
@@ -3509,11 +3541,11 @@
       <c r="O78" s="9">
         <v>0</v>
       </c>
-      <c r="P78" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q78" s="9">
-        <v>-1</v>
+      <c r="P78" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q78" s="19">
+        <v>0.4</v>
       </c>
       <c r="R78" s="9">
         <v>-1</v>
@@ -3533,8 +3565,8 @@
         <v>9</v>
       </c>
       <c r="F79" s="15">
-        <f t="shared" ref="F79:F92" si="4">F78+1</f>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="G79" s="10" t="s">
         <v>30</v>
@@ -3563,11 +3595,11 @@
       <c r="O79" s="9">
         <v>0</v>
       </c>
-      <c r="P79" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q79" s="9">
-        <v>-1</v>
+      <c r="P79" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q79" s="19">
+        <v>0.4</v>
       </c>
       <c r="R79" s="9">
         <v>-1</v>
@@ -3588,7 +3620,7 @@
       </c>
       <c r="F80" s="15">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G80" s="10" t="s">
         <v>30</v>
@@ -3642,7 +3674,7 @@
       </c>
       <c r="F81" s="15">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G81" s="10" t="s">
         <v>30</v>
@@ -3696,7 +3728,7 @@
       </c>
       <c r="F82" s="15">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G82" s="10" t="s">
         <v>30</v>
@@ -3750,7 +3782,7 @@
       </c>
       <c r="F83" s="15">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G83" s="10" t="s">
         <v>30</v>
@@ -3804,7 +3836,7 @@
       </c>
       <c r="F84" s="15">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G84" s="10" t="s">
         <v>30</v>
@@ -3858,7 +3890,7 @@
       </c>
       <c r="F85" s="15">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G85" s="10" t="s">
         <v>30</v>
@@ -3887,11 +3919,11 @@
       <c r="O85" s="9">
         <v>0</v>
       </c>
-      <c r="P85" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q85" s="19">
-        <v>0.4</v>
+      <c r="P85" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q85" s="9">
+        <v>-1</v>
       </c>
       <c r="R85" s="9">
         <v>-1</v>
@@ -3912,7 +3944,7 @@
       </c>
       <c r="F86" s="15">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G86" s="10" t="s">
         <v>30</v>
@@ -3941,11 +3973,11 @@
       <c r="O86" s="9">
         <v>0</v>
       </c>
-      <c r="P86" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q86" s="19">
-        <v>0.4</v>
+      <c r="P86" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q86" s="9">
+        <v>-1</v>
       </c>
       <c r="R86" s="9">
         <v>-1</v>
@@ -3966,7 +3998,7 @@
       </c>
       <c r="F87" s="15">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G87" s="10" t="s">
         <v>30</v>
@@ -4020,7 +4052,7 @@
       </c>
       <c r="F88" s="15">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G88" s="10" t="s">
         <v>30</v>
@@ -4049,17 +4081,17 @@
       <c r="O88" s="9">
         <v>0</v>
       </c>
-      <c r="P88" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S88" s="9">
-        <v>-1</v>
+      <c r="P88" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q88" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R88" s="19">
+        <v>67</v>
+      </c>
+      <c r="S88" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="2:22" x14ac:dyDescent="0.25">
@@ -4074,7 +4106,7 @@
       </c>
       <c r="F89" s="15">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G89" s="10" t="s">
         <v>30</v>
@@ -4103,245 +4135,137 @@
       <c r="O89" s="9">
         <v>0</v>
       </c>
-      <c r="P89" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S89" s="9">
-        <v>-1</v>
+      <c r="P89" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q89" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R89" s="19">
+        <v>67</v>
+      </c>
+      <c r="S89" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="21" t="s">
         <v>56</v>
       </c>
       <c r="D90" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E90" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F90" s="15">
+      <c r="E90" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="16">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="G90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L90" s="9">
-        <v>0</v>
-      </c>
-      <c r="M90" s="9">
-        <v>0</v>
-      </c>
-      <c r="N90" s="9">
-        <v>0</v>
-      </c>
-      <c r="O90" s="9">
-        <v>0</v>
-      </c>
-      <c r="P90" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q90" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R90" s="19">
-        <v>67</v>
-      </c>
-      <c r="S90" s="19">
-        <v>72</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L90" s="12">
+        <v>0</v>
+      </c>
+      <c r="M90" s="12">
+        <v>0</v>
+      </c>
+      <c r="N90" s="12">
+        <v>0</v>
+      </c>
+      <c r="O90" s="12">
+        <v>0</v>
+      </c>
+      <c r="P90" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
     </row>
     <row r="91" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C91" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D91" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F91" s="15">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="G91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L91" s="9">
-        <v>0</v>
-      </c>
-      <c r="M91" s="9">
-        <v>0</v>
-      </c>
-      <c r="N91" s="9">
-        <v>0</v>
-      </c>
-      <c r="O91" s="9">
-        <v>0</v>
-      </c>
-      <c r="P91" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q91" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R91" s="19">
-        <v>67</v>
-      </c>
-      <c r="S91" s="19">
-        <v>72</v>
+      <c r="C91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L91" s="13">
+        <v>0</v>
+      </c>
+      <c r="M91" s="13">
+        <v>0</v>
+      </c>
+      <c r="N91" s="13">
+        <v>0</v>
+      </c>
+      <c r="O91" s="13">
+        <v>0</v>
+      </c>
+      <c r="P91" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="R91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="S91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="T91" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U91" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C92" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D92" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F92" s="16">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="G92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L92" s="12">
-        <v>0</v>
-      </c>
-      <c r="M92" s="12">
-        <v>0</v>
-      </c>
-      <c r="N92" s="12">
-        <v>0</v>
-      </c>
-      <c r="O92" s="12">
-        <v>0</v>
-      </c>
-      <c r="P92" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T92" s="3"/>
-      <c r="U92" s="3"/>
-      <c r="V92" s="3"/>
-    </row>
-    <row r="93" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F93" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="L93" s="13">
-        <v>0</v>
-      </c>
-      <c r="M93" s="13">
-        <v>0</v>
-      </c>
-      <c r="N93" s="13">
-        <v>0</v>
-      </c>
-      <c r="O93" s="13">
-        <v>0</v>
-      </c>
-      <c r="P93" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="R93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="S93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="T93" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U93" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="94" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+      <c r="B92" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding SF TDS results for 2025.2/remove 2025.1.0
</commit_message>
<xml_diff>
--- a/Documentation/T24Res/T24RCustomStdDesign.xlsx
+++ b/Documentation/T24Res/T24RCustomStdDesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\git-vscode\CBECC-Dev\Documentation\T24Res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\SVN\branches\CBECC-Com_MFamRestructure\Documentation\T24Res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDE9C57-C7E1-4939-B768-B6C30AC952B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71481180-D713-48D8-97D8-A5E088BA1223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="2580" windowWidth="26790" windowHeight="14340" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
+    <workbookView xWindow="24549" yWindow="2571" windowWidth="22868" windowHeight="14615" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="67">
   <si>
     <t>;</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>default  -or-  Electricity  -or-  Gas</t>
-  </si>
-  <si>
-    <t>09/18/25 - SAC - modified '2025 Final' LowRiseRes records for DHW, CompactDHW &amp; DrnWtrHtRec data</t>
   </si>
 </sst>
 </file>
@@ -289,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,12 +296,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -438,19 +429,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -767,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C373ABC9-0F2E-48ED-B208-F0F9FC7924F4}">
-  <dimension ref="A1:V94"/>
+  <dimension ref="A1:V92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,8 +767,7 @@
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="9" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.5703125" customWidth="1"/>
@@ -829,7 +814,7 @@
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -837,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -845,7 +830,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -853,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -861,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -869,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -877,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,28 +886,31 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" t="s">
-        <v>15</v>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -930,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -941,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -952,10 +940,10 @@
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -963,10 +951,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -974,37 +962,37 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>19</v>
+      <c r="E22" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>27</v>
+      <c r="E23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E24" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1012,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1023,10 +1011,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,10 +1022,10 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1045,10 +1033,10 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" t="s">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1056,10 +1044,10 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1067,128 +1055,177 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="5" t="s">
+    <row r="34" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F34" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H34" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J34" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K34" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L35" s="8" t="s">
+      <c r="L34" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="M34" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N35" s="8" t="s">
+      <c r="N34" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O35" s="8" t="s">
+      <c r="O34" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P35" s="8" t="s">
+      <c r="P34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Q35" s="8" t="s">
+      <c r="Q34" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="R35" s="8" t="s">
+      <c r="R34" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="S35" s="8" t="s">
+      <c r="S34" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="T35" s="5"/>
-      <c r="U35" s="5"/>
-      <c r="V35" s="5"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>57</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D35" t="s">
         <v>36</v>
       </c>
+      <c r="E35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="15">
+        <v>1</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L35" s="26">
+        <v>0.7</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0</v>
+      </c>
+      <c r="N35" s="9">
+        <v>0</v>
+      </c>
+      <c r="O35" s="9">
+        <v>0</v>
+      </c>
+      <c r="P35" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="T35" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C36" s="20" t="str">
+        <f>C35</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="E36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F36" s="15">
+        <v>16</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="M36" s="7">
         <v>1</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L36" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M36" s="9">
-        <v>0</v>
-      </c>
       <c r="N36" s="9">
         <v>0</v>
       </c>
@@ -1207,14 +1244,10 @@
       <c r="S36" s="9">
         <v>-1</v>
       </c>
-      <c r="T36" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T36" s="10"/>
+      <c r="U36" s="1"/>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C37" s="20" t="str">
         <f>C36</f>
         <v>2025 Final</v>
@@ -1225,8 +1258,8 @@
       <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="15">
-        <v>16</v>
+      <c r="F37" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>30</v>
@@ -1243,11 +1276,11 @@
       <c r="K37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L37" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="M37" s="7">
-        <v>1</v>
+      <c r="L37" s="9">
+        <v>0</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0</v>
       </c>
       <c r="N37" s="9">
         <v>0</v>
@@ -1270,359 +1303,364 @@
       <c r="T37" s="10"/>
       <c r="U37" s="1"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C38" s="20" t="str">
-        <f>C37</f>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C38" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="24">
+        <v>16</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L38" s="27">
+        <v>0</v>
+      </c>
+      <c r="M38" s="27">
+        <v>0</v>
+      </c>
+      <c r="N38" s="27">
+        <v>0</v>
+      </c>
+      <c r="O38" s="27">
+        <v>0</v>
+      </c>
+      <c r="P38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T38" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U38" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="V38" s="22"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C39" s="20" t="str">
+        <f>C38</f>
         <v>2025 Final</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D39" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L39" s="9">
+        <v>0</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0</v>
+      </c>
+      <c r="N39" s="9">
+        <v>0</v>
+      </c>
+      <c r="O39" s="9">
+        <v>0</v>
+      </c>
+      <c r="P39" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S39" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C40" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="24">
+        <v>1</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" s="27">
+        <v>0</v>
+      </c>
+      <c r="M40" s="27">
+        <v>0</v>
+      </c>
+      <c r="N40" s="27">
+        <v>0</v>
+      </c>
+      <c r="O40" s="27">
+        <v>0</v>
+      </c>
+      <c r="P40" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T40" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U40" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="V40" s="22"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C41" s="20" t="str">
+        <f t="shared" ref="C41" si="0">C40</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="15">
+        <v>16</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="L41" s="29">
+        <v>0</v>
+      </c>
+      <c r="M41" s="29">
+        <v>0</v>
+      </c>
+      <c r="N41" s="29">
+        <v>0</v>
+      </c>
+      <c r="O41" s="29">
+        <v>0</v>
+      </c>
+      <c r="P41" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="R41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="S41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C42" s="20" t="str">
+        <f t="shared" ref="C42" si="1">C41</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L42" s="9">
+        <v>0</v>
+      </c>
+      <c r="M42" s="9">
+        <v>0</v>
+      </c>
+      <c r="N42" s="9">
+        <v>0</v>
+      </c>
+      <c r="O42" s="9">
+        <v>0</v>
+      </c>
+      <c r="P42" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S42" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C43" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L38" s="9">
-        <v>0</v>
-      </c>
-      <c r="M38" s="9">
-        <v>0</v>
-      </c>
-      <c r="N38" s="9">
-        <v>0</v>
-      </c>
-      <c r="O38" s="9">
-        <v>0</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="T38" s="10"/>
-      <c r="U38" s="1"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C39" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="24">
+      <c r="E43" s="23">
+        <v>0</v>
+      </c>
+      <c r="F43" s="24">
         <v>1</v>
       </c>
-      <c r="G39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I39" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="L39" s="32">
+      <c r="G43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L43" s="26">
         <v>0.7</v>
       </c>
-      <c r="M39" s="27">
-        <v>0</v>
-      </c>
-      <c r="N39" s="27">
-        <v>0</v>
-      </c>
-      <c r="O39" s="27">
-        <v>0</v>
-      </c>
-      <c r="P39" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T39" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U39" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="V39" s="22"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C40" s="20" t="str">
-        <f>C39</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D40" s="20" t="str">
-        <f>D39</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="15">
-        <v>16</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="K40" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L40" s="33">
-        <v>0.7</v>
-      </c>
-      <c r="M40" s="33">
-        <v>1</v>
-      </c>
-      <c r="N40" s="9">
-        <v>0</v>
-      </c>
-      <c r="O40" s="9">
-        <v>0</v>
-      </c>
-      <c r="P40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S40" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C41" s="20" t="str">
-        <f>C40</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D41" s="20" t="str">
-        <f>D40</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K41" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L41" s="9">
-        <v>0</v>
-      </c>
-      <c r="M41" s="9">
-        <v>0</v>
-      </c>
-      <c r="N41" s="9">
-        <v>0</v>
-      </c>
-      <c r="O41" s="9">
-        <v>0</v>
-      </c>
-      <c r="P41" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S41" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C42" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="24">
-        <v>1</v>
-      </c>
-      <c r="G42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I42" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J42" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="L42" s="27">
-        <v>0</v>
-      </c>
-      <c r="M42" s="27">
-        <v>0</v>
-      </c>
-      <c r="N42" s="27">
-        <v>0</v>
-      </c>
-      <c r="O42" s="27">
-        <v>0</v>
-      </c>
-      <c r="P42" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T42" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U42" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="V42" s="22"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C43" s="20" t="str">
-        <f t="shared" ref="C43" si="0">C42</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="15">
-        <v>16</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L43" s="9">
-        <v>0</v>
-      </c>
-      <c r="M43" s="9">
-        <v>0</v>
-      </c>
-      <c r="N43" s="9">
-        <v>0</v>
-      </c>
-      <c r="O43" s="9">
-        <v>0</v>
-      </c>
-      <c r="P43" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S43" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C44" s="20" t="str">
-        <f t="shared" ref="C44" si="1">C43</f>
-        <v>2025 Final</v>
+      <c r="M43" s="27">
+        <v>0</v>
+      </c>
+      <c r="N43" s="27">
+        <v>0</v>
+      </c>
+      <c r="O43" s="27">
+        <v>0</v>
+      </c>
+      <c r="P43" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T43" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U43" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="V43" s="22"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C44" s="20" t="s">
+        <v>56</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="E44" s="9">
+        <v>0</v>
+      </c>
+      <c r="F44" s="15">
+        <f>F43+1</f>
+        <v>2</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>30</v>
@@ -1631,13 +1669,13 @@
         <v>30</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="L44" s="9">
         <v>0</v>
@@ -1664,67 +1702,61 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C45" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="22" t="s">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C45" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="23">
-        <v>0</v>
-      </c>
-      <c r="F45" s="24">
-        <v>1</v>
-      </c>
-      <c r="G45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="J45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="K45" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="L45" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M45" s="27">
-        <v>0</v>
-      </c>
-      <c r="N45" s="27">
-        <v>0</v>
-      </c>
-      <c r="O45" s="27">
-        <v>0</v>
-      </c>
-      <c r="P45" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T45" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U45" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="V45" s="22"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E45" s="9">
+        <v>0</v>
+      </c>
+      <c r="F45" s="15">
+        <f t="shared" ref="F45:F58" si="2">F44+1</f>
+        <v>3</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L45" s="9">
+        <v>0</v>
+      </c>
+      <c r="M45" s="9">
+        <v>0</v>
+      </c>
+      <c r="N45" s="9">
+        <v>0</v>
+      </c>
+      <c r="O45" s="9">
+        <v>0</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S45" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C46" s="20" t="s">
         <v>56</v>
       </c>
@@ -1735,8 +1767,8 @@
         <v>0</v>
       </c>
       <c r="F46" s="15">
-        <f>F45+1</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>30</v>
@@ -1745,13 +1777,13 @@
         <v>30</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L46" s="9">
         <v>0</v>
@@ -1778,7 +1810,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C47" s="20" t="s">
         <v>56</v>
       </c>
@@ -1789,8 +1821,8 @@
         <v>0</v>
       </c>
       <c r="F47" s="15">
-        <f t="shared" ref="F47:F60" si="2">F46+1</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>30</v>
@@ -1799,13 +1831,13 @@
         <v>30</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L47" s="9">
         <v>0</v>
@@ -1832,7 +1864,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C48" s="20" t="s">
         <v>56</v>
       </c>
@@ -1844,7 +1876,7 @@
       </c>
       <c r="F48" s="15">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>30</v>
@@ -1853,13 +1885,13 @@
         <v>30</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L48" s="9">
         <v>0</v>
@@ -1898,7 +1930,7 @@
       </c>
       <c r="F49" s="15">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>30</v>
@@ -1952,7 +1984,7 @@
       </c>
       <c r="F50" s="15">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G50" s="10" t="s">
         <v>30</v>
@@ -2006,7 +2038,7 @@
       </c>
       <c r="F51" s="15">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G51" s="10" t="s">
         <v>30</v>
@@ -2060,7 +2092,7 @@
       </c>
       <c r="F52" s="15">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G52" s="10" t="s">
         <v>30</v>
@@ -2114,7 +2146,7 @@
       </c>
       <c r="F53" s="15">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G53" s="10" t="s">
         <v>30</v>
@@ -2168,7 +2200,7 @@
       </c>
       <c r="F54" s="15">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>30</v>
@@ -2222,7 +2254,7 @@
       </c>
       <c r="F55" s="15">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G55" s="10" t="s">
         <v>30</v>
@@ -2231,13 +2263,13 @@
         <v>30</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L55" s="9">
         <v>0</v>
@@ -2276,7 +2308,7 @@
       </c>
       <c r="F56" s="15">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>30</v>
@@ -2285,13 +2317,13 @@
         <v>30</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L56" s="9">
         <v>0</v>
@@ -2330,7 +2362,7 @@
       </c>
       <c r="F57" s="15">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>30</v>
@@ -2339,13 +2371,13 @@
         <v>30</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L57" s="9">
         <v>0</v>
@@ -2373,72 +2405,74 @@
       </c>
     </row>
     <row r="58" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C58" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D58" s="20" t="s">
+      <c r="C58" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="9">
-        <v>0</v>
-      </c>
-      <c r="F58" s="15">
+      <c r="E58" s="12">
+        <v>0</v>
+      </c>
+      <c r="F58" s="16">
         <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L58" s="9">
-        <v>0</v>
-      </c>
-      <c r="M58" s="9">
-        <v>0</v>
-      </c>
-      <c r="N58" s="9">
-        <v>0</v>
-      </c>
-      <c r="O58" s="9">
-        <v>0</v>
-      </c>
-      <c r="P58" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S58" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L58" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M58" s="8">
+        <v>1</v>
+      </c>
+      <c r="N58" s="12">
+        <v>0</v>
+      </c>
+      <c r="O58" s="12">
+        <v>0</v>
+      </c>
+      <c r="P58" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
     </row>
     <row r="59" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C59" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D59" s="20" t="s">
+      <c r="C59" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" t="s">
         <v>36</v>
       </c>
-      <c r="E59" s="9">
-        <v>0</v>
+      <c r="E59" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F59" s="15">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G59" s="10" t="s">
         <v>30</v>
@@ -2455,8 +2489,8 @@
       <c r="K59" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L59" s="9">
-        <v>0</v>
+      <c r="L59" s="7">
+        <v>0.7</v>
       </c>
       <c r="M59" s="9">
         <v>0</v>
@@ -2479,76 +2513,80 @@
       <c r="S59" s="9">
         <v>-1</v>
       </c>
+      <c r="T59" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U59" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="60" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C60" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D60" s="21" t="s">
+      <c r="C60" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="12">
-        <v>0</v>
-      </c>
-      <c r="F60" s="16">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L60" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M60" s="8">
-        <v>1</v>
-      </c>
-      <c r="N60" s="12">
-        <v>0</v>
-      </c>
-      <c r="O60" s="12">
-        <v>0</v>
-      </c>
-      <c r="P60" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
+      <c r="E60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="15">
+        <f>F59+1</f>
+        <v>2</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L60" s="9">
+        <v>0</v>
+      </c>
+      <c r="M60" s="9">
+        <v>0</v>
+      </c>
+      <c r="N60" s="9">
+        <v>0</v>
+      </c>
+      <c r="O60" s="9">
+        <v>0</v>
+      </c>
+      <c r="P60" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S60" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="61" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>56</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="C61" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F61" s="15">
-        <v>1</v>
+        <f t="shared" ref="F61:F74" si="3">F60+1</f>
+        <v>3</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>30</v>
@@ -2565,8 +2603,8 @@
       <c r="K61" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L61" s="7">
-        <v>0.7</v>
+      <c r="L61" s="9">
+        <v>0</v>
       </c>
       <c r="M61" s="9">
         <v>0</v>
@@ -2588,12 +2626,6 @@
       </c>
       <c r="S61" s="9">
         <v>-1</v>
-      </c>
-      <c r="T61" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U61" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="62" spans="3:22" x14ac:dyDescent="0.25">
@@ -2607,8 +2639,8 @@
         <v>9</v>
       </c>
       <c r="F62" s="15">
-        <f>F61+1</f>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>30</v>
@@ -2661,8 +2693,8 @@
         <v>9</v>
       </c>
       <c r="F63" s="15">
-        <f t="shared" ref="F63:F76" si="3">F62+1</f>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>30</v>
@@ -2716,7 +2748,7 @@
       </c>
       <c r="F64" s="15">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G64" s="10" t="s">
         <v>30</v>
@@ -2770,7 +2802,7 @@
       </c>
       <c r="F65" s="15">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>30</v>
@@ -2824,7 +2856,7 @@
       </c>
       <c r="F66" s="15">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G66" s="10" t="s">
         <v>30</v>
@@ -2878,7 +2910,7 @@
       </c>
       <c r="F67" s="15">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G67" s="10" t="s">
         <v>30</v>
@@ -2932,7 +2964,7 @@
       </c>
       <c r="F68" s="15">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G68" s="10" t="s">
         <v>30</v>
@@ -2986,7 +3018,7 @@
       </c>
       <c r="F69" s="15">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G69" s="10" t="s">
         <v>30</v>
@@ -3040,7 +3072,7 @@
       </c>
       <c r="F70" s="15">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G70" s="10" t="s">
         <v>30</v>
@@ -3094,7 +3126,7 @@
       </c>
       <c r="F71" s="15">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G71" s="10" t="s">
         <v>30</v>
@@ -3148,7 +3180,7 @@
       </c>
       <c r="F72" s="15">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G72" s="10" t="s">
         <v>30</v>
@@ -3202,7 +3234,7 @@
       </c>
       <c r="F73" s="15">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G73" s="10" t="s">
         <v>30</v>
@@ -3245,72 +3277,74 @@
       </c>
     </row>
     <row r="74" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C74" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D74" s="20" t="s">
+      <c r="C74" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E74" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="15">
+      <c r="E74" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="16">
         <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="G74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L74" s="9">
-        <v>0</v>
-      </c>
-      <c r="M74" s="9">
-        <v>0</v>
-      </c>
-      <c r="N74" s="9">
-        <v>0</v>
-      </c>
-      <c r="O74" s="9">
-        <v>0</v>
-      </c>
-      <c r="P74" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S74" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L74" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M74" s="8">
+        <v>1</v>
+      </c>
+      <c r="N74" s="12">
+        <v>0</v>
+      </c>
+      <c r="O74" s="12">
+        <v>0</v>
+      </c>
+      <c r="P74" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+      <c r="V74" s="3"/>
     </row>
     <row r="75" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C75" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E75" s="9" t="s">
+      <c r="C75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="15">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G75" s="10" t="s">
         <v>30</v>
@@ -3319,13 +3353,13 @@
         <v>30</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="K75" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="L75" s="9">
         <v>0</v>
@@ -3351,76 +3385,80 @@
       <c r="S75" s="9">
         <v>-1</v>
       </c>
+      <c r="T75" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U75" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="76" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C76" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D76" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="16">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K76" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L76" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M76" s="8">
-        <v>1</v>
-      </c>
-      <c r="N76" s="12">
-        <v>0</v>
-      </c>
-      <c r="O76" s="12">
-        <v>0</v>
-      </c>
-      <c r="P76" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T76" s="3"/>
-      <c r="U76" s="3"/>
-      <c r="V76" s="3"/>
+      <c r="C76" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="15">
+        <f>F75+1</f>
+        <v>2</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L76" s="9">
+        <v>0</v>
+      </c>
+      <c r="M76" s="9">
+        <v>0</v>
+      </c>
+      <c r="N76" s="9">
+        <v>0</v>
+      </c>
+      <c r="O76" s="9">
+        <v>0</v>
+      </c>
+      <c r="P76" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S76" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="77" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>56</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="2" t="s">
+      <c r="C77" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="15">
-        <v>1</v>
+        <f t="shared" ref="F77:F90" si="4">F76+1</f>
+        <v>3</v>
       </c>
       <c r="G77" s="10" t="s">
         <v>30</v>
@@ -3460,12 +3498,6 @@
       </c>
       <c r="S77" s="9">
         <v>-1</v>
-      </c>
-      <c r="T77" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U77" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="78" spans="3:22" x14ac:dyDescent="0.25">
@@ -3479,8 +3511,8 @@
         <v>9</v>
       </c>
       <c r="F78" s="15">
-        <f>F77+1</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="G78" s="10" t="s">
         <v>30</v>
@@ -3509,11 +3541,11 @@
       <c r="O78" s="9">
         <v>0</v>
       </c>
-      <c r="P78" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q78" s="9">
-        <v>-1</v>
+      <c r="P78" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q78" s="19">
+        <v>0.4</v>
       </c>
       <c r="R78" s="9">
         <v>-1</v>
@@ -3533,8 +3565,8 @@
         <v>9</v>
       </c>
       <c r="F79" s="15">
-        <f t="shared" ref="F79:F92" si="4">F78+1</f>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="G79" s="10" t="s">
         <v>30</v>
@@ -3563,11 +3595,11 @@
       <c r="O79" s="9">
         <v>0</v>
       </c>
-      <c r="P79" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q79" s="9">
-        <v>-1</v>
+      <c r="P79" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q79" s="19">
+        <v>0.4</v>
       </c>
       <c r="R79" s="9">
         <v>-1</v>
@@ -3588,7 +3620,7 @@
       </c>
       <c r="F80" s="15">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G80" s="10" t="s">
         <v>30</v>
@@ -3642,7 +3674,7 @@
       </c>
       <c r="F81" s="15">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G81" s="10" t="s">
         <v>30</v>
@@ -3696,7 +3728,7 @@
       </c>
       <c r="F82" s="15">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G82" s="10" t="s">
         <v>30</v>
@@ -3750,7 +3782,7 @@
       </c>
       <c r="F83" s="15">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G83" s="10" t="s">
         <v>30</v>
@@ -3804,7 +3836,7 @@
       </c>
       <c r="F84" s="15">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G84" s="10" t="s">
         <v>30</v>
@@ -3858,7 +3890,7 @@
       </c>
       <c r="F85" s="15">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G85" s="10" t="s">
         <v>30</v>
@@ -3887,11 +3919,11 @@
       <c r="O85" s="9">
         <v>0</v>
       </c>
-      <c r="P85" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q85" s="19">
-        <v>0.4</v>
+      <c r="P85" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q85" s="9">
+        <v>-1</v>
       </c>
       <c r="R85" s="9">
         <v>-1</v>
@@ -3912,7 +3944,7 @@
       </c>
       <c r="F86" s="15">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G86" s="10" t="s">
         <v>30</v>
@@ -3941,11 +3973,11 @@
       <c r="O86" s="9">
         <v>0</v>
       </c>
-      <c r="P86" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q86" s="19">
-        <v>0.4</v>
+      <c r="P86" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q86" s="9">
+        <v>-1</v>
       </c>
       <c r="R86" s="9">
         <v>-1</v>
@@ -3966,7 +3998,7 @@
       </c>
       <c r="F87" s="15">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G87" s="10" t="s">
         <v>30</v>
@@ -4020,7 +4052,7 @@
       </c>
       <c r="F88" s="15">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G88" s="10" t="s">
         <v>30</v>
@@ -4049,17 +4081,17 @@
       <c r="O88" s="9">
         <v>0</v>
       </c>
-      <c r="P88" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S88" s="9">
-        <v>-1</v>
+      <c r="P88" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q88" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R88" s="19">
+        <v>67</v>
+      </c>
+      <c r="S88" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="2:22" x14ac:dyDescent="0.25">
@@ -4074,7 +4106,7 @@
       </c>
       <c r="F89" s="15">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G89" s="10" t="s">
         <v>30</v>
@@ -4103,245 +4135,137 @@
       <c r="O89" s="9">
         <v>0</v>
       </c>
-      <c r="P89" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S89" s="9">
-        <v>-1</v>
+      <c r="P89" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q89" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R89" s="19">
+        <v>67</v>
+      </c>
+      <c r="S89" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="21" t="s">
         <v>56</v>
       </c>
       <c r="D90" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E90" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F90" s="15">
+      <c r="E90" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="16">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="G90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L90" s="9">
-        <v>0</v>
-      </c>
-      <c r="M90" s="9">
-        <v>0</v>
-      </c>
-      <c r="N90" s="9">
-        <v>0</v>
-      </c>
-      <c r="O90" s="9">
-        <v>0</v>
-      </c>
-      <c r="P90" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q90" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R90" s="19">
-        <v>67</v>
-      </c>
-      <c r="S90" s="19">
-        <v>72</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L90" s="12">
+        <v>0</v>
+      </c>
+      <c r="M90" s="12">
+        <v>0</v>
+      </c>
+      <c r="N90" s="12">
+        <v>0</v>
+      </c>
+      <c r="O90" s="12">
+        <v>0</v>
+      </c>
+      <c r="P90" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
     </row>
     <row r="91" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C91" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D91" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F91" s="15">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="G91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L91" s="9">
-        <v>0</v>
-      </c>
-      <c r="M91" s="9">
-        <v>0</v>
-      </c>
-      <c r="N91" s="9">
-        <v>0</v>
-      </c>
-      <c r="O91" s="9">
-        <v>0</v>
-      </c>
-      <c r="P91" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q91" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R91" s="19">
-        <v>67</v>
-      </c>
-      <c r="S91" s="19">
-        <v>72</v>
+      <c r="C91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L91" s="13">
+        <v>0</v>
+      </c>
+      <c r="M91" s="13">
+        <v>0</v>
+      </c>
+      <c r="N91" s="13">
+        <v>0</v>
+      </c>
+      <c r="O91" s="13">
+        <v>0</v>
+      </c>
+      <c r="P91" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="R91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="S91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="T91" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U91" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C92" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D92" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F92" s="16">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="G92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L92" s="12">
-        <v>0</v>
-      </c>
-      <c r="M92" s="12">
-        <v>0</v>
-      </c>
-      <c r="N92" s="12">
-        <v>0</v>
-      </c>
-      <c r="O92" s="12">
-        <v>0</v>
-      </c>
-      <c r="P92" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T92" s="3"/>
-      <c r="U92" s="3"/>
-      <c r="V92" s="3"/>
-    </row>
-    <row r="93" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F93" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="L93" s="13">
-        <v>0</v>
-      </c>
-      <c r="M93" s="13">
-        <v>0</v>
-      </c>
-      <c r="N93" s="13">
-        <v>0</v>
-      </c>
-      <c r="O93" s="13">
-        <v>0</v>
-      </c>
-      <c r="P93" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="R93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="S93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="T93" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U93" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="94" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+      <c r="B92" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue (com) #3670 MFam Title24-2025 Envelope Update - Added Model Check on Area weighted metal framed walls u-factor maximum of 0.151 -  Added Model Checks on ResExtWall 2x4 and 2x6 Wood framed and others Constructions maximum u-factor of 0.095
</commit_message>
<xml_diff>
--- a/Documentation/T24Res/T24RCustomStdDesign.xlsx
+++ b/Documentation/T24Res/T24RCustomStdDesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\git-vscode\CBECC-Dev\Documentation\T24Res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\SVN\branches\CBECC-Com_MFamRestructure\Documentation\T24Res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDE9C57-C7E1-4939-B768-B6C30AC952B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71481180-D713-48D8-97D8-A5E088BA1223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="2580" windowWidth="26790" windowHeight="14340" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
+    <workbookView xWindow="24549" yWindow="2571" windowWidth="22868" windowHeight="14615" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="67">
   <si>
     <t>;</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>default  -or-  Electricity  -or-  Gas</t>
-  </si>
-  <si>
-    <t>09/18/25 - SAC - modified '2025 Final' LowRiseRes records for DHW, CompactDHW &amp; DrnWtrHtRec data</t>
   </si>
 </sst>
 </file>
@@ -289,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,12 +296,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -438,19 +429,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -767,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C373ABC9-0F2E-48ED-B208-F0F9FC7924F4}">
-  <dimension ref="A1:V94"/>
+  <dimension ref="A1:V92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,8 +767,7 @@
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="9" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.5703125" customWidth="1"/>
@@ -829,7 +814,7 @@
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -837,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -845,7 +830,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -853,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -861,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -869,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -877,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,28 +886,31 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" t="s">
-        <v>15</v>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -930,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -941,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -952,10 +940,10 @@
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -963,10 +951,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -974,37 +962,37 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>19</v>
+      <c r="E22" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>27</v>
+      <c r="E23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E24" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1012,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1023,10 +1011,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,10 +1022,10 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1045,10 +1033,10 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" t="s">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1056,10 +1044,10 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1067,128 +1055,177 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="5" t="s">
+    <row r="34" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F34" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H34" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J34" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K34" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L35" s="8" t="s">
+      <c r="L34" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="M34" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N35" s="8" t="s">
+      <c r="N34" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O35" s="8" t="s">
+      <c r="O34" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P35" s="8" t="s">
+      <c r="P34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Q35" s="8" t="s">
+      <c r="Q34" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="R35" s="8" t="s">
+      <c r="R34" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="S35" s="8" t="s">
+      <c r="S34" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="T35" s="5"/>
-      <c r="U35" s="5"/>
-      <c r="V35" s="5"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>57</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D35" t="s">
         <v>36</v>
       </c>
+      <c r="E35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="15">
+        <v>1</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L35" s="26">
+        <v>0.7</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0</v>
+      </c>
+      <c r="N35" s="9">
+        <v>0</v>
+      </c>
+      <c r="O35" s="9">
+        <v>0</v>
+      </c>
+      <c r="P35" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="T35" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C36" s="20" t="str">
+        <f>C35</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="E36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F36" s="15">
+        <v>16</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="M36" s="7">
         <v>1</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L36" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M36" s="9">
-        <v>0</v>
-      </c>
       <c r="N36" s="9">
         <v>0</v>
       </c>
@@ -1207,14 +1244,10 @@
       <c r="S36" s="9">
         <v>-1</v>
       </c>
-      <c r="T36" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T36" s="10"/>
+      <c r="U36" s="1"/>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C37" s="20" t="str">
         <f>C36</f>
         <v>2025 Final</v>
@@ -1225,8 +1258,8 @@
       <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="15">
-        <v>16</v>
+      <c r="F37" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>30</v>
@@ -1243,11 +1276,11 @@
       <c r="K37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L37" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="M37" s="7">
-        <v>1</v>
+      <c r="L37" s="9">
+        <v>0</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0</v>
       </c>
       <c r="N37" s="9">
         <v>0</v>
@@ -1270,359 +1303,364 @@
       <c r="T37" s="10"/>
       <c r="U37" s="1"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C38" s="20" t="str">
-        <f>C37</f>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C38" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="24">
+        <v>16</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L38" s="27">
+        <v>0</v>
+      </c>
+      <c r="M38" s="27">
+        <v>0</v>
+      </c>
+      <c r="N38" s="27">
+        <v>0</v>
+      </c>
+      <c r="O38" s="27">
+        <v>0</v>
+      </c>
+      <c r="P38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T38" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U38" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="V38" s="22"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C39" s="20" t="str">
+        <f>C38</f>
         <v>2025 Final</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D39" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L39" s="9">
+        <v>0</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0</v>
+      </c>
+      <c r="N39" s="9">
+        <v>0</v>
+      </c>
+      <c r="O39" s="9">
+        <v>0</v>
+      </c>
+      <c r="P39" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S39" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C40" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="24">
+        <v>1</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" s="27">
+        <v>0</v>
+      </c>
+      <c r="M40" s="27">
+        <v>0</v>
+      </c>
+      <c r="N40" s="27">
+        <v>0</v>
+      </c>
+      <c r="O40" s="27">
+        <v>0</v>
+      </c>
+      <c r="P40" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T40" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U40" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="V40" s="22"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C41" s="20" t="str">
+        <f t="shared" ref="C41" si="0">C40</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="15">
+        <v>16</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="L41" s="29">
+        <v>0</v>
+      </c>
+      <c r="M41" s="29">
+        <v>0</v>
+      </c>
+      <c r="N41" s="29">
+        <v>0</v>
+      </c>
+      <c r="O41" s="29">
+        <v>0</v>
+      </c>
+      <c r="P41" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="R41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="S41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C42" s="20" t="str">
+        <f t="shared" ref="C42" si="1">C41</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L42" s="9">
+        <v>0</v>
+      </c>
+      <c r="M42" s="9">
+        <v>0</v>
+      </c>
+      <c r="N42" s="9">
+        <v>0</v>
+      </c>
+      <c r="O42" s="9">
+        <v>0</v>
+      </c>
+      <c r="P42" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S42" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C43" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L38" s="9">
-        <v>0</v>
-      </c>
-      <c r="M38" s="9">
-        <v>0</v>
-      </c>
-      <c r="N38" s="9">
-        <v>0</v>
-      </c>
-      <c r="O38" s="9">
-        <v>0</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="T38" s="10"/>
-      <c r="U38" s="1"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C39" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="24">
+      <c r="E43" s="23">
+        <v>0</v>
+      </c>
+      <c r="F43" s="24">
         <v>1</v>
       </c>
-      <c r="G39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I39" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="L39" s="32">
+      <c r="G43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L43" s="26">
         <v>0.7</v>
       </c>
-      <c r="M39" s="27">
-        <v>0</v>
-      </c>
-      <c r="N39" s="27">
-        <v>0</v>
-      </c>
-      <c r="O39" s="27">
-        <v>0</v>
-      </c>
-      <c r="P39" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T39" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U39" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="V39" s="22"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C40" s="20" t="str">
-        <f>C39</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D40" s="20" t="str">
-        <f>D39</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="15">
-        <v>16</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="K40" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L40" s="33">
-        <v>0.7</v>
-      </c>
-      <c r="M40" s="33">
-        <v>1</v>
-      </c>
-      <c r="N40" s="9">
-        <v>0</v>
-      </c>
-      <c r="O40" s="9">
-        <v>0</v>
-      </c>
-      <c r="P40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S40" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C41" s="20" t="str">
-        <f>C40</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D41" s="20" t="str">
-        <f>D40</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K41" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L41" s="9">
-        <v>0</v>
-      </c>
-      <c r="M41" s="9">
-        <v>0</v>
-      </c>
-      <c r="N41" s="9">
-        <v>0</v>
-      </c>
-      <c r="O41" s="9">
-        <v>0</v>
-      </c>
-      <c r="P41" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S41" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C42" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="24">
-        <v>1</v>
-      </c>
-      <c r="G42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I42" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J42" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="L42" s="27">
-        <v>0</v>
-      </c>
-      <c r="M42" s="27">
-        <v>0</v>
-      </c>
-      <c r="N42" s="27">
-        <v>0</v>
-      </c>
-      <c r="O42" s="27">
-        <v>0</v>
-      </c>
-      <c r="P42" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T42" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U42" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="V42" s="22"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C43" s="20" t="str">
-        <f t="shared" ref="C43" si="0">C42</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="15">
-        <v>16</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L43" s="9">
-        <v>0</v>
-      </c>
-      <c r="M43" s="9">
-        <v>0</v>
-      </c>
-      <c r="N43" s="9">
-        <v>0</v>
-      </c>
-      <c r="O43" s="9">
-        <v>0</v>
-      </c>
-      <c r="P43" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S43" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C44" s="20" t="str">
-        <f t="shared" ref="C44" si="1">C43</f>
-        <v>2025 Final</v>
+      <c r="M43" s="27">
+        <v>0</v>
+      </c>
+      <c r="N43" s="27">
+        <v>0</v>
+      </c>
+      <c r="O43" s="27">
+        <v>0</v>
+      </c>
+      <c r="P43" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T43" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U43" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="V43" s="22"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C44" s="20" t="s">
+        <v>56</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="E44" s="9">
+        <v>0</v>
+      </c>
+      <c r="F44" s="15">
+        <f>F43+1</f>
+        <v>2</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>30</v>
@@ -1631,13 +1669,13 @@
         <v>30</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="L44" s="9">
         <v>0</v>
@@ -1664,67 +1702,61 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C45" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="22" t="s">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C45" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="23">
-        <v>0</v>
-      </c>
-      <c r="F45" s="24">
-        <v>1</v>
-      </c>
-      <c r="G45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="J45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="K45" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="L45" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M45" s="27">
-        <v>0</v>
-      </c>
-      <c r="N45" s="27">
-        <v>0</v>
-      </c>
-      <c r="O45" s="27">
-        <v>0</v>
-      </c>
-      <c r="P45" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T45" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U45" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="V45" s="22"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E45" s="9">
+        <v>0</v>
+      </c>
+      <c r="F45" s="15">
+        <f t="shared" ref="F45:F58" si="2">F44+1</f>
+        <v>3</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L45" s="9">
+        <v>0</v>
+      </c>
+      <c r="M45" s="9">
+        <v>0</v>
+      </c>
+      <c r="N45" s="9">
+        <v>0</v>
+      </c>
+      <c r="O45" s="9">
+        <v>0</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S45" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C46" s="20" t="s">
         <v>56</v>
       </c>
@@ -1735,8 +1767,8 @@
         <v>0</v>
       </c>
       <c r="F46" s="15">
-        <f>F45+1</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>30</v>
@@ -1745,13 +1777,13 @@
         <v>30</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L46" s="9">
         <v>0</v>
@@ -1778,7 +1810,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C47" s="20" t="s">
         <v>56</v>
       </c>
@@ -1789,8 +1821,8 @@
         <v>0</v>
       </c>
       <c r="F47" s="15">
-        <f t="shared" ref="F47:F60" si="2">F46+1</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>30</v>
@@ -1799,13 +1831,13 @@
         <v>30</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L47" s="9">
         <v>0</v>
@@ -1832,7 +1864,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C48" s="20" t="s">
         <v>56</v>
       </c>
@@ -1844,7 +1876,7 @@
       </c>
       <c r="F48" s="15">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>30</v>
@@ -1853,13 +1885,13 @@
         <v>30</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L48" s="9">
         <v>0</v>
@@ -1898,7 +1930,7 @@
       </c>
       <c r="F49" s="15">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>30</v>
@@ -1952,7 +1984,7 @@
       </c>
       <c r="F50" s="15">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G50" s="10" t="s">
         <v>30</v>
@@ -2006,7 +2038,7 @@
       </c>
       <c r="F51" s="15">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G51" s="10" t="s">
         <v>30</v>
@@ -2060,7 +2092,7 @@
       </c>
       <c r="F52" s="15">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G52" s="10" t="s">
         <v>30</v>
@@ -2114,7 +2146,7 @@
       </c>
       <c r="F53" s="15">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G53" s="10" t="s">
         <v>30</v>
@@ -2168,7 +2200,7 @@
       </c>
       <c r="F54" s="15">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>30</v>
@@ -2222,7 +2254,7 @@
       </c>
       <c r="F55" s="15">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G55" s="10" t="s">
         <v>30</v>
@@ -2231,13 +2263,13 @@
         <v>30</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L55" s="9">
         <v>0</v>
@@ -2276,7 +2308,7 @@
       </c>
       <c r="F56" s="15">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>30</v>
@@ -2285,13 +2317,13 @@
         <v>30</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L56" s="9">
         <v>0</v>
@@ -2330,7 +2362,7 @@
       </c>
       <c r="F57" s="15">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>30</v>
@@ -2339,13 +2371,13 @@
         <v>30</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L57" s="9">
         <v>0</v>
@@ -2373,72 +2405,74 @@
       </c>
     </row>
     <row r="58" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C58" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D58" s="20" t="s">
+      <c r="C58" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="9">
-        <v>0</v>
-      </c>
-      <c r="F58" s="15">
+      <c r="E58" s="12">
+        <v>0</v>
+      </c>
+      <c r="F58" s="16">
         <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L58" s="9">
-        <v>0</v>
-      </c>
-      <c r="M58" s="9">
-        <v>0</v>
-      </c>
-      <c r="N58" s="9">
-        <v>0</v>
-      </c>
-      <c r="O58" s="9">
-        <v>0</v>
-      </c>
-      <c r="P58" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S58" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L58" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M58" s="8">
+        <v>1</v>
+      </c>
+      <c r="N58" s="12">
+        <v>0</v>
+      </c>
+      <c r="O58" s="12">
+        <v>0</v>
+      </c>
+      <c r="P58" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
     </row>
     <row r="59" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C59" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D59" s="20" t="s">
+      <c r="C59" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" t="s">
         <v>36</v>
       </c>
-      <c r="E59" s="9">
-        <v>0</v>
+      <c r="E59" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F59" s="15">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G59" s="10" t="s">
         <v>30</v>
@@ -2455,8 +2489,8 @@
       <c r="K59" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L59" s="9">
-        <v>0</v>
+      <c r="L59" s="7">
+        <v>0.7</v>
       </c>
       <c r="M59" s="9">
         <v>0</v>
@@ -2479,76 +2513,80 @@
       <c r="S59" s="9">
         <v>-1</v>
       </c>
+      <c r="T59" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U59" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="60" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C60" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D60" s="21" t="s">
+      <c r="C60" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="12">
-        <v>0</v>
-      </c>
-      <c r="F60" s="16">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L60" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M60" s="8">
-        <v>1</v>
-      </c>
-      <c r="N60" s="12">
-        <v>0</v>
-      </c>
-      <c r="O60" s="12">
-        <v>0</v>
-      </c>
-      <c r="P60" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
+      <c r="E60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="15">
+        <f>F59+1</f>
+        <v>2</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L60" s="9">
+        <v>0</v>
+      </c>
+      <c r="M60" s="9">
+        <v>0</v>
+      </c>
+      <c r="N60" s="9">
+        <v>0</v>
+      </c>
+      <c r="O60" s="9">
+        <v>0</v>
+      </c>
+      <c r="P60" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S60" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="61" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>56</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="C61" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F61" s="15">
-        <v>1</v>
+        <f t="shared" ref="F61:F74" si="3">F60+1</f>
+        <v>3</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>30</v>
@@ -2565,8 +2603,8 @@
       <c r="K61" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L61" s="7">
-        <v>0.7</v>
+      <c r="L61" s="9">
+        <v>0</v>
       </c>
       <c r="M61" s="9">
         <v>0</v>
@@ -2588,12 +2626,6 @@
       </c>
       <c r="S61" s="9">
         <v>-1</v>
-      </c>
-      <c r="T61" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U61" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="62" spans="3:22" x14ac:dyDescent="0.25">
@@ -2607,8 +2639,8 @@
         <v>9</v>
       </c>
       <c r="F62" s="15">
-        <f>F61+1</f>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>30</v>
@@ -2661,8 +2693,8 @@
         <v>9</v>
       </c>
       <c r="F63" s="15">
-        <f t="shared" ref="F63:F76" si="3">F62+1</f>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>30</v>
@@ -2716,7 +2748,7 @@
       </c>
       <c r="F64" s="15">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G64" s="10" t="s">
         <v>30</v>
@@ -2770,7 +2802,7 @@
       </c>
       <c r="F65" s="15">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>30</v>
@@ -2824,7 +2856,7 @@
       </c>
       <c r="F66" s="15">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G66" s="10" t="s">
         <v>30</v>
@@ -2878,7 +2910,7 @@
       </c>
       <c r="F67" s="15">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G67" s="10" t="s">
         <v>30</v>
@@ -2932,7 +2964,7 @@
       </c>
       <c r="F68" s="15">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G68" s="10" t="s">
         <v>30</v>
@@ -2986,7 +3018,7 @@
       </c>
       <c r="F69" s="15">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G69" s="10" t="s">
         <v>30</v>
@@ -3040,7 +3072,7 @@
       </c>
       <c r="F70" s="15">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G70" s="10" t="s">
         <v>30</v>
@@ -3094,7 +3126,7 @@
       </c>
       <c r="F71" s="15">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G71" s="10" t="s">
         <v>30</v>
@@ -3148,7 +3180,7 @@
       </c>
       <c r="F72" s="15">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G72" s="10" t="s">
         <v>30</v>
@@ -3202,7 +3234,7 @@
       </c>
       <c r="F73" s="15">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G73" s="10" t="s">
         <v>30</v>
@@ -3245,72 +3277,74 @@
       </c>
     </row>
     <row r="74" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C74" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D74" s="20" t="s">
+      <c r="C74" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E74" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="15">
+      <c r="E74" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="16">
         <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="G74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L74" s="9">
-        <v>0</v>
-      </c>
-      <c r="M74" s="9">
-        <v>0</v>
-      </c>
-      <c r="N74" s="9">
-        <v>0</v>
-      </c>
-      <c r="O74" s="9">
-        <v>0</v>
-      </c>
-      <c r="P74" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S74" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L74" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M74" s="8">
+        <v>1</v>
+      </c>
+      <c r="N74" s="12">
+        <v>0</v>
+      </c>
+      <c r="O74" s="12">
+        <v>0</v>
+      </c>
+      <c r="P74" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+      <c r="V74" s="3"/>
     </row>
     <row r="75" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C75" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E75" s="9" t="s">
+      <c r="C75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="15">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G75" s="10" t="s">
         <v>30</v>
@@ -3319,13 +3353,13 @@
         <v>30</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="K75" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="L75" s="9">
         <v>0</v>
@@ -3351,76 +3385,80 @@
       <c r="S75" s="9">
         <v>-1</v>
       </c>
+      <c r="T75" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U75" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="76" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C76" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D76" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="16">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K76" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L76" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M76" s="8">
-        <v>1</v>
-      </c>
-      <c r="N76" s="12">
-        <v>0</v>
-      </c>
-      <c r="O76" s="12">
-        <v>0</v>
-      </c>
-      <c r="P76" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T76" s="3"/>
-      <c r="U76" s="3"/>
-      <c r="V76" s="3"/>
+      <c r="C76" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="15">
+        <f>F75+1</f>
+        <v>2</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L76" s="9">
+        <v>0</v>
+      </c>
+      <c r="M76" s="9">
+        <v>0</v>
+      </c>
+      <c r="N76" s="9">
+        <v>0</v>
+      </c>
+      <c r="O76" s="9">
+        <v>0</v>
+      </c>
+      <c r="P76" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S76" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="77" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>56</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="2" t="s">
+      <c r="C77" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="15">
-        <v>1</v>
+        <f t="shared" ref="F77:F90" si="4">F76+1</f>
+        <v>3</v>
       </c>
       <c r="G77" s="10" t="s">
         <v>30</v>
@@ -3460,12 +3498,6 @@
       </c>
       <c r="S77" s="9">
         <v>-1</v>
-      </c>
-      <c r="T77" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U77" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="78" spans="3:22" x14ac:dyDescent="0.25">
@@ -3479,8 +3511,8 @@
         <v>9</v>
       </c>
       <c r="F78" s="15">
-        <f>F77+1</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="G78" s="10" t="s">
         <v>30</v>
@@ -3509,11 +3541,11 @@
       <c r="O78" s="9">
         <v>0</v>
       </c>
-      <c r="P78" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q78" s="9">
-        <v>-1</v>
+      <c r="P78" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q78" s="19">
+        <v>0.4</v>
       </c>
       <c r="R78" s="9">
         <v>-1</v>
@@ -3533,8 +3565,8 @@
         <v>9</v>
       </c>
       <c r="F79" s="15">
-        <f t="shared" ref="F79:F92" si="4">F78+1</f>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="G79" s="10" t="s">
         <v>30</v>
@@ -3563,11 +3595,11 @@
       <c r="O79" s="9">
         <v>0</v>
       </c>
-      <c r="P79" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q79" s="9">
-        <v>-1</v>
+      <c r="P79" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q79" s="19">
+        <v>0.4</v>
       </c>
       <c r="R79" s="9">
         <v>-1</v>
@@ -3588,7 +3620,7 @@
       </c>
       <c r="F80" s="15">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G80" s="10" t="s">
         <v>30</v>
@@ -3642,7 +3674,7 @@
       </c>
       <c r="F81" s="15">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G81" s="10" t="s">
         <v>30</v>
@@ -3696,7 +3728,7 @@
       </c>
       <c r="F82" s="15">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G82" s="10" t="s">
         <v>30</v>
@@ -3750,7 +3782,7 @@
       </c>
       <c r="F83" s="15">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G83" s="10" t="s">
         <v>30</v>
@@ -3804,7 +3836,7 @@
       </c>
       <c r="F84" s="15">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G84" s="10" t="s">
         <v>30</v>
@@ -3858,7 +3890,7 @@
       </c>
       <c r="F85" s="15">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G85" s="10" t="s">
         <v>30</v>
@@ -3887,11 +3919,11 @@
       <c r="O85" s="9">
         <v>0</v>
       </c>
-      <c r="P85" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q85" s="19">
-        <v>0.4</v>
+      <c r="P85" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q85" s="9">
+        <v>-1</v>
       </c>
       <c r="R85" s="9">
         <v>-1</v>
@@ -3912,7 +3944,7 @@
       </c>
       <c r="F86" s="15">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G86" s="10" t="s">
         <v>30</v>
@@ -3941,11 +3973,11 @@
       <c r="O86" s="9">
         <v>0</v>
       </c>
-      <c r="P86" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q86" s="19">
-        <v>0.4</v>
+      <c r="P86" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q86" s="9">
+        <v>-1</v>
       </c>
       <c r="R86" s="9">
         <v>-1</v>
@@ -3966,7 +3998,7 @@
       </c>
       <c r="F87" s="15">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G87" s="10" t="s">
         <v>30</v>
@@ -4020,7 +4052,7 @@
       </c>
       <c r="F88" s="15">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G88" s="10" t="s">
         <v>30</v>
@@ -4049,17 +4081,17 @@
       <c r="O88" s="9">
         <v>0</v>
       </c>
-      <c r="P88" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S88" s="9">
-        <v>-1</v>
+      <c r="P88" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q88" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R88" s="19">
+        <v>67</v>
+      </c>
+      <c r="S88" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="2:22" x14ac:dyDescent="0.25">
@@ -4074,7 +4106,7 @@
       </c>
       <c r="F89" s="15">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G89" s="10" t="s">
         <v>30</v>
@@ -4103,245 +4135,137 @@
       <c r="O89" s="9">
         <v>0</v>
       </c>
-      <c r="P89" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S89" s="9">
-        <v>-1</v>
+      <c r="P89" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q89" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R89" s="19">
+        <v>67</v>
+      </c>
+      <c r="S89" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="21" t="s">
         <v>56</v>
       </c>
       <c r="D90" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E90" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F90" s="15">
+      <c r="E90" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="16">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="G90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L90" s="9">
-        <v>0</v>
-      </c>
-      <c r="M90" s="9">
-        <v>0</v>
-      </c>
-      <c r="N90" s="9">
-        <v>0</v>
-      </c>
-      <c r="O90" s="9">
-        <v>0</v>
-      </c>
-      <c r="P90" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q90" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R90" s="19">
-        <v>67</v>
-      </c>
-      <c r="S90" s="19">
-        <v>72</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L90" s="12">
+        <v>0</v>
+      </c>
+      <c r="M90" s="12">
+        <v>0</v>
+      </c>
+      <c r="N90" s="12">
+        <v>0</v>
+      </c>
+      <c r="O90" s="12">
+        <v>0</v>
+      </c>
+      <c r="P90" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
     </row>
     <row r="91" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C91" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D91" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F91" s="15">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="G91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L91" s="9">
-        <v>0</v>
-      </c>
-      <c r="M91" s="9">
-        <v>0</v>
-      </c>
-      <c r="N91" s="9">
-        <v>0</v>
-      </c>
-      <c r="O91" s="9">
-        <v>0</v>
-      </c>
-      <c r="P91" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q91" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R91" s="19">
-        <v>67</v>
-      </c>
-      <c r="S91" s="19">
-        <v>72</v>
+      <c r="C91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L91" s="13">
+        <v>0</v>
+      </c>
+      <c r="M91" s="13">
+        <v>0</v>
+      </c>
+      <c r="N91" s="13">
+        <v>0</v>
+      </c>
+      <c r="O91" s="13">
+        <v>0</v>
+      </c>
+      <c r="P91" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="R91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="S91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="T91" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U91" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C92" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D92" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F92" s="16">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="G92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L92" s="12">
-        <v>0</v>
-      </c>
-      <c r="M92" s="12">
-        <v>0</v>
-      </c>
-      <c r="N92" s="12">
-        <v>0</v>
-      </c>
-      <c r="O92" s="12">
-        <v>0</v>
-      </c>
-      <c r="P92" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T92" s="3"/>
-      <c r="U92" s="3"/>
-      <c r="V92" s="3"/>
-    </row>
-    <row r="93" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F93" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="L93" s="13">
-        <v>0</v>
-      </c>
-      <c r="M93" s="13">
-        <v>0</v>
-      </c>
-      <c r="N93" s="13">
-        <v>0</v>
-      </c>
-      <c r="O93" s="13">
-        <v>0</v>
-      </c>
-      <c r="P93" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="R93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="S93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="T93" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U93" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="94" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+      <c r="B92" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
disable CommunitySolar in '25 analysis but retain for CUAC
</commit_message>
<xml_diff>
--- a/Documentation/T24Res/T24RCustomStdDesign.xlsx
+++ b/Documentation/T24Res/T24RCustomStdDesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\git-vscode\CBECC-Dev\Documentation\T24Res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\SVN\branches\CBECC-Com_MFamRestructure\Documentation\T24Res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDE9C57-C7E1-4939-B768-B6C30AC952B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71481180-D713-48D8-97D8-A5E088BA1223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="2580" windowWidth="26790" windowHeight="14340" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
+    <workbookView xWindow="24549" yWindow="2571" windowWidth="22868" windowHeight="14615" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="67">
   <si>
     <t>;</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>default  -or-  Electricity  -or-  Gas</t>
-  </si>
-  <si>
-    <t>09/18/25 - SAC - modified '2025 Final' LowRiseRes records for DHW, CompactDHW &amp; DrnWtrHtRec data</t>
   </si>
 </sst>
 </file>
@@ -289,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,12 +296,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -438,19 +429,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -767,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C373ABC9-0F2E-48ED-B208-F0F9FC7924F4}">
-  <dimension ref="A1:V94"/>
+  <dimension ref="A1:V92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,8 +767,7 @@
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="9" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.5703125" customWidth="1"/>
@@ -829,7 +814,7 @@
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -837,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -845,7 +830,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -853,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -861,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -869,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -877,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,28 +886,31 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" t="s">
-        <v>15</v>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -930,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -941,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -952,10 +940,10 @@
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -963,10 +951,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -974,37 +962,37 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>19</v>
+      <c r="E22" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>27</v>
+      <c r="E23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E24" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1012,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1023,10 +1011,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,10 +1022,10 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1045,10 +1033,10 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" t="s">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1056,10 +1044,10 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1067,128 +1055,177 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="5" t="s">
+    <row r="34" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F34" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H34" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J34" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K34" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L35" s="8" t="s">
+      <c r="L34" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="M34" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N35" s="8" t="s">
+      <c r="N34" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O35" s="8" t="s">
+      <c r="O34" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P35" s="8" t="s">
+      <c r="P34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Q35" s="8" t="s">
+      <c r="Q34" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="R35" s="8" t="s">
+      <c r="R34" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="S35" s="8" t="s">
+      <c r="S34" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="T35" s="5"/>
-      <c r="U35" s="5"/>
-      <c r="V35" s="5"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>57</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D35" t="s">
         <v>36</v>
       </c>
+      <c r="E35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="15">
+        <v>1</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L35" s="26">
+        <v>0.7</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0</v>
+      </c>
+      <c r="N35" s="9">
+        <v>0</v>
+      </c>
+      <c r="O35" s="9">
+        <v>0</v>
+      </c>
+      <c r="P35" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="T35" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C36" s="20" t="str">
+        <f>C35</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="E36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F36" s="15">
+        <v>16</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="M36" s="7">
         <v>1</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L36" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M36" s="9">
-        <v>0</v>
-      </c>
       <c r="N36" s="9">
         <v>0</v>
       </c>
@@ -1207,14 +1244,10 @@
       <c r="S36" s="9">
         <v>-1</v>
       </c>
-      <c r="T36" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T36" s="10"/>
+      <c r="U36" s="1"/>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C37" s="20" t="str">
         <f>C36</f>
         <v>2025 Final</v>
@@ -1225,8 +1258,8 @@
       <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="15">
-        <v>16</v>
+      <c r="F37" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>30</v>
@@ -1243,11 +1276,11 @@
       <c r="K37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L37" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="M37" s="7">
-        <v>1</v>
+      <c r="L37" s="9">
+        <v>0</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0</v>
       </c>
       <c r="N37" s="9">
         <v>0</v>
@@ -1270,359 +1303,364 @@
       <c r="T37" s="10"/>
       <c r="U37" s="1"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C38" s="20" t="str">
-        <f>C37</f>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C38" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="24">
+        <v>16</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L38" s="27">
+        <v>0</v>
+      </c>
+      <c r="M38" s="27">
+        <v>0</v>
+      </c>
+      <c r="N38" s="27">
+        <v>0</v>
+      </c>
+      <c r="O38" s="27">
+        <v>0</v>
+      </c>
+      <c r="P38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T38" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U38" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="V38" s="22"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C39" s="20" t="str">
+        <f>C38</f>
         <v>2025 Final</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D39" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L39" s="9">
+        <v>0</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0</v>
+      </c>
+      <c r="N39" s="9">
+        <v>0</v>
+      </c>
+      <c r="O39" s="9">
+        <v>0</v>
+      </c>
+      <c r="P39" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S39" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C40" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="24">
+        <v>1</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" s="27">
+        <v>0</v>
+      </c>
+      <c r="M40" s="27">
+        <v>0</v>
+      </c>
+      <c r="N40" s="27">
+        <v>0</v>
+      </c>
+      <c r="O40" s="27">
+        <v>0</v>
+      </c>
+      <c r="P40" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T40" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U40" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="V40" s="22"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C41" s="20" t="str">
+        <f t="shared" ref="C41" si="0">C40</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="15">
+        <v>16</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="L41" s="29">
+        <v>0</v>
+      </c>
+      <c r="M41" s="29">
+        <v>0</v>
+      </c>
+      <c r="N41" s="29">
+        <v>0</v>
+      </c>
+      <c r="O41" s="29">
+        <v>0</v>
+      </c>
+      <c r="P41" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="R41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="S41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C42" s="20" t="str">
+        <f t="shared" ref="C42" si="1">C41</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L42" s="9">
+        <v>0</v>
+      </c>
+      <c r="M42" s="9">
+        <v>0</v>
+      </c>
+      <c r="N42" s="9">
+        <v>0</v>
+      </c>
+      <c r="O42" s="9">
+        <v>0</v>
+      </c>
+      <c r="P42" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S42" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C43" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L38" s="9">
-        <v>0</v>
-      </c>
-      <c r="M38" s="9">
-        <v>0</v>
-      </c>
-      <c r="N38" s="9">
-        <v>0</v>
-      </c>
-      <c r="O38" s="9">
-        <v>0</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="T38" s="10"/>
-      <c r="U38" s="1"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C39" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="24">
+      <c r="E43" s="23">
+        <v>0</v>
+      </c>
+      <c r="F43" s="24">
         <v>1</v>
       </c>
-      <c r="G39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I39" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="L39" s="32">
+      <c r="G43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L43" s="26">
         <v>0.7</v>
       </c>
-      <c r="M39" s="27">
-        <v>0</v>
-      </c>
-      <c r="N39" s="27">
-        <v>0</v>
-      </c>
-      <c r="O39" s="27">
-        <v>0</v>
-      </c>
-      <c r="P39" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T39" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U39" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="V39" s="22"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C40" s="20" t="str">
-        <f>C39</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D40" s="20" t="str">
-        <f>D39</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="15">
-        <v>16</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="K40" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L40" s="33">
-        <v>0.7</v>
-      </c>
-      <c r="M40" s="33">
-        <v>1</v>
-      </c>
-      <c r="N40" s="9">
-        <v>0</v>
-      </c>
-      <c r="O40" s="9">
-        <v>0</v>
-      </c>
-      <c r="P40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S40" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C41" s="20" t="str">
-        <f>C40</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D41" s="20" t="str">
-        <f>D40</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K41" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L41" s="9">
-        <v>0</v>
-      </c>
-      <c r="M41" s="9">
-        <v>0</v>
-      </c>
-      <c r="N41" s="9">
-        <v>0</v>
-      </c>
-      <c r="O41" s="9">
-        <v>0</v>
-      </c>
-      <c r="P41" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S41" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C42" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="24">
-        <v>1</v>
-      </c>
-      <c r="G42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I42" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J42" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="L42" s="27">
-        <v>0</v>
-      </c>
-      <c r="M42" s="27">
-        <v>0</v>
-      </c>
-      <c r="N42" s="27">
-        <v>0</v>
-      </c>
-      <c r="O42" s="27">
-        <v>0</v>
-      </c>
-      <c r="P42" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T42" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U42" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="V42" s="22"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C43" s="20" t="str">
-        <f t="shared" ref="C43" si="0">C42</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="15">
-        <v>16</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L43" s="9">
-        <v>0</v>
-      </c>
-      <c r="M43" s="9">
-        <v>0</v>
-      </c>
-      <c r="N43" s="9">
-        <v>0</v>
-      </c>
-      <c r="O43" s="9">
-        <v>0</v>
-      </c>
-      <c r="P43" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S43" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C44" s="20" t="str">
-        <f t="shared" ref="C44" si="1">C43</f>
-        <v>2025 Final</v>
+      <c r="M43" s="27">
+        <v>0</v>
+      </c>
+      <c r="N43" s="27">
+        <v>0</v>
+      </c>
+      <c r="O43" s="27">
+        <v>0</v>
+      </c>
+      <c r="P43" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T43" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U43" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="V43" s="22"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C44" s="20" t="s">
+        <v>56</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="E44" s="9">
+        <v>0</v>
+      </c>
+      <c r="F44" s="15">
+        <f>F43+1</f>
+        <v>2</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>30</v>
@@ -1631,13 +1669,13 @@
         <v>30</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="L44" s="9">
         <v>0</v>
@@ -1664,67 +1702,61 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C45" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="22" t="s">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C45" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="23">
-        <v>0</v>
-      </c>
-      <c r="F45" s="24">
-        <v>1</v>
-      </c>
-      <c r="G45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="J45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="K45" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="L45" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M45" s="27">
-        <v>0</v>
-      </c>
-      <c r="N45" s="27">
-        <v>0</v>
-      </c>
-      <c r="O45" s="27">
-        <v>0</v>
-      </c>
-      <c r="P45" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T45" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U45" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="V45" s="22"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E45" s="9">
+        <v>0</v>
+      </c>
+      <c r="F45" s="15">
+        <f t="shared" ref="F45:F58" si="2">F44+1</f>
+        <v>3</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L45" s="9">
+        <v>0</v>
+      </c>
+      <c r="M45" s="9">
+        <v>0</v>
+      </c>
+      <c r="N45" s="9">
+        <v>0</v>
+      </c>
+      <c r="O45" s="9">
+        <v>0</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S45" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C46" s="20" t="s">
         <v>56</v>
       </c>
@@ -1735,8 +1767,8 @@
         <v>0</v>
       </c>
       <c r="F46" s="15">
-        <f>F45+1</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>30</v>
@@ -1745,13 +1777,13 @@
         <v>30</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L46" s="9">
         <v>0</v>
@@ -1778,7 +1810,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C47" s="20" t="s">
         <v>56</v>
       </c>
@@ -1789,8 +1821,8 @@
         <v>0</v>
       </c>
       <c r="F47" s="15">
-        <f t="shared" ref="F47:F60" si="2">F46+1</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>30</v>
@@ -1799,13 +1831,13 @@
         <v>30</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L47" s="9">
         <v>0</v>
@@ -1832,7 +1864,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C48" s="20" t="s">
         <v>56</v>
       </c>
@@ -1844,7 +1876,7 @@
       </c>
       <c r="F48" s="15">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>30</v>
@@ -1853,13 +1885,13 @@
         <v>30</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L48" s="9">
         <v>0</v>
@@ -1898,7 +1930,7 @@
       </c>
       <c r="F49" s="15">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>30</v>
@@ -1952,7 +1984,7 @@
       </c>
       <c r="F50" s="15">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G50" s="10" t="s">
         <v>30</v>
@@ -2006,7 +2038,7 @@
       </c>
       <c r="F51" s="15">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G51" s="10" t="s">
         <v>30</v>
@@ -2060,7 +2092,7 @@
       </c>
       <c r="F52" s="15">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G52" s="10" t="s">
         <v>30</v>
@@ -2114,7 +2146,7 @@
       </c>
       <c r="F53" s="15">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G53" s="10" t="s">
         <v>30</v>
@@ -2168,7 +2200,7 @@
       </c>
       <c r="F54" s="15">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>30</v>
@@ -2222,7 +2254,7 @@
       </c>
       <c r="F55" s="15">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G55" s="10" t="s">
         <v>30</v>
@@ -2231,13 +2263,13 @@
         <v>30</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L55" s="9">
         <v>0</v>
@@ -2276,7 +2308,7 @@
       </c>
       <c r="F56" s="15">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>30</v>
@@ -2285,13 +2317,13 @@
         <v>30</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L56" s="9">
         <v>0</v>
@@ -2330,7 +2362,7 @@
       </c>
       <c r="F57" s="15">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>30</v>
@@ -2339,13 +2371,13 @@
         <v>30</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L57" s="9">
         <v>0</v>
@@ -2373,72 +2405,74 @@
       </c>
     </row>
     <row r="58" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C58" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D58" s="20" t="s">
+      <c r="C58" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="9">
-        <v>0</v>
-      </c>
-      <c r="F58" s="15">
+      <c r="E58" s="12">
+        <v>0</v>
+      </c>
+      <c r="F58" s="16">
         <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L58" s="9">
-        <v>0</v>
-      </c>
-      <c r="M58" s="9">
-        <v>0</v>
-      </c>
-      <c r="N58" s="9">
-        <v>0</v>
-      </c>
-      <c r="O58" s="9">
-        <v>0</v>
-      </c>
-      <c r="P58" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S58" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L58" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M58" s="8">
+        <v>1</v>
+      </c>
+      <c r="N58" s="12">
+        <v>0</v>
+      </c>
+      <c r="O58" s="12">
+        <v>0</v>
+      </c>
+      <c r="P58" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
     </row>
     <row r="59" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C59" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D59" s="20" t="s">
+      <c r="C59" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" t="s">
         <v>36</v>
       </c>
-      <c r="E59" s="9">
-        <v>0</v>
+      <c r="E59" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F59" s="15">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G59" s="10" t="s">
         <v>30</v>
@@ -2455,8 +2489,8 @@
       <c r="K59" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L59" s="9">
-        <v>0</v>
+      <c r="L59" s="7">
+        <v>0.7</v>
       </c>
       <c r="M59" s="9">
         <v>0</v>
@@ -2479,76 +2513,80 @@
       <c r="S59" s="9">
         <v>-1</v>
       </c>
+      <c r="T59" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U59" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="60" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C60" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D60" s="21" t="s">
+      <c r="C60" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="12">
-        <v>0</v>
-      </c>
-      <c r="F60" s="16">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L60" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M60" s="8">
-        <v>1</v>
-      </c>
-      <c r="N60" s="12">
-        <v>0</v>
-      </c>
-      <c r="O60" s="12">
-        <v>0</v>
-      </c>
-      <c r="P60" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
+      <c r="E60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="15">
+        <f>F59+1</f>
+        <v>2</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L60" s="9">
+        <v>0</v>
+      </c>
+      <c r="M60" s="9">
+        <v>0</v>
+      </c>
+      <c r="N60" s="9">
+        <v>0</v>
+      </c>
+      <c r="O60" s="9">
+        <v>0</v>
+      </c>
+      <c r="P60" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S60" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="61" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>56</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="C61" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F61" s="15">
-        <v>1</v>
+        <f t="shared" ref="F61:F74" si="3">F60+1</f>
+        <v>3</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>30</v>
@@ -2565,8 +2603,8 @@
       <c r="K61" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L61" s="7">
-        <v>0.7</v>
+      <c r="L61" s="9">
+        <v>0</v>
       </c>
       <c r="M61" s="9">
         <v>0</v>
@@ -2588,12 +2626,6 @@
       </c>
       <c r="S61" s="9">
         <v>-1</v>
-      </c>
-      <c r="T61" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U61" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="62" spans="3:22" x14ac:dyDescent="0.25">
@@ -2607,8 +2639,8 @@
         <v>9</v>
       </c>
       <c r="F62" s="15">
-        <f>F61+1</f>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>30</v>
@@ -2661,8 +2693,8 @@
         <v>9</v>
       </c>
       <c r="F63" s="15">
-        <f t="shared" ref="F63:F76" si="3">F62+1</f>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>30</v>
@@ -2716,7 +2748,7 @@
       </c>
       <c r="F64" s="15">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G64" s="10" t="s">
         <v>30</v>
@@ -2770,7 +2802,7 @@
       </c>
       <c r="F65" s="15">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>30</v>
@@ -2824,7 +2856,7 @@
       </c>
       <c r="F66" s="15">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G66" s="10" t="s">
         <v>30</v>
@@ -2878,7 +2910,7 @@
       </c>
       <c r="F67" s="15">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G67" s="10" t="s">
         <v>30</v>
@@ -2932,7 +2964,7 @@
       </c>
       <c r="F68" s="15">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G68" s="10" t="s">
         <v>30</v>
@@ -2986,7 +3018,7 @@
       </c>
       <c r="F69" s="15">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G69" s="10" t="s">
         <v>30</v>
@@ -3040,7 +3072,7 @@
       </c>
       <c r="F70" s="15">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G70" s="10" t="s">
         <v>30</v>
@@ -3094,7 +3126,7 @@
       </c>
       <c r="F71" s="15">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G71" s="10" t="s">
         <v>30</v>
@@ -3148,7 +3180,7 @@
       </c>
       <c r="F72" s="15">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G72" s="10" t="s">
         <v>30</v>
@@ -3202,7 +3234,7 @@
       </c>
       <c r="F73" s="15">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G73" s="10" t="s">
         <v>30</v>
@@ -3245,72 +3277,74 @@
       </c>
     </row>
     <row r="74" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C74" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D74" s="20" t="s">
+      <c r="C74" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E74" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="15">
+      <c r="E74" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="16">
         <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="G74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L74" s="9">
-        <v>0</v>
-      </c>
-      <c r="M74" s="9">
-        <v>0</v>
-      </c>
-      <c r="N74" s="9">
-        <v>0</v>
-      </c>
-      <c r="O74" s="9">
-        <v>0</v>
-      </c>
-      <c r="P74" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S74" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L74" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M74" s="8">
+        <v>1</v>
+      </c>
+      <c r="N74" s="12">
+        <v>0</v>
+      </c>
+      <c r="O74" s="12">
+        <v>0</v>
+      </c>
+      <c r="P74" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+      <c r="V74" s="3"/>
     </row>
     <row r="75" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C75" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E75" s="9" t="s">
+      <c r="C75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="15">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G75" s="10" t="s">
         <v>30</v>
@@ -3319,13 +3353,13 @@
         <v>30</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="K75" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="L75" s="9">
         <v>0</v>
@@ -3351,76 +3385,80 @@
       <c r="S75" s="9">
         <v>-1</v>
       </c>
+      <c r="T75" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U75" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="76" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C76" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D76" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="16">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K76" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L76" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M76" s="8">
-        <v>1</v>
-      </c>
-      <c r="N76" s="12">
-        <v>0</v>
-      </c>
-      <c r="O76" s="12">
-        <v>0</v>
-      </c>
-      <c r="P76" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T76" s="3"/>
-      <c r="U76" s="3"/>
-      <c r="V76" s="3"/>
+      <c r="C76" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="15">
+        <f>F75+1</f>
+        <v>2</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L76" s="9">
+        <v>0</v>
+      </c>
+      <c r="M76" s="9">
+        <v>0</v>
+      </c>
+      <c r="N76" s="9">
+        <v>0</v>
+      </c>
+      <c r="O76" s="9">
+        <v>0</v>
+      </c>
+      <c r="P76" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S76" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="77" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>56</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="2" t="s">
+      <c r="C77" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="15">
-        <v>1</v>
+        <f t="shared" ref="F77:F90" si="4">F76+1</f>
+        <v>3</v>
       </c>
       <c r="G77" s="10" t="s">
         <v>30</v>
@@ -3460,12 +3498,6 @@
       </c>
       <c r="S77" s="9">
         <v>-1</v>
-      </c>
-      <c r="T77" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U77" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="78" spans="3:22" x14ac:dyDescent="0.25">
@@ -3479,8 +3511,8 @@
         <v>9</v>
       </c>
       <c r="F78" s="15">
-        <f>F77+1</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="G78" s="10" t="s">
         <v>30</v>
@@ -3509,11 +3541,11 @@
       <c r="O78" s="9">
         <v>0</v>
       </c>
-      <c r="P78" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q78" s="9">
-        <v>-1</v>
+      <c r="P78" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q78" s="19">
+        <v>0.4</v>
       </c>
       <c r="R78" s="9">
         <v>-1</v>
@@ -3533,8 +3565,8 @@
         <v>9</v>
       </c>
       <c r="F79" s="15">
-        <f t="shared" ref="F79:F92" si="4">F78+1</f>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="G79" s="10" t="s">
         <v>30</v>
@@ -3563,11 +3595,11 @@
       <c r="O79" s="9">
         <v>0</v>
       </c>
-      <c r="P79" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q79" s="9">
-        <v>-1</v>
+      <c r="P79" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q79" s="19">
+        <v>0.4</v>
       </c>
       <c r="R79" s="9">
         <v>-1</v>
@@ -3588,7 +3620,7 @@
       </c>
       <c r="F80" s="15">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G80" s="10" t="s">
         <v>30</v>
@@ -3642,7 +3674,7 @@
       </c>
       <c r="F81" s="15">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G81" s="10" t="s">
         <v>30</v>
@@ -3696,7 +3728,7 @@
       </c>
       <c r="F82" s="15">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G82" s="10" t="s">
         <v>30</v>
@@ -3750,7 +3782,7 @@
       </c>
       <c r="F83" s="15">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G83" s="10" t="s">
         <v>30</v>
@@ -3804,7 +3836,7 @@
       </c>
       <c r="F84" s="15">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G84" s="10" t="s">
         <v>30</v>
@@ -3858,7 +3890,7 @@
       </c>
       <c r="F85" s="15">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G85" s="10" t="s">
         <v>30</v>
@@ -3887,11 +3919,11 @@
       <c r="O85" s="9">
         <v>0</v>
       </c>
-      <c r="P85" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q85" s="19">
-        <v>0.4</v>
+      <c r="P85" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q85" s="9">
+        <v>-1</v>
       </c>
       <c r="R85" s="9">
         <v>-1</v>
@@ -3912,7 +3944,7 @@
       </c>
       <c r="F86" s="15">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G86" s="10" t="s">
         <v>30</v>
@@ -3941,11 +3973,11 @@
       <c r="O86" s="9">
         <v>0</v>
       </c>
-      <c r="P86" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q86" s="19">
-        <v>0.4</v>
+      <c r="P86" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q86" s="9">
+        <v>-1</v>
       </c>
       <c r="R86" s="9">
         <v>-1</v>
@@ -3966,7 +3998,7 @@
       </c>
       <c r="F87" s="15">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G87" s="10" t="s">
         <v>30</v>
@@ -4020,7 +4052,7 @@
       </c>
       <c r="F88" s="15">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G88" s="10" t="s">
         <v>30</v>
@@ -4049,17 +4081,17 @@
       <c r="O88" s="9">
         <v>0</v>
       </c>
-      <c r="P88" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S88" s="9">
-        <v>-1</v>
+      <c r="P88" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q88" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R88" s="19">
+        <v>67</v>
+      </c>
+      <c r="S88" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="2:22" x14ac:dyDescent="0.25">
@@ -4074,7 +4106,7 @@
       </c>
       <c r="F89" s="15">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G89" s="10" t="s">
         <v>30</v>
@@ -4103,245 +4135,137 @@
       <c r="O89" s="9">
         <v>0</v>
       </c>
-      <c r="P89" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S89" s="9">
-        <v>-1</v>
+      <c r="P89" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q89" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R89" s="19">
+        <v>67</v>
+      </c>
+      <c r="S89" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="21" t="s">
         <v>56</v>
       </c>
       <c r="D90" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E90" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F90" s="15">
+      <c r="E90" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="16">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="G90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L90" s="9">
-        <v>0</v>
-      </c>
-      <c r="M90" s="9">
-        <v>0</v>
-      </c>
-      <c r="N90" s="9">
-        <v>0</v>
-      </c>
-      <c r="O90" s="9">
-        <v>0</v>
-      </c>
-      <c r="P90" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q90" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R90" s="19">
-        <v>67</v>
-      </c>
-      <c r="S90" s="19">
-        <v>72</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L90" s="12">
+        <v>0</v>
+      </c>
+      <c r="M90" s="12">
+        <v>0</v>
+      </c>
+      <c r="N90" s="12">
+        <v>0</v>
+      </c>
+      <c r="O90" s="12">
+        <v>0</v>
+      </c>
+      <c r="P90" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
     </row>
     <row r="91" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C91" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D91" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F91" s="15">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="G91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L91" s="9">
-        <v>0</v>
-      </c>
-      <c r="M91" s="9">
-        <v>0</v>
-      </c>
-      <c r="N91" s="9">
-        <v>0</v>
-      </c>
-      <c r="O91" s="9">
-        <v>0</v>
-      </c>
-      <c r="P91" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q91" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R91" s="19">
-        <v>67</v>
-      </c>
-      <c r="S91" s="19">
-        <v>72</v>
+      <c r="C91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L91" s="13">
+        <v>0</v>
+      </c>
+      <c r="M91" s="13">
+        <v>0</v>
+      </c>
+      <c r="N91" s="13">
+        <v>0</v>
+      </c>
+      <c r="O91" s="13">
+        <v>0</v>
+      </c>
+      <c r="P91" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="R91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="S91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="T91" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U91" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C92" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D92" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F92" s="16">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="G92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L92" s="12">
-        <v>0</v>
-      </c>
-      <c r="M92" s="12">
-        <v>0</v>
-      </c>
-      <c r="N92" s="12">
-        <v>0</v>
-      </c>
-      <c r="O92" s="12">
-        <v>0</v>
-      </c>
-      <c r="P92" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T92" s="3"/>
-      <c r="U92" s="3"/>
-      <c r="V92" s="3"/>
-    </row>
-    <row r="93" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F93" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="L93" s="13">
-        <v>0</v>
-      </c>
-      <c r="M93" s="13">
-        <v>0</v>
-      </c>
-      <c r="N93" s="13">
-        <v>0</v>
-      </c>
-      <c r="O93" s="13">
-        <v>0</v>
-      </c>
-      <c r="P93" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="R93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="S93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="T93" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U93" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="94" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+      <c r="B92" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2025-CBECC-Res-Schema Issue 63 2025 CF1R XML output - Renamed Section_E to Section_Features and moved in XML to follow Section_C - Renamed Section_Ea to Section_ECC and moved in XML to follow Section_Features
</commit_message>
<xml_diff>
--- a/Documentation/T24Res/T24RCustomStdDesign.xlsx
+++ b/Documentation/T24Res/T24RCustomStdDesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\git-vscode\CBECC-Dev\Documentation\T24Res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\SVN\branches\CBECC-Com_MFamRestructure\Documentation\T24Res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDE9C57-C7E1-4939-B768-B6C30AC952B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71481180-D713-48D8-97D8-A5E088BA1223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="2580" windowWidth="26790" windowHeight="14340" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
+    <workbookView xWindow="24549" yWindow="2571" windowWidth="22868" windowHeight="14615" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="67">
   <si>
     <t>;</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>default  -or-  Electricity  -or-  Gas</t>
-  </si>
-  <si>
-    <t>09/18/25 - SAC - modified '2025 Final' LowRiseRes records for DHW, CompactDHW &amp; DrnWtrHtRec data</t>
   </si>
 </sst>
 </file>
@@ -289,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,12 +296,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -438,19 +429,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -767,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C373ABC9-0F2E-48ED-B208-F0F9FC7924F4}">
-  <dimension ref="A1:V94"/>
+  <dimension ref="A1:V92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,8 +767,7 @@
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="9" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.5703125" customWidth="1"/>
@@ -829,7 +814,7 @@
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -837,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -845,7 +830,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -853,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -861,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -869,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -877,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,28 +886,31 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" t="s">
-        <v>15</v>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -930,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -941,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -952,10 +940,10 @@
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -963,10 +951,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -974,37 +962,37 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>19</v>
+      <c r="E22" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>27</v>
+      <c r="E23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E24" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1012,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1023,10 +1011,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,10 +1022,10 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1045,10 +1033,10 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" t="s">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1056,10 +1044,10 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1067,128 +1055,177 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="5" t="s">
+    <row r="34" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F34" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H34" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J34" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K34" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L35" s="8" t="s">
+      <c r="L34" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="M34" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N35" s="8" t="s">
+      <c r="N34" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O35" s="8" t="s">
+      <c r="O34" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P35" s="8" t="s">
+      <c r="P34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Q35" s="8" t="s">
+      <c r="Q34" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="R35" s="8" t="s">
+      <c r="R34" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="S35" s="8" t="s">
+      <c r="S34" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="T35" s="5"/>
-      <c r="U35" s="5"/>
-      <c r="V35" s="5"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>57</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D35" t="s">
         <v>36</v>
       </c>
+      <c r="E35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="15">
+        <v>1</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L35" s="26">
+        <v>0.7</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0</v>
+      </c>
+      <c r="N35" s="9">
+        <v>0</v>
+      </c>
+      <c r="O35" s="9">
+        <v>0</v>
+      </c>
+      <c r="P35" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="T35" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C36" s="20" t="str">
+        <f>C35</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="E36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F36" s="15">
+        <v>16</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="M36" s="7">
         <v>1</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L36" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M36" s="9">
-        <v>0</v>
-      </c>
       <c r="N36" s="9">
         <v>0</v>
       </c>
@@ -1207,14 +1244,10 @@
       <c r="S36" s="9">
         <v>-1</v>
       </c>
-      <c r="T36" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T36" s="10"/>
+      <c r="U36" s="1"/>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C37" s="20" t="str">
         <f>C36</f>
         <v>2025 Final</v>
@@ -1225,8 +1258,8 @@
       <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="15">
-        <v>16</v>
+      <c r="F37" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>30</v>
@@ -1243,11 +1276,11 @@
       <c r="K37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L37" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="M37" s="7">
-        <v>1</v>
+      <c r="L37" s="9">
+        <v>0</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0</v>
       </c>
       <c r="N37" s="9">
         <v>0</v>
@@ -1270,359 +1303,364 @@
       <c r="T37" s="10"/>
       <c r="U37" s="1"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C38" s="20" t="str">
-        <f>C37</f>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C38" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="24">
+        <v>16</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L38" s="27">
+        <v>0</v>
+      </c>
+      <c r="M38" s="27">
+        <v>0</v>
+      </c>
+      <c r="N38" s="27">
+        <v>0</v>
+      </c>
+      <c r="O38" s="27">
+        <v>0</v>
+      </c>
+      <c r="P38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T38" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U38" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="V38" s="22"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C39" s="20" t="str">
+        <f>C38</f>
         <v>2025 Final</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D39" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L39" s="9">
+        <v>0</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0</v>
+      </c>
+      <c r="N39" s="9">
+        <v>0</v>
+      </c>
+      <c r="O39" s="9">
+        <v>0</v>
+      </c>
+      <c r="P39" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S39" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C40" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="24">
+        <v>1</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" s="27">
+        <v>0</v>
+      </c>
+      <c r="M40" s="27">
+        <v>0</v>
+      </c>
+      <c r="N40" s="27">
+        <v>0</v>
+      </c>
+      <c r="O40" s="27">
+        <v>0</v>
+      </c>
+      <c r="P40" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T40" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U40" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="V40" s="22"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C41" s="20" t="str">
+        <f t="shared" ref="C41" si="0">C40</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="15">
+        <v>16</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="L41" s="29">
+        <v>0</v>
+      </c>
+      <c r="M41" s="29">
+        <v>0</v>
+      </c>
+      <c r="N41" s="29">
+        <v>0</v>
+      </c>
+      <c r="O41" s="29">
+        <v>0</v>
+      </c>
+      <c r="P41" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="R41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="S41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C42" s="20" t="str">
+        <f t="shared" ref="C42" si="1">C41</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L42" s="9">
+        <v>0</v>
+      </c>
+      <c r="M42" s="9">
+        <v>0</v>
+      </c>
+      <c r="N42" s="9">
+        <v>0</v>
+      </c>
+      <c r="O42" s="9">
+        <v>0</v>
+      </c>
+      <c r="P42" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S42" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C43" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L38" s="9">
-        <v>0</v>
-      </c>
-      <c r="M38" s="9">
-        <v>0</v>
-      </c>
-      <c r="N38" s="9">
-        <v>0</v>
-      </c>
-      <c r="O38" s="9">
-        <v>0</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="T38" s="10"/>
-      <c r="U38" s="1"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C39" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="24">
+      <c r="E43" s="23">
+        <v>0</v>
+      </c>
+      <c r="F43" s="24">
         <v>1</v>
       </c>
-      <c r="G39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I39" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="L39" s="32">
+      <c r="G43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L43" s="26">
         <v>0.7</v>
       </c>
-      <c r="M39" s="27">
-        <v>0</v>
-      </c>
-      <c r="N39" s="27">
-        <v>0</v>
-      </c>
-      <c r="O39" s="27">
-        <v>0</v>
-      </c>
-      <c r="P39" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T39" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U39" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="V39" s="22"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C40" s="20" t="str">
-        <f>C39</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D40" s="20" t="str">
-        <f>D39</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="15">
-        <v>16</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="K40" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L40" s="33">
-        <v>0.7</v>
-      </c>
-      <c r="M40" s="33">
-        <v>1</v>
-      </c>
-      <c r="N40" s="9">
-        <v>0</v>
-      </c>
-      <c r="O40" s="9">
-        <v>0</v>
-      </c>
-      <c r="P40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S40" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C41" s="20" t="str">
-        <f>C40</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D41" s="20" t="str">
-        <f>D40</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K41" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L41" s="9">
-        <v>0</v>
-      </c>
-      <c r="M41" s="9">
-        <v>0</v>
-      </c>
-      <c r="N41" s="9">
-        <v>0</v>
-      </c>
-      <c r="O41" s="9">
-        <v>0</v>
-      </c>
-      <c r="P41" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S41" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C42" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="24">
-        <v>1</v>
-      </c>
-      <c r="G42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I42" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J42" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="L42" s="27">
-        <v>0</v>
-      </c>
-      <c r="M42" s="27">
-        <v>0</v>
-      </c>
-      <c r="N42" s="27">
-        <v>0</v>
-      </c>
-      <c r="O42" s="27">
-        <v>0</v>
-      </c>
-      <c r="P42" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T42" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U42" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="V42" s="22"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C43" s="20" t="str">
-        <f t="shared" ref="C43" si="0">C42</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="15">
-        <v>16</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L43" s="9">
-        <v>0</v>
-      </c>
-      <c r="M43" s="9">
-        <v>0</v>
-      </c>
-      <c r="N43" s="9">
-        <v>0</v>
-      </c>
-      <c r="O43" s="9">
-        <v>0</v>
-      </c>
-      <c r="P43" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S43" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C44" s="20" t="str">
-        <f t="shared" ref="C44" si="1">C43</f>
-        <v>2025 Final</v>
+      <c r="M43" s="27">
+        <v>0</v>
+      </c>
+      <c r="N43" s="27">
+        <v>0</v>
+      </c>
+      <c r="O43" s="27">
+        <v>0</v>
+      </c>
+      <c r="P43" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T43" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U43" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="V43" s="22"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C44" s="20" t="s">
+        <v>56</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="E44" s="9">
+        <v>0</v>
+      </c>
+      <c r="F44" s="15">
+        <f>F43+1</f>
+        <v>2</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>30</v>
@@ -1631,13 +1669,13 @@
         <v>30</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="L44" s="9">
         <v>0</v>
@@ -1664,67 +1702,61 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C45" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="22" t="s">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C45" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="23">
-        <v>0</v>
-      </c>
-      <c r="F45" s="24">
-        <v>1</v>
-      </c>
-      <c r="G45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="J45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="K45" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="L45" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M45" s="27">
-        <v>0</v>
-      </c>
-      <c r="N45" s="27">
-        <v>0</v>
-      </c>
-      <c r="O45" s="27">
-        <v>0</v>
-      </c>
-      <c r="P45" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T45" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U45" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="V45" s="22"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E45" s="9">
+        <v>0</v>
+      </c>
+      <c r="F45" s="15">
+        <f t="shared" ref="F45:F58" si="2">F44+1</f>
+        <v>3</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L45" s="9">
+        <v>0</v>
+      </c>
+      <c r="M45" s="9">
+        <v>0</v>
+      </c>
+      <c r="N45" s="9">
+        <v>0</v>
+      </c>
+      <c r="O45" s="9">
+        <v>0</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S45" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C46" s="20" t="s">
         <v>56</v>
       </c>
@@ -1735,8 +1767,8 @@
         <v>0</v>
       </c>
       <c r="F46" s="15">
-        <f>F45+1</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>30</v>
@@ -1745,13 +1777,13 @@
         <v>30</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L46" s="9">
         <v>0</v>
@@ -1778,7 +1810,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C47" s="20" t="s">
         <v>56</v>
       </c>
@@ -1789,8 +1821,8 @@
         <v>0</v>
       </c>
       <c r="F47" s="15">
-        <f t="shared" ref="F47:F60" si="2">F46+1</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>30</v>
@@ -1799,13 +1831,13 @@
         <v>30</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L47" s="9">
         <v>0</v>
@@ -1832,7 +1864,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C48" s="20" t="s">
         <v>56</v>
       </c>
@@ -1844,7 +1876,7 @@
       </c>
       <c r="F48" s="15">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>30</v>
@@ -1853,13 +1885,13 @@
         <v>30</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L48" s="9">
         <v>0</v>
@@ -1898,7 +1930,7 @@
       </c>
       <c r="F49" s="15">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>30</v>
@@ -1952,7 +1984,7 @@
       </c>
       <c r="F50" s="15">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G50" s="10" t="s">
         <v>30</v>
@@ -2006,7 +2038,7 @@
       </c>
       <c r="F51" s="15">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G51" s="10" t="s">
         <v>30</v>
@@ -2060,7 +2092,7 @@
       </c>
       <c r="F52" s="15">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G52" s="10" t="s">
         <v>30</v>
@@ -2114,7 +2146,7 @@
       </c>
       <c r="F53" s="15">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G53" s="10" t="s">
         <v>30</v>
@@ -2168,7 +2200,7 @@
       </c>
       <c r="F54" s="15">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>30</v>
@@ -2222,7 +2254,7 @@
       </c>
       <c r="F55" s="15">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G55" s="10" t="s">
         <v>30</v>
@@ -2231,13 +2263,13 @@
         <v>30</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L55" s="9">
         <v>0</v>
@@ -2276,7 +2308,7 @@
       </c>
       <c r="F56" s="15">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>30</v>
@@ -2285,13 +2317,13 @@
         <v>30</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L56" s="9">
         <v>0</v>
@@ -2330,7 +2362,7 @@
       </c>
       <c r="F57" s="15">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>30</v>
@@ -2339,13 +2371,13 @@
         <v>30</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L57" s="9">
         <v>0</v>
@@ -2373,72 +2405,74 @@
       </c>
     </row>
     <row r="58" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C58" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D58" s="20" t="s">
+      <c r="C58" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="9">
-        <v>0</v>
-      </c>
-      <c r="F58" s="15">
+      <c r="E58" s="12">
+        <v>0</v>
+      </c>
+      <c r="F58" s="16">
         <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L58" s="9">
-        <v>0</v>
-      </c>
-      <c r="M58" s="9">
-        <v>0</v>
-      </c>
-      <c r="N58" s="9">
-        <v>0</v>
-      </c>
-      <c r="O58" s="9">
-        <v>0</v>
-      </c>
-      <c r="P58" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S58" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L58" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M58" s="8">
+        <v>1</v>
+      </c>
+      <c r="N58" s="12">
+        <v>0</v>
+      </c>
+      <c r="O58" s="12">
+        <v>0</v>
+      </c>
+      <c r="P58" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
     </row>
     <row r="59" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C59" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D59" s="20" t="s">
+      <c r="C59" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" t="s">
         <v>36</v>
       </c>
-      <c r="E59" s="9">
-        <v>0</v>
+      <c r="E59" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F59" s="15">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G59" s="10" t="s">
         <v>30</v>
@@ -2455,8 +2489,8 @@
       <c r="K59" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L59" s="9">
-        <v>0</v>
+      <c r="L59" s="7">
+        <v>0.7</v>
       </c>
       <c r="M59" s="9">
         <v>0</v>
@@ -2479,76 +2513,80 @@
       <c r="S59" s="9">
         <v>-1</v>
       </c>
+      <c r="T59" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U59" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="60" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C60" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D60" s="21" t="s">
+      <c r="C60" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="12">
-        <v>0</v>
-      </c>
-      <c r="F60" s="16">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L60" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M60" s="8">
-        <v>1</v>
-      </c>
-      <c r="N60" s="12">
-        <v>0</v>
-      </c>
-      <c r="O60" s="12">
-        <v>0</v>
-      </c>
-      <c r="P60" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
+      <c r="E60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="15">
+        <f>F59+1</f>
+        <v>2</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L60" s="9">
+        <v>0</v>
+      </c>
+      <c r="M60" s="9">
+        <v>0</v>
+      </c>
+      <c r="N60" s="9">
+        <v>0</v>
+      </c>
+      <c r="O60" s="9">
+        <v>0</v>
+      </c>
+      <c r="P60" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S60" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="61" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>56</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="C61" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F61" s="15">
-        <v>1</v>
+        <f t="shared" ref="F61:F74" si="3">F60+1</f>
+        <v>3</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>30</v>
@@ -2565,8 +2603,8 @@
       <c r="K61" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L61" s="7">
-        <v>0.7</v>
+      <c r="L61" s="9">
+        <v>0</v>
       </c>
       <c r="M61" s="9">
         <v>0</v>
@@ -2588,12 +2626,6 @@
       </c>
       <c r="S61" s="9">
         <v>-1</v>
-      </c>
-      <c r="T61" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U61" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="62" spans="3:22" x14ac:dyDescent="0.25">
@@ -2607,8 +2639,8 @@
         <v>9</v>
       </c>
       <c r="F62" s="15">
-        <f>F61+1</f>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>30</v>
@@ -2661,8 +2693,8 @@
         <v>9</v>
       </c>
       <c r="F63" s="15">
-        <f t="shared" ref="F63:F76" si="3">F62+1</f>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>30</v>
@@ -2716,7 +2748,7 @@
       </c>
       <c r="F64" s="15">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G64" s="10" t="s">
         <v>30</v>
@@ -2770,7 +2802,7 @@
       </c>
       <c r="F65" s="15">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>30</v>
@@ -2824,7 +2856,7 @@
       </c>
       <c r="F66" s="15">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G66" s="10" t="s">
         <v>30</v>
@@ -2878,7 +2910,7 @@
       </c>
       <c r="F67" s="15">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G67" s="10" t="s">
         <v>30</v>
@@ -2932,7 +2964,7 @@
       </c>
       <c r="F68" s="15">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G68" s="10" t="s">
         <v>30</v>
@@ -2986,7 +3018,7 @@
       </c>
       <c r="F69" s="15">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G69" s="10" t="s">
         <v>30</v>
@@ -3040,7 +3072,7 @@
       </c>
       <c r="F70" s="15">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G70" s="10" t="s">
         <v>30</v>
@@ -3094,7 +3126,7 @@
       </c>
       <c r="F71" s="15">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G71" s="10" t="s">
         <v>30</v>
@@ -3148,7 +3180,7 @@
       </c>
       <c r="F72" s="15">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G72" s="10" t="s">
         <v>30</v>
@@ -3202,7 +3234,7 @@
       </c>
       <c r="F73" s="15">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G73" s="10" t="s">
         <v>30</v>
@@ -3245,72 +3277,74 @@
       </c>
     </row>
     <row r="74" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C74" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D74" s="20" t="s">
+      <c r="C74" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E74" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="15">
+      <c r="E74" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="16">
         <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="G74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L74" s="9">
-        <v>0</v>
-      </c>
-      <c r="M74" s="9">
-        <v>0</v>
-      </c>
-      <c r="N74" s="9">
-        <v>0</v>
-      </c>
-      <c r="O74" s="9">
-        <v>0</v>
-      </c>
-      <c r="P74" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S74" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L74" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M74" s="8">
+        <v>1</v>
+      </c>
+      <c r="N74" s="12">
+        <v>0</v>
+      </c>
+      <c r="O74" s="12">
+        <v>0</v>
+      </c>
+      <c r="P74" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+      <c r="V74" s="3"/>
     </row>
     <row r="75" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C75" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E75" s="9" t="s">
+      <c r="C75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="15">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G75" s="10" t="s">
         <v>30</v>
@@ -3319,13 +3353,13 @@
         <v>30</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="K75" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="L75" s="9">
         <v>0</v>
@@ -3351,76 +3385,80 @@
       <c r="S75" s="9">
         <v>-1</v>
       </c>
+      <c r="T75" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U75" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="76" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C76" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D76" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="16">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K76" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L76" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M76" s="8">
-        <v>1</v>
-      </c>
-      <c r="N76" s="12">
-        <v>0</v>
-      </c>
-      <c r="O76" s="12">
-        <v>0</v>
-      </c>
-      <c r="P76" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T76" s="3"/>
-      <c r="U76" s="3"/>
-      <c r="V76" s="3"/>
+      <c r="C76" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="15">
+        <f>F75+1</f>
+        <v>2</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L76" s="9">
+        <v>0</v>
+      </c>
+      <c r="M76" s="9">
+        <v>0</v>
+      </c>
+      <c r="N76" s="9">
+        <v>0</v>
+      </c>
+      <c r="O76" s="9">
+        <v>0</v>
+      </c>
+      <c r="P76" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S76" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="77" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>56</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="2" t="s">
+      <c r="C77" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="15">
-        <v>1</v>
+        <f t="shared" ref="F77:F90" si="4">F76+1</f>
+        <v>3</v>
       </c>
       <c r="G77" s="10" t="s">
         <v>30</v>
@@ -3460,12 +3498,6 @@
       </c>
       <c r="S77" s="9">
         <v>-1</v>
-      </c>
-      <c r="T77" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U77" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="78" spans="3:22" x14ac:dyDescent="0.25">
@@ -3479,8 +3511,8 @@
         <v>9</v>
       </c>
       <c r="F78" s="15">
-        <f>F77+1</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="G78" s="10" t="s">
         <v>30</v>
@@ -3509,11 +3541,11 @@
       <c r="O78" s="9">
         <v>0</v>
       </c>
-      <c r="P78" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q78" s="9">
-        <v>-1</v>
+      <c r="P78" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q78" s="19">
+        <v>0.4</v>
       </c>
       <c r="R78" s="9">
         <v>-1</v>
@@ -3533,8 +3565,8 @@
         <v>9</v>
       </c>
       <c r="F79" s="15">
-        <f t="shared" ref="F79:F92" si="4">F78+1</f>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="G79" s="10" t="s">
         <v>30</v>
@@ -3563,11 +3595,11 @@
       <c r="O79" s="9">
         <v>0</v>
       </c>
-      <c r="P79" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q79" s="9">
-        <v>-1</v>
+      <c r="P79" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q79" s="19">
+        <v>0.4</v>
       </c>
       <c r="R79" s="9">
         <v>-1</v>
@@ -3588,7 +3620,7 @@
       </c>
       <c r="F80" s="15">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G80" s="10" t="s">
         <v>30</v>
@@ -3642,7 +3674,7 @@
       </c>
       <c r="F81" s="15">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G81" s="10" t="s">
         <v>30</v>
@@ -3696,7 +3728,7 @@
       </c>
       <c r="F82" s="15">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G82" s="10" t="s">
         <v>30</v>
@@ -3750,7 +3782,7 @@
       </c>
       <c r="F83" s="15">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G83" s="10" t="s">
         <v>30</v>
@@ -3804,7 +3836,7 @@
       </c>
       <c r="F84" s="15">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G84" s="10" t="s">
         <v>30</v>
@@ -3858,7 +3890,7 @@
       </c>
       <c r="F85" s="15">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G85" s="10" t="s">
         <v>30</v>
@@ -3887,11 +3919,11 @@
       <c r="O85" s="9">
         <v>0</v>
       </c>
-      <c r="P85" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q85" s="19">
-        <v>0.4</v>
+      <c r="P85" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q85" s="9">
+        <v>-1</v>
       </c>
       <c r="R85" s="9">
         <v>-1</v>
@@ -3912,7 +3944,7 @@
       </c>
       <c r="F86" s="15">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G86" s="10" t="s">
         <v>30</v>
@@ -3941,11 +3973,11 @@
       <c r="O86" s="9">
         <v>0</v>
       </c>
-      <c r="P86" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q86" s="19">
-        <v>0.4</v>
+      <c r="P86" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q86" s="9">
+        <v>-1</v>
       </c>
       <c r="R86" s="9">
         <v>-1</v>
@@ -3966,7 +3998,7 @@
       </c>
       <c r="F87" s="15">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G87" s="10" t="s">
         <v>30</v>
@@ -4020,7 +4052,7 @@
       </c>
       <c r="F88" s="15">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G88" s="10" t="s">
         <v>30</v>
@@ -4049,17 +4081,17 @@
       <c r="O88" s="9">
         <v>0</v>
       </c>
-      <c r="P88" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S88" s="9">
-        <v>-1</v>
+      <c r="P88" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q88" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R88" s="19">
+        <v>67</v>
+      </c>
+      <c r="S88" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="2:22" x14ac:dyDescent="0.25">
@@ -4074,7 +4106,7 @@
       </c>
       <c r="F89" s="15">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G89" s="10" t="s">
         <v>30</v>
@@ -4103,245 +4135,137 @@
       <c r="O89" s="9">
         <v>0</v>
       </c>
-      <c r="P89" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S89" s="9">
-        <v>-1</v>
+      <c r="P89" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q89" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R89" s="19">
+        <v>67</v>
+      </c>
+      <c r="S89" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="21" t="s">
         <v>56</v>
       </c>
       <c r="D90" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E90" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F90" s="15">
+      <c r="E90" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="16">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="G90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L90" s="9">
-        <v>0</v>
-      </c>
-      <c r="M90" s="9">
-        <v>0</v>
-      </c>
-      <c r="N90" s="9">
-        <v>0</v>
-      </c>
-      <c r="O90" s="9">
-        <v>0</v>
-      </c>
-      <c r="P90" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q90" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R90" s="19">
-        <v>67</v>
-      </c>
-      <c r="S90" s="19">
-        <v>72</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L90" s="12">
+        <v>0</v>
+      </c>
+      <c r="M90" s="12">
+        <v>0</v>
+      </c>
+      <c r="N90" s="12">
+        <v>0</v>
+      </c>
+      <c r="O90" s="12">
+        <v>0</v>
+      </c>
+      <c r="P90" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
     </row>
     <row r="91" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C91" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D91" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F91" s="15">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="G91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L91" s="9">
-        <v>0</v>
-      </c>
-      <c r="M91" s="9">
-        <v>0</v>
-      </c>
-      <c r="N91" s="9">
-        <v>0</v>
-      </c>
-      <c r="O91" s="9">
-        <v>0</v>
-      </c>
-      <c r="P91" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q91" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R91" s="19">
-        <v>67</v>
-      </c>
-      <c r="S91" s="19">
-        <v>72</v>
+      <c r="C91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L91" s="13">
+        <v>0</v>
+      </c>
+      <c r="M91" s="13">
+        <v>0</v>
+      </c>
+      <c r="N91" s="13">
+        <v>0</v>
+      </c>
+      <c r="O91" s="13">
+        <v>0</v>
+      </c>
+      <c r="P91" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="R91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="S91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="T91" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U91" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C92" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D92" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F92" s="16">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="G92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L92" s="12">
-        <v>0</v>
-      </c>
-      <c r="M92" s="12">
-        <v>0</v>
-      </c>
-      <c r="N92" s="12">
-        <v>0</v>
-      </c>
-      <c r="O92" s="12">
-        <v>0</v>
-      </c>
-      <c r="P92" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T92" s="3"/>
-      <c r="U92" s="3"/>
-      <c r="V92" s="3"/>
-    </row>
-    <row r="93" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F93" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="L93" s="13">
-        <v>0</v>
-      </c>
-      <c r="M93" s="13">
-        <v>0</v>
-      </c>
-      <c r="N93" s="13">
-        <v>0</v>
-      </c>
-      <c r="O93" s="13">
-        <v>0</v>
-      </c>
-      <c r="P93" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="R93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="S93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="T93" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U93" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="94" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+      <c r="B92" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2025-CBECC-Res-Schema Issues - 14: Corrected PV+Bat output values. Added Compliance Margin values output for missing rows. - 61: Added XML output for Section_Y (HVAC - HEAT PUMPS) Y14a_IsVSD - 62: Added XML output for Section_Y (HVAC - HEAT PUMPS) Y06b_HeatPumpBackupFuel
</commit_message>
<xml_diff>
--- a/Documentation/T24Res/T24RCustomStdDesign.xlsx
+++ b/Documentation/T24Res/T24RCustomStdDesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\git-vscode\CBECC-Dev\Documentation\T24Res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CBECC\SVN\branches\CBECC-Com_MFamRestructure\Documentation\T24Res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDE9C57-C7E1-4939-B768-B6C30AC952B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71481180-D713-48D8-97D8-A5E088BA1223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="2580" windowWidth="26790" windowHeight="14340" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
+    <workbookView xWindow="24549" yWindow="2571" windowWidth="22868" windowHeight="14615" xr2:uid="{07D8E957-2C9A-4D7E-8925-FE375302CA45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="67">
   <si>
     <t>;</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>default  -or-  Electricity  -or-  Gas</t>
-  </si>
-  <si>
-    <t>09/18/25 - SAC - modified '2025 Final' LowRiseRes records for DHW, CompactDHW &amp; DrnWtrHtRec data</t>
   </si>
 </sst>
 </file>
@@ -289,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,12 +296,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -438,19 +429,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -767,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C373ABC9-0F2E-48ED-B208-F0F9FC7924F4}">
-  <dimension ref="A1:V94"/>
+  <dimension ref="A1:V92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,8 +767,7 @@
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="9" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.5703125" customWidth="1"/>
@@ -829,7 +814,7 @@
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -837,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -845,7 +830,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -853,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -861,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -869,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -877,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,7 +870,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -901,28 +886,31 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" t="s">
-        <v>15</v>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -930,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -941,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -952,10 +940,10 @@
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -963,10 +951,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -974,37 +962,37 @@
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>19</v>
+      <c r="E22" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>27</v>
+      <c r="E23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E24" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1012,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1023,10 +1011,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,10 +1022,10 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1045,10 +1033,10 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" t="s">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1056,10 +1044,10 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1067,128 +1055,177 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="5" t="s">
+    <row r="34" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F34" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H34" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J34" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K34" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="L35" s="8" t="s">
+      <c r="L34" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="M34" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N35" s="8" t="s">
+      <c r="N34" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O35" s="8" t="s">
+      <c r="O34" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P35" s="8" t="s">
+      <c r="P34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Q35" s="8" t="s">
+      <c r="Q34" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="R35" s="8" t="s">
+      <c r="R34" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="S35" s="8" t="s">
+      <c r="S34" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="T35" s="5"/>
-      <c r="U35" s="5"/>
-      <c r="V35" s="5"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>57</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D35" t="s">
         <v>36</v>
       </c>
+      <c r="E35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="15">
+        <v>1</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L35" s="26">
+        <v>0.7</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0</v>
+      </c>
+      <c r="N35" s="9">
+        <v>0</v>
+      </c>
+      <c r="O35" s="9">
+        <v>0</v>
+      </c>
+      <c r="P35" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S35" s="9">
+        <v>-1</v>
+      </c>
+      <c r="T35" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C36" s="20" t="str">
+        <f>C35</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="E36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F36" s="15">
+        <v>16</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="M36" s="7">
         <v>1</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L36" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M36" s="9">
-        <v>0</v>
-      </c>
       <c r="N36" s="9">
         <v>0</v>
       </c>
@@ -1207,14 +1244,10 @@
       <c r="S36" s="9">
         <v>-1</v>
       </c>
-      <c r="T36" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T36" s="10"/>
+      <c r="U36" s="1"/>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C37" s="20" t="str">
         <f>C36</f>
         <v>2025 Final</v>
@@ -1225,8 +1258,8 @@
       <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="15">
-        <v>16</v>
+      <c r="F37" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>30</v>
@@ -1243,11 +1276,11 @@
       <c r="K37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L37" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="M37" s="7">
-        <v>1</v>
+      <c r="L37" s="9">
+        <v>0</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0</v>
       </c>
       <c r="N37" s="9">
         <v>0</v>
@@ -1270,359 +1303,364 @@
       <c r="T37" s="10"/>
       <c r="U37" s="1"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C38" s="20" t="str">
-        <f>C37</f>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C38" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="24">
+        <v>16</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L38" s="27">
+        <v>0</v>
+      </c>
+      <c r="M38" s="27">
+        <v>0</v>
+      </c>
+      <c r="N38" s="27">
+        <v>0</v>
+      </c>
+      <c r="O38" s="27">
+        <v>0</v>
+      </c>
+      <c r="P38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T38" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U38" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="V38" s="22"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C39" s="20" t="str">
+        <f>C38</f>
         <v>2025 Final</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D39" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L39" s="9">
+        <v>0</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0</v>
+      </c>
+      <c r="N39" s="9">
+        <v>0</v>
+      </c>
+      <c r="O39" s="9">
+        <v>0</v>
+      </c>
+      <c r="P39" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R39" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S39" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C40" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="24">
+        <v>1</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" s="27">
+        <v>0</v>
+      </c>
+      <c r="M40" s="27">
+        <v>0</v>
+      </c>
+      <c r="N40" s="27">
+        <v>0</v>
+      </c>
+      <c r="O40" s="27">
+        <v>0</v>
+      </c>
+      <c r="P40" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S40" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T40" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U40" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="V40" s="22"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C41" s="20" t="str">
+        <f t="shared" ref="C41" si="0">C40</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="15">
+        <v>16</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="L41" s="29">
+        <v>0</v>
+      </c>
+      <c r="M41" s="29">
+        <v>0</v>
+      </c>
+      <c r="N41" s="29">
+        <v>0</v>
+      </c>
+      <c r="O41" s="29">
+        <v>0</v>
+      </c>
+      <c r="P41" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="R41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="S41" s="29">
+        <v>-1</v>
+      </c>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C42" s="20" t="str">
+        <f t="shared" ref="C42" si="1">C41</f>
+        <v>2025 Final</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L42" s="9">
+        <v>0</v>
+      </c>
+      <c r="M42" s="9">
+        <v>0</v>
+      </c>
+      <c r="N42" s="9">
+        <v>0</v>
+      </c>
+      <c r="O42" s="9">
+        <v>0</v>
+      </c>
+      <c r="P42" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R42" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S42" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C43" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L38" s="9">
-        <v>0</v>
-      </c>
-      <c r="M38" s="9">
-        <v>0</v>
-      </c>
-      <c r="N38" s="9">
-        <v>0</v>
-      </c>
-      <c r="O38" s="9">
-        <v>0</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S38" s="9">
-        <v>-1</v>
-      </c>
-      <c r="T38" s="10"/>
-      <c r="U38" s="1"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C39" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="24">
+      <c r="E43" s="23">
+        <v>0</v>
+      </c>
+      <c r="F43" s="24">
         <v>1</v>
       </c>
-      <c r="G39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I39" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="L39" s="32">
+      <c r="G43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L43" s="26">
         <v>0.7</v>
       </c>
-      <c r="M39" s="27">
-        <v>0</v>
-      </c>
-      <c r="N39" s="27">
-        <v>0</v>
-      </c>
-      <c r="O39" s="27">
-        <v>0</v>
-      </c>
-      <c r="P39" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T39" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U39" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="V39" s="22"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C40" s="20" t="str">
-        <f>C39</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D40" s="20" t="str">
-        <f>D39</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="15">
-        <v>16</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="K40" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L40" s="33">
-        <v>0.7</v>
-      </c>
-      <c r="M40" s="33">
-        <v>1</v>
-      </c>
-      <c r="N40" s="9">
-        <v>0</v>
-      </c>
-      <c r="O40" s="9">
-        <v>0</v>
-      </c>
-      <c r="P40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R40" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S40" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C41" s="20" t="str">
-        <f>C40</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D41" s="20" t="str">
-        <f>D40</f>
-        <v>LowRiseRes</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K41" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="L41" s="9">
-        <v>0</v>
-      </c>
-      <c r="M41" s="9">
-        <v>0</v>
-      </c>
-      <c r="N41" s="9">
-        <v>0</v>
-      </c>
-      <c r="O41" s="9">
-        <v>0</v>
-      </c>
-      <c r="P41" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S41" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C42" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="24">
-        <v>1</v>
-      </c>
-      <c r="G42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I42" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J42" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="K42" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="L42" s="27">
-        <v>0</v>
-      </c>
-      <c r="M42" s="27">
-        <v>0</v>
-      </c>
-      <c r="N42" s="27">
-        <v>0</v>
-      </c>
-      <c r="O42" s="27">
-        <v>0</v>
-      </c>
-      <c r="P42" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S42" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T42" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U42" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="V42" s="22"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C43" s="20" t="str">
-        <f t="shared" ref="C43" si="0">C42</f>
-        <v>2025 Final</v>
-      </c>
-      <c r="D43" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="15">
-        <v>16</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K43" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L43" s="9">
-        <v>0</v>
-      </c>
-      <c r="M43" s="9">
-        <v>0</v>
-      </c>
-      <c r="N43" s="9">
-        <v>0</v>
-      </c>
-      <c r="O43" s="9">
-        <v>0</v>
-      </c>
-      <c r="P43" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R43" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S43" s="9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C44" s="20" t="str">
-        <f t="shared" ref="C44" si="1">C43</f>
-        <v>2025 Final</v>
+      <c r="M43" s="27">
+        <v>0</v>
+      </c>
+      <c r="N43" s="27">
+        <v>0</v>
+      </c>
+      <c r="O43" s="27">
+        <v>0</v>
+      </c>
+      <c r="P43" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="R43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="S43" s="27">
+        <v>-1</v>
+      </c>
+      <c r="T43" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U43" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="V43" s="22"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C44" s="20" t="s">
+        <v>56</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="E44" s="9">
+        <v>0</v>
+      </c>
+      <c r="F44" s="15">
+        <f>F43+1</f>
+        <v>2</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>30</v>
@@ -1631,13 +1669,13 @@
         <v>30</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="L44" s="9">
         <v>0</v>
@@ -1664,67 +1702,61 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C45" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="22" t="s">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C45" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="23">
-        <v>0</v>
-      </c>
-      <c r="F45" s="24">
-        <v>1</v>
-      </c>
-      <c r="G45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H45" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="J45" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="K45" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="L45" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="M45" s="27">
-        <v>0</v>
-      </c>
-      <c r="N45" s="27">
-        <v>0</v>
-      </c>
-      <c r="O45" s="27">
-        <v>0</v>
-      </c>
-      <c r="P45" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="R45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="S45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="T45" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="U45" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="V45" s="22"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E45" s="9">
+        <v>0</v>
+      </c>
+      <c r="F45" s="15">
+        <f t="shared" ref="F45:F58" si="2">F44+1</f>
+        <v>3</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L45" s="9">
+        <v>0</v>
+      </c>
+      <c r="M45" s="9">
+        <v>0</v>
+      </c>
+      <c r="N45" s="9">
+        <v>0</v>
+      </c>
+      <c r="O45" s="9">
+        <v>0</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S45" s="9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C46" s="20" t="s">
         <v>56</v>
       </c>
@@ -1735,8 +1767,8 @@
         <v>0</v>
       </c>
       <c r="F46" s="15">
-        <f>F45+1</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>30</v>
@@ -1745,13 +1777,13 @@
         <v>30</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L46" s="9">
         <v>0</v>
@@ -1778,7 +1810,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C47" s="20" t="s">
         <v>56</v>
       </c>
@@ -1789,8 +1821,8 @@
         <v>0</v>
       </c>
       <c r="F47" s="15">
-        <f t="shared" ref="F47:F60" si="2">F46+1</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>30</v>
@@ -1799,13 +1831,13 @@
         <v>30</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L47" s="9">
         <v>0</v>
@@ -1832,7 +1864,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C48" s="20" t="s">
         <v>56</v>
       </c>
@@ -1844,7 +1876,7 @@
       </c>
       <c r="F48" s="15">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>30</v>
@@ -1853,13 +1885,13 @@
         <v>30</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L48" s="9">
         <v>0</v>
@@ -1898,7 +1930,7 @@
       </c>
       <c r="F49" s="15">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G49" s="10" t="s">
         <v>30</v>
@@ -1952,7 +1984,7 @@
       </c>
       <c r="F50" s="15">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G50" s="10" t="s">
         <v>30</v>
@@ -2006,7 +2038,7 @@
       </c>
       <c r="F51" s="15">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G51" s="10" t="s">
         <v>30</v>
@@ -2060,7 +2092,7 @@
       </c>
       <c r="F52" s="15">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G52" s="10" t="s">
         <v>30</v>
@@ -2114,7 +2146,7 @@
       </c>
       <c r="F53" s="15">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G53" s="10" t="s">
         <v>30</v>
@@ -2168,7 +2200,7 @@
       </c>
       <c r="F54" s="15">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>30</v>
@@ -2222,7 +2254,7 @@
       </c>
       <c r="F55" s="15">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G55" s="10" t="s">
         <v>30</v>
@@ -2231,13 +2263,13 @@
         <v>30</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L55" s="9">
         <v>0</v>
@@ -2276,7 +2308,7 @@
       </c>
       <c r="F56" s="15">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>30</v>
@@ -2285,13 +2317,13 @@
         <v>30</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L56" s="9">
         <v>0</v>
@@ -2330,7 +2362,7 @@
       </c>
       <c r="F57" s="15">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G57" s="10" t="s">
         <v>30</v>
@@ -2339,13 +2371,13 @@
         <v>30</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L57" s="9">
         <v>0</v>
@@ -2373,72 +2405,74 @@
       </c>
     </row>
     <row r="58" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C58" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D58" s="20" t="s">
+      <c r="C58" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="9">
-        <v>0</v>
-      </c>
-      <c r="F58" s="15">
+      <c r="E58" s="12">
+        <v>0</v>
+      </c>
+      <c r="F58" s="16">
         <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L58" s="9">
-        <v>0</v>
-      </c>
-      <c r="M58" s="9">
-        <v>0</v>
-      </c>
-      <c r="N58" s="9">
-        <v>0</v>
-      </c>
-      <c r="O58" s="9">
-        <v>0</v>
-      </c>
-      <c r="P58" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R58" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S58" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L58" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M58" s="8">
+        <v>1</v>
+      </c>
+      <c r="N58" s="12">
+        <v>0</v>
+      </c>
+      <c r="O58" s="12">
+        <v>0</v>
+      </c>
+      <c r="P58" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S58" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
     </row>
     <row r="59" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C59" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D59" s="20" t="s">
+      <c r="C59" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" t="s">
         <v>36</v>
       </c>
-      <c r="E59" s="9">
-        <v>0</v>
+      <c r="E59" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="F59" s="15">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G59" s="10" t="s">
         <v>30</v>
@@ -2455,8 +2489,8 @@
       <c r="K59" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L59" s="9">
-        <v>0</v>
+      <c r="L59" s="7">
+        <v>0.7</v>
       </c>
       <c r="M59" s="9">
         <v>0</v>
@@ -2479,76 +2513,80 @@
       <c r="S59" s="9">
         <v>-1</v>
       </c>
+      <c r="T59" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U59" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="60" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C60" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D60" s="21" t="s">
+      <c r="C60" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="12">
-        <v>0</v>
-      </c>
-      <c r="F60" s="16">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L60" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M60" s="8">
-        <v>1</v>
-      </c>
-      <c r="N60" s="12">
-        <v>0</v>
-      </c>
-      <c r="O60" s="12">
-        <v>0</v>
-      </c>
-      <c r="P60" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S60" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
+      <c r="E60" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="15">
+        <f>F59+1</f>
+        <v>2</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L60" s="9">
+        <v>0</v>
+      </c>
+      <c r="M60" s="9">
+        <v>0</v>
+      </c>
+      <c r="N60" s="9">
+        <v>0</v>
+      </c>
+      <c r="O60" s="9">
+        <v>0</v>
+      </c>
+      <c r="P60" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R60" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S60" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="61" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>56</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="C61" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F61" s="15">
-        <v>1</v>
+        <f t="shared" ref="F61:F74" si="3">F60+1</f>
+        <v>3</v>
       </c>
       <c r="G61" s="10" t="s">
         <v>30</v>
@@ -2565,8 +2603,8 @@
       <c r="K61" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L61" s="7">
-        <v>0.7</v>
+      <c r="L61" s="9">
+        <v>0</v>
       </c>
       <c r="M61" s="9">
         <v>0</v>
@@ -2588,12 +2626,6 @@
       </c>
       <c r="S61" s="9">
         <v>-1</v>
-      </c>
-      <c r="T61" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U61" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="62" spans="3:22" x14ac:dyDescent="0.25">
@@ -2607,8 +2639,8 @@
         <v>9</v>
       </c>
       <c r="F62" s="15">
-        <f>F61+1</f>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>30</v>
@@ -2661,8 +2693,8 @@
         <v>9</v>
       </c>
       <c r="F63" s="15">
-        <f t="shared" ref="F63:F76" si="3">F62+1</f>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>30</v>
@@ -2716,7 +2748,7 @@
       </c>
       <c r="F64" s="15">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G64" s="10" t="s">
         <v>30</v>
@@ -2770,7 +2802,7 @@
       </c>
       <c r="F65" s="15">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>30</v>
@@ -2824,7 +2856,7 @@
       </c>
       <c r="F66" s="15">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G66" s="10" t="s">
         <v>30</v>
@@ -2878,7 +2910,7 @@
       </c>
       <c r="F67" s="15">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G67" s="10" t="s">
         <v>30</v>
@@ -2932,7 +2964,7 @@
       </c>
       <c r="F68" s="15">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G68" s="10" t="s">
         <v>30</v>
@@ -2986,7 +3018,7 @@
       </c>
       <c r="F69" s="15">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G69" s="10" t="s">
         <v>30</v>
@@ -3040,7 +3072,7 @@
       </c>
       <c r="F70" s="15">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G70" s="10" t="s">
         <v>30</v>
@@ -3094,7 +3126,7 @@
       </c>
       <c r="F71" s="15">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G71" s="10" t="s">
         <v>30</v>
@@ -3148,7 +3180,7 @@
       </c>
       <c r="F72" s="15">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G72" s="10" t="s">
         <v>30</v>
@@ -3202,7 +3234,7 @@
       </c>
       <c r="F73" s="15">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G73" s="10" t="s">
         <v>30</v>
@@ -3245,72 +3277,74 @@
       </c>
     </row>
     <row r="74" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C74" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D74" s="20" t="s">
+      <c r="C74" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E74" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="15">
+      <c r="E74" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="16">
         <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="G74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H74" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L74" s="9">
-        <v>0</v>
-      </c>
-      <c r="M74" s="9">
-        <v>0</v>
-      </c>
-      <c r="N74" s="9">
-        <v>0</v>
-      </c>
-      <c r="O74" s="9">
-        <v>0</v>
-      </c>
-      <c r="P74" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R74" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S74" s="9">
-        <v>-1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L74" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="M74" s="8">
+        <v>1</v>
+      </c>
+      <c r="N74" s="12">
+        <v>0</v>
+      </c>
+      <c r="O74" s="12">
+        <v>0</v>
+      </c>
+      <c r="P74" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+      <c r="V74" s="3"/>
     </row>
     <row r="75" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C75" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E75" s="9" t="s">
+      <c r="C75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="15">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G75" s="10" t="s">
         <v>30</v>
@@ -3319,13 +3353,13 @@
         <v>30</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="K75" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="L75" s="9">
         <v>0</v>
@@ -3351,76 +3385,80 @@
       <c r="S75" s="9">
         <v>-1</v>
       </c>
+      <c r="T75" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U75" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="76" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C76" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D76" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="16">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H76" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K76" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L76" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="M76" s="8">
-        <v>1</v>
-      </c>
-      <c r="N76" s="12">
-        <v>0</v>
-      </c>
-      <c r="O76" s="12">
-        <v>0</v>
-      </c>
-      <c r="P76" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S76" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T76" s="3"/>
-      <c r="U76" s="3"/>
-      <c r="V76" s="3"/>
+      <c r="C76" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="15">
+        <f>F75+1</f>
+        <v>2</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K76" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L76" s="9">
+        <v>0</v>
+      </c>
+      <c r="M76" s="9">
+        <v>0</v>
+      </c>
+      <c r="N76" s="9">
+        <v>0</v>
+      </c>
+      <c r="O76" s="9">
+        <v>0</v>
+      </c>
+      <c r="P76" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="R76" s="9">
+        <v>-1</v>
+      </c>
+      <c r="S76" s="9">
+        <v>-1</v>
+      </c>
     </row>
     <row r="77" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>56</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="2" t="s">
+      <c r="C77" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="15">
-        <v>1</v>
+        <f t="shared" ref="F77:F90" si="4">F76+1</f>
+        <v>3</v>
       </c>
       <c r="G77" s="10" t="s">
         <v>30</v>
@@ -3460,12 +3498,6 @@
       </c>
       <c r="S77" s="9">
         <v>-1</v>
-      </c>
-      <c r="T77" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U77" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="78" spans="3:22" x14ac:dyDescent="0.25">
@@ -3479,8 +3511,8 @@
         <v>9</v>
       </c>
       <c r="F78" s="15">
-        <f>F77+1</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="G78" s="10" t="s">
         <v>30</v>
@@ -3509,11 +3541,11 @@
       <c r="O78" s="9">
         <v>0</v>
       </c>
-      <c r="P78" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q78" s="9">
-        <v>-1</v>
+      <c r="P78" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q78" s="19">
+        <v>0.4</v>
       </c>
       <c r="R78" s="9">
         <v>-1</v>
@@ -3533,8 +3565,8 @@
         <v>9</v>
       </c>
       <c r="F79" s="15">
-        <f t="shared" ref="F79:F92" si="4">F78+1</f>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="G79" s="10" t="s">
         <v>30</v>
@@ -3563,11 +3595,11 @@
       <c r="O79" s="9">
         <v>0</v>
       </c>
-      <c r="P79" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q79" s="9">
-        <v>-1</v>
+      <c r="P79" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q79" s="19">
+        <v>0.4</v>
       </c>
       <c r="R79" s="9">
         <v>-1</v>
@@ -3588,7 +3620,7 @@
       </c>
       <c r="F80" s="15">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G80" s="10" t="s">
         <v>30</v>
@@ -3642,7 +3674,7 @@
       </c>
       <c r="F81" s="15">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G81" s="10" t="s">
         <v>30</v>
@@ -3696,7 +3728,7 @@
       </c>
       <c r="F82" s="15">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G82" s="10" t="s">
         <v>30</v>
@@ -3750,7 +3782,7 @@
       </c>
       <c r="F83" s="15">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G83" s="10" t="s">
         <v>30</v>
@@ -3804,7 +3836,7 @@
       </c>
       <c r="F84" s="15">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G84" s="10" t="s">
         <v>30</v>
@@ -3858,7 +3890,7 @@
       </c>
       <c r="F85" s="15">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G85" s="10" t="s">
         <v>30</v>
@@ -3887,11 +3919,11 @@
       <c r="O85" s="9">
         <v>0</v>
       </c>
-      <c r="P85" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q85" s="19">
-        <v>0.4</v>
+      <c r="P85" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q85" s="9">
+        <v>-1</v>
       </c>
       <c r="R85" s="9">
         <v>-1</v>
@@ -3912,7 +3944,7 @@
       </c>
       <c r="F86" s="15">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G86" s="10" t="s">
         <v>30</v>
@@ -3941,11 +3973,11 @@
       <c r="O86" s="9">
         <v>0</v>
       </c>
-      <c r="P86" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q86" s="19">
-        <v>0.4</v>
+      <c r="P86" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q86" s="9">
+        <v>-1</v>
       </c>
       <c r="R86" s="9">
         <v>-1</v>
@@ -3966,7 +3998,7 @@
       </c>
       <c r="F87" s="15">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G87" s="10" t="s">
         <v>30</v>
@@ -4020,7 +4052,7 @@
       </c>
       <c r="F88" s="15">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G88" s="10" t="s">
         <v>30</v>
@@ -4049,17 +4081,17 @@
       <c r="O88" s="9">
         <v>0</v>
       </c>
-      <c r="P88" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R88" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S88" s="9">
-        <v>-1</v>
+      <c r="P88" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q88" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R88" s="19">
+        <v>67</v>
+      </c>
+      <c r="S88" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="2:22" x14ac:dyDescent="0.25">
@@ -4074,7 +4106,7 @@
       </c>
       <c r="F89" s="15">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G89" s="10" t="s">
         <v>30</v>
@@ -4103,245 +4135,137 @@
       <c r="O89" s="9">
         <v>0</v>
       </c>
-      <c r="P89" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="R89" s="9">
-        <v>-1</v>
-      </c>
-      <c r="S89" s="9">
-        <v>-1</v>
+      <c r="P89" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q89" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="R89" s="19">
+        <v>67</v>
+      </c>
+      <c r="S89" s="19">
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="21" t="s">
         <v>56</v>
       </c>
       <c r="D90" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E90" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F90" s="15">
+      <c r="E90" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="16">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="G90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K90" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L90" s="9">
-        <v>0</v>
-      </c>
-      <c r="M90" s="9">
-        <v>0</v>
-      </c>
-      <c r="N90" s="9">
-        <v>0</v>
-      </c>
-      <c r="O90" s="9">
-        <v>0</v>
-      </c>
-      <c r="P90" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q90" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R90" s="19">
-        <v>67</v>
-      </c>
-      <c r="S90" s="19">
-        <v>72</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K90" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L90" s="12">
+        <v>0</v>
+      </c>
+      <c r="M90" s="12">
+        <v>0</v>
+      </c>
+      <c r="N90" s="12">
+        <v>0</v>
+      </c>
+      <c r="O90" s="12">
+        <v>0</v>
+      </c>
+      <c r="P90" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="R90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="S90" s="12">
+        <v>-1</v>
+      </c>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
     </row>
     <row r="91" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C91" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D91" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F91" s="15">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="G91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K91" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L91" s="9">
-        <v>0</v>
-      </c>
-      <c r="M91" s="9">
-        <v>0</v>
-      </c>
-      <c r="N91" s="9">
-        <v>0</v>
-      </c>
-      <c r="O91" s="9">
-        <v>0</v>
-      </c>
-      <c r="P91" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q91" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="R91" s="19">
-        <v>67</v>
-      </c>
-      <c r="S91" s="19">
-        <v>72</v>
+      <c r="C91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K91" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L91" s="13">
+        <v>0</v>
+      </c>
+      <c r="M91" s="13">
+        <v>0</v>
+      </c>
+      <c r="N91" s="13">
+        <v>0</v>
+      </c>
+      <c r="O91" s="13">
+        <v>0</v>
+      </c>
+      <c r="P91" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="R91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="S91" s="13">
+        <v>-1</v>
+      </c>
+      <c r="T91" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U91" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C92" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D92" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F92" s="16">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="G92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K92" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L92" s="12">
-        <v>0</v>
-      </c>
-      <c r="M92" s="12">
-        <v>0</v>
-      </c>
-      <c r="N92" s="12">
-        <v>0</v>
-      </c>
-      <c r="O92" s="12">
-        <v>0</v>
-      </c>
-      <c r="P92" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="R92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="S92" s="12">
-        <v>-1</v>
-      </c>
-      <c r="T92" s="3"/>
-      <c r="U92" s="3"/>
-      <c r="V92" s="3"/>
-    </row>
-    <row r="93" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F93" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K93" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="L93" s="13">
-        <v>0</v>
-      </c>
-      <c r="M93" s="13">
-        <v>0</v>
-      </c>
-      <c r="N93" s="13">
-        <v>0</v>
-      </c>
-      <c r="O93" s="13">
-        <v>0</v>
-      </c>
-      <c r="P93" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="R93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="S93" s="13">
-        <v>-1</v>
-      </c>
-      <c r="T93" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="U93" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="94" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+      <c r="B92" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>